<commit_message>
did some extra analysis of the metabolics data
</commit_message>
<xml_diff>
--- a/metabolicsData_revised.xlsx
+++ b/metabolicsData_revised.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FD07A5-8FF8-4961-B65B-8D81B34D43D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2134A4-D220-4903-B4C0-ED848356537E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2639" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2649" uniqueCount="388">
   <si>
     <t>Metabolic power [W/kg]</t>
   </si>
@@ -1210,6 +1210,33 @@
   <si>
     <t>std dev</t>
   </si>
+  <si>
+    <t>natural day 1</t>
+  </si>
+  <si>
+    <t>natural day 2</t>
+  </si>
+  <si>
+    <t>natural day 3</t>
+  </si>
+  <si>
+    <t>natural sim</t>
+  </si>
+  <si>
+    <t>Gross values</t>
+  </si>
+  <si>
+    <t>exo day 1</t>
+  </si>
+  <si>
+    <t>exo day 2</t>
+  </si>
+  <si>
+    <t>exo day 3</t>
+  </si>
+  <si>
+    <t>exo sim</t>
+  </si>
 </sst>
 </file>
 
@@ -1218,7 +1245,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m\-d"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1293,6 +1320,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -1373,7 +1407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1508,6 +1542,12 @@
     <xf numFmtId="21" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1516,12 +1556,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2191,7 +2226,742 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>natural day 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>welk!$L$92:$L$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>11.908789844999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.511600475</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.576088309999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.736576370000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1C5B-4BE6-A91D-1BA0FFCC5ADA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>natural day 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>welk!$M$92:$M$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>11.857586510000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.58447911</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.346393774999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.080272190000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1C5B-4BE6-A91D-1BA0FFCC5ADA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>natural day 3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>welk!$N$92:$N$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>13.12447721</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.00523155</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.737313759999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.98796596</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-1C5B-4BE6-A91D-1BA0FFCC5ADA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>natural simulation</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>welk!$O$92:$O$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>11.879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.395</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.469999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.445</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-1C5B-4BE6-A91D-1BA0FFCC5ADA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>exo day 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>welk!$P$92:$P$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>11.831386155000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.549725084999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.471758205</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.167520115</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-1C5B-4BE6-A91D-1BA0FFCC5ADA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>exo day 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>welk!$Q$92:$Q$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>11.724543785</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.38107684</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.864205569999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.53917869</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-1C5B-4BE6-A91D-1BA0FFCC5ADA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>exo day 3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>welk!$R$92:$R$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12.913345469999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.60252912</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.41887084</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.078948069999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-1C5B-4BE6-A91D-1BA0FFCC5ADA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>exo simulation</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>welk!$S$92:$S$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>11.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.955</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.914999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-1C5B-4BE6-A91D-1BA0FFCC5ADA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="199"/>
+        <c:axId val="673243800"/>
+        <c:axId val="673238552"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="673243800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Subject</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="673238552"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="673238552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Gross met cost [W/kg]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="673243800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2807,6 +3577,506 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="212">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2845,13 +4115,49 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>321129</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>96613</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>140153</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6290486-E54F-443D-884C-C191A6F193D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Custom 3">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
@@ -2865,28 +4171,28 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="FBD9D6"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="F5A09A"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="EC4235"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="A4190F"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="D5E4FD"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="96BDFA"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="2E7BF6"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="042F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
@@ -3063,12 +4369,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="D1" s="72"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
@@ -3247,8 +4553,8 @@
   <dimension ref="A1:R517"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B206" sqref="B206"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -11562,8 +12868,8 @@
   </sheetPr>
   <dimension ref="A1:AA99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T92" sqref="T92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -11588,12 +12894,12 @@
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
-      <c r="G3" s="74" t="s">
+      <c r="G3" s="78" t="s">
         <v>170</v>
       </c>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
       <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" customHeight="1">
@@ -12795,51 +14101,51 @@
         <v>3</v>
       </c>
       <c r="C44" s="4">
-        <f>C15*$J6</f>
+        <f t="shared" ref="C44:K44" si="15">C15*$J6</f>
         <v>132.57810432719998</v>
       </c>
       <c r="D44" s="4">
-        <f>D15*$J6</f>
+        <f t="shared" si="15"/>
         <v>975.14865670300003</v>
       </c>
       <c r="E44" s="4">
-        <f>E15*$J6</f>
+        <f t="shared" si="15"/>
         <v>959.46156842099992</v>
       </c>
       <c r="F44" s="4">
-        <f>F15*$J6</f>
+        <f t="shared" si="15"/>
         <v>998.52364177099992</v>
       </c>
       <c r="G44" s="4">
-        <f>G15*$J6</f>
+        <f t="shared" si="15"/>
         <v>941.37322079</v>
       </c>
       <c r="H44" s="4">
-        <f>H15*$J6</f>
+        <f t="shared" si="15"/>
         <v>946.49641457299992</v>
       </c>
       <c r="I44" s="4">
-        <f>I15*$J6</f>
+        <f t="shared" si="15"/>
         <v>961.67068202599989</v>
       </c>
       <c r="J44" s="4">
-        <f>J15*$J6</f>
+        <f t="shared" si="15"/>
         <v>929.94470759299998</v>
       </c>
       <c r="K44" s="4">
-        <f>K15*$J6</f>
+        <f t="shared" si="15"/>
         <v>927.88389827399988</v>
       </c>
       <c r="M44" s="4">
-        <f t="shared" ref="M44:M47" si="15">MAX(D44:K44)</f>
+        <f t="shared" ref="M44:M47" si="16">MAX(D44:K44)</f>
         <v>998.52364177099992</v>
       </c>
       <c r="N44" s="4">
-        <f t="shared" ref="N44:N47" si="16">MIN(D44:K44)</f>
+        <f t="shared" ref="N44:N47" si="17">MIN(D44:K44)</f>
         <v>927.88389827399988</v>
       </c>
       <c r="O44" s="4">
-        <f t="shared" ref="O44:O47" si="17">AVERAGE(D44:K44)</f>
+        <f t="shared" ref="O44:O47" si="18">AVERAGE(D44:K44)</f>
         <v>955.06284876887491</v>
       </c>
       <c r="Q44" s="4">
@@ -12863,51 +14169,51 @@
         <v>3</v>
       </c>
       <c r="C45" s="4">
-        <f>C16*$J7</f>
+        <f t="shared" ref="C45:K45" si="19">C16*$J7</f>
         <v>107.74512708999998</v>
       </c>
       <c r="D45" s="4">
-        <f>D16*$J7</f>
+        <f t="shared" si="19"/>
         <v>735.51630859166653</v>
       </c>
       <c r="E45" s="4">
-        <f>E16*$J7</f>
+        <f t="shared" si="19"/>
         <v>708.60236285333326</v>
       </c>
       <c r="F45" s="4">
-        <f>F16*$J7</f>
+        <f t="shared" si="19"/>
         <v>775.70782548</v>
       </c>
       <c r="G45" s="4">
-        <f>G16*$J7</f>
+        <f t="shared" si="19"/>
         <v>729.72669264666661</v>
       </c>
       <c r="H45" s="4">
-        <f>H16*$J7</f>
+        <f t="shared" si="19"/>
         <v>726.00171408999984</v>
       </c>
       <c r="I45" s="4">
-        <f>I16*$J7</f>
+        <f t="shared" si="19"/>
         <v>734.4425488866666</v>
       </c>
       <c r="J45" s="4">
-        <f>J16*$J7</f>
+        <f t="shared" si="19"/>
         <v>685.00525052</v>
       </c>
       <c r="K45" s="4">
-        <f>K16*$J7</f>
+        <f t="shared" si="19"/>
         <v>691.08480349999991</v>
       </c>
       <c r="M45" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>775.70782548</v>
       </c>
       <c r="N45" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>685.00525052</v>
       </c>
       <c r="O45" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>723.26093832104164</v>
       </c>
     </row>
@@ -12919,51 +14225,51 @@
         <v>3</v>
       </c>
       <c r="C46" s="4">
-        <f>C17*$J8</f>
+        <f t="shared" ref="C46:K46" si="20">C17*$J8</f>
         <v>122.6555019684</v>
       </c>
       <c r="D46" s="4">
-        <f>D17*$J8</f>
+        <f t="shared" si="20"/>
         <v>759.40420027200003</v>
       </c>
       <c r="E46" s="4">
-        <f>E17*$J8</f>
+        <f t="shared" si="20"/>
         <v>738.80094334800003</v>
       </c>
       <c r="F46" s="4">
-        <f>F17*$J8</f>
+        <f t="shared" si="20"/>
         <v>826.94279889999996</v>
       </c>
       <c r="G46" s="4">
-        <f>G17*$J8</f>
+        <f t="shared" si="20"/>
         <v>748.67044633300009</v>
       </c>
       <c r="H46" s="4">
-        <f>H17*$J8</f>
+        <f t="shared" si="20"/>
         <v>738.79350155400004</v>
       </c>
       <c r="I46" s="4">
-        <f>I17*$J8</f>
+        <f t="shared" si="20"/>
         <v>743.37563060600007</v>
       </c>
       <c r="J46" s="4">
-        <f>J17*$J8</f>
+        <f t="shared" si="20"/>
         <v>729.31306878400005</v>
       </c>
       <c r="K46" s="4">
-        <f>K17*$J8</f>
+        <f t="shared" si="20"/>
         <v>702.26458290200003</v>
       </c>
       <c r="M46" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>826.94279889999996</v>
       </c>
       <c r="N46" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>702.26458290200003</v>
       </c>
       <c r="O46" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>748.44564658737511</v>
       </c>
     </row>
@@ -12975,51 +14281,51 @@
         <v>3</v>
       </c>
       <c r="C47" s="4">
-        <f>C18*$J9</f>
+        <f t="shared" ref="C47:K47" si="21">C18*$J9</f>
         <v>174.73035954213333</v>
       </c>
       <c r="D47" s="4">
-        <f>D18*$J9</f>
+        <f t="shared" si="21"/>
         <v>1027.0085517279999</v>
       </c>
       <c r="E47" s="4">
-        <f>E18*$J9</f>
+        <f t="shared" si="21"/>
         <v>1035.5123462759998</v>
       </c>
       <c r="F47" s="4">
-        <f>F18*$J9</f>
+        <f t="shared" si="21"/>
         <v>1028.3225594039998</v>
       </c>
       <c r="G47" s="4">
-        <f>G18*$J9</f>
+        <f t="shared" si="21"/>
         <v>992.4917323279999</v>
       </c>
       <c r="H47" s="4">
-        <f>H18*$J9</f>
+        <f t="shared" si="21"/>
         <v>1036.3878709746666</v>
       </c>
       <c r="I47" s="4">
-        <f>I18*$J9</f>
+        <f t="shared" si="21"/>
         <v>1031.2867762253331</v>
       </c>
       <c r="J47" s="4">
-        <f>J18*$J9</f>
+        <f t="shared" si="21"/>
         <v>992.66196597199996</v>
       </c>
       <c r="K47" s="4">
-        <f>K18*$J9</f>
+        <f t="shared" si="21"/>
         <v>991.59806201066647</v>
       </c>
       <c r="M47" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1036.3878709746666</v>
       </c>
       <c r="N47" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>991.59806201066647</v>
       </c>
       <c r="O47" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1016.9087331148331</v>
       </c>
     </row>
@@ -13044,39 +14350,39 @@
         <v>4</v>
       </c>
       <c r="C50" s="3">
-        <f t="shared" ref="C50:K50" si="18">MAX(C44:C47)</f>
+        <f t="shared" ref="C50:K50" si="22">MAX(C44:C47)</f>
         <v>174.73035954213333</v>
       </c>
       <c r="D50" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>1027.0085517279999</v>
       </c>
       <c r="E50" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>1035.5123462759998</v>
       </c>
       <c r="F50" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>1028.3225594039998</v>
       </c>
       <c r="G50" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>992.4917323279999</v>
       </c>
       <c r="H50" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>1036.3878709746666</v>
       </c>
       <c r="I50" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>1031.2867762253331</v>
       </c>
       <c r="J50" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>992.66196597199996</v>
       </c>
       <c r="K50" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>991.59806201066647</v>
       </c>
     </row>
@@ -13086,39 +14392,39 @@
         <v>5</v>
       </c>
       <c r="C51" s="3">
-        <f t="shared" ref="C51:K51" si="19">MIN(C44:C47)</f>
+        <f t="shared" ref="C51:K51" si="23">MIN(C44:C47)</f>
         <v>107.74512708999998</v>
       </c>
       <c r="D51" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>735.51630859166653</v>
       </c>
       <c r="E51" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>708.60236285333326</v>
       </c>
       <c r="F51" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>775.70782548</v>
       </c>
       <c r="G51" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>729.72669264666661</v>
       </c>
       <c r="H51" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>726.00171408999984</v>
       </c>
       <c r="I51" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>734.4425488866666</v>
       </c>
       <c r="J51" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>685.00525052</v>
       </c>
       <c r="K51" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>691.08480349999991</v>
       </c>
     </row>
@@ -13128,39 +14434,39 @@
         <v>6</v>
       </c>
       <c r="C52" s="3">
-        <f t="shared" ref="C52:K52" si="20">AVERAGE(C44:C47)</f>
+        <f t="shared" ref="C52:K52" si="24">AVERAGE(C44:C47)</f>
         <v>134.42727323193333</v>
       </c>
       <c r="D52" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>874.26942932366671</v>
       </c>
       <c r="E52" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>860.59430522458331</v>
       </c>
       <c r="F52" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>907.37420638874983</v>
       </c>
       <c r="G52" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>853.06552302441673</v>
       </c>
       <c r="H52" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>861.91987529791663</v>
       </c>
       <c r="I52" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>867.6939094359999</v>
       </c>
       <c r="J52" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>834.23124821724991</v>
       </c>
       <c r="K52" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>828.20783667166666</v>
       </c>
     </row>
@@ -13274,47 +14580,47 @@
         <v>3</v>
       </c>
       <c r="D57" s="4">
-        <f>D28*$J6</f>
+        <f t="shared" ref="D57:K60" si="25">D28*$J6</f>
         <v>842.57055237580005</v>
       </c>
       <c r="E57" s="4">
-        <f>E28*$J6</f>
+        <f t="shared" si="25"/>
         <v>826.88346409379994</v>
       </c>
       <c r="F57" s="4">
-        <f>F28*$J6</f>
+        <f t="shared" si="25"/>
         <v>865.94553744380005</v>
       </c>
       <c r="G57" s="4">
-        <f>G28*$J6</f>
+        <f t="shared" si="25"/>
         <v>808.79511646280002</v>
       </c>
       <c r="H57" s="4">
-        <f>H28*$J6</f>
+        <f t="shared" si="25"/>
         <v>813.91831024579994</v>
       </c>
       <c r="I57" s="4">
-        <f>I28*$J6</f>
+        <f t="shared" si="25"/>
         <v>829.09257769879991</v>
       </c>
       <c r="J57" s="4">
-        <f>J28*$J6</f>
+        <f t="shared" si="25"/>
         <v>797.36660326580011</v>
       </c>
       <c r="K57" s="4">
-        <f>K28*$J6</f>
+        <f t="shared" si="25"/>
         <v>795.30579394680001</v>
       </c>
       <c r="M57" s="4">
-        <f t="shared" ref="M57:M60" si="21">MAX(D57:K57)</f>
+        <f t="shared" ref="M57:M60" si="26">MAX(D57:K57)</f>
         <v>865.94553744380005</v>
       </c>
       <c r="N57" s="4">
-        <f t="shared" ref="N57:N60" si="22">MIN(D57:K57)</f>
+        <f t="shared" ref="N57:N60" si="27">MIN(D57:K57)</f>
         <v>795.30579394680001</v>
       </c>
       <c r="O57" s="4">
-        <f t="shared" ref="O57:O60" si="23">AVERAGE(D57:K57)</f>
+        <f t="shared" ref="O57:O60" si="28">AVERAGE(D57:K57)</f>
         <v>822.48474444167505</v>
       </c>
       <c r="Q57" s="4">
@@ -13338,47 +14644,47 @@
         <v>3</v>
       </c>
       <c r="D58" s="4">
-        <f>D29*$J7</f>
+        <f t="shared" si="25"/>
         <v>627.77118150166666</v>
       </c>
       <c r="E58" s="4">
-        <f>E29*$J7</f>
+        <f t="shared" si="25"/>
         <v>600.85723576333328</v>
       </c>
       <c r="F58" s="4">
-        <f>F29*$J7</f>
+        <f t="shared" si="25"/>
         <v>667.96269839000001</v>
       </c>
       <c r="G58" s="4">
-        <f>G29*$J7</f>
+        <f t="shared" si="25"/>
         <v>621.98156555666662</v>
       </c>
       <c r="H58" s="4">
-        <f>H29*$J7</f>
+        <f t="shared" si="25"/>
         <v>618.25658699999997</v>
       </c>
       <c r="I58" s="4">
-        <f>I29*$J7</f>
+        <f t="shared" si="25"/>
         <v>626.69742179666662</v>
       </c>
       <c r="J58" s="4">
-        <f>J29*$J7</f>
+        <f t="shared" si="25"/>
         <v>577.26012343000002</v>
       </c>
       <c r="K58" s="4">
-        <f>K29*$J7</f>
+        <f t="shared" si="25"/>
         <v>583.33967640999992</v>
       </c>
       <c r="M58" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>667.96269839000001</v>
       </c>
       <c r="N58" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>577.26012343000002</v>
       </c>
       <c r="O58" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>615.51581123104165</v>
       </c>
     </row>
@@ -13390,47 +14696,47 @@
         <v>3</v>
       </c>
       <c r="D59" s="4">
-        <f>D30*$J8</f>
+        <f t="shared" si="25"/>
         <v>636.74869830360001</v>
       </c>
       <c r="E59" s="4">
-        <f>E30*$J8</f>
+        <f t="shared" si="25"/>
         <v>616.14544137960002</v>
       </c>
       <c r="F59" s="4">
-        <f>F30*$J8</f>
+        <f t="shared" si="25"/>
         <v>704.28729693159994</v>
       </c>
       <c r="G59" s="4">
-        <f>G30*$J8</f>
+        <f t="shared" si="25"/>
         <v>626.01494436459996</v>
       </c>
       <c r="H59" s="4">
-        <f>H30*$J8</f>
+        <f t="shared" si="25"/>
         <v>616.13799958560003</v>
       </c>
       <c r="I59" s="4">
-        <f>I30*$J8</f>
+        <f t="shared" si="25"/>
         <v>620.72012863760006</v>
       </c>
       <c r="J59" s="4">
-        <f>J30*$J8</f>
+        <f t="shared" si="25"/>
         <v>606.65756681560003</v>
       </c>
       <c r="K59" s="4">
-        <f>K30*$J8</f>
+        <f t="shared" si="25"/>
         <v>579.60908093360001</v>
       </c>
       <c r="M59" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>704.28729693159994</v>
       </c>
       <c r="N59" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>579.60908093360001</v>
       </c>
       <c r="O59" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>625.79014461897509</v>
       </c>
     </row>
@@ -13442,47 +14748,47 @@
         <v>3</v>
       </c>
       <c r="D60" s="4">
-        <f>D31*$J9</f>
+        <f t="shared" si="25"/>
         <v>852.27819218586671</v>
       </c>
       <c r="E60" s="4">
-        <f>E31*$J9</f>
+        <f t="shared" si="25"/>
         <v>860.78198673386657</v>
       </c>
       <c r="F60" s="4">
-        <f>F31*$J9</f>
+        <f t="shared" si="25"/>
         <v>853.59219986186667</v>
       </c>
       <c r="G60" s="4">
-        <f>G31*$J9</f>
+        <f t="shared" si="25"/>
         <v>817.76137278586668</v>
       </c>
       <c r="H60" s="4">
-        <f>H31*$J9</f>
+        <f t="shared" si="25"/>
         <v>861.65751143253317</v>
       </c>
       <c r="I60" s="4">
-        <f>I31*$J9</f>
+        <f t="shared" si="25"/>
         <v>856.55641668319993</v>
       </c>
       <c r="J60" s="4">
-        <f>J31*$J9</f>
+        <f t="shared" si="25"/>
         <v>817.93160642986652</v>
       </c>
       <c r="K60" s="4">
-        <f>K31*$J9</f>
+        <f t="shared" si="25"/>
         <v>816.86770246853325</v>
       </c>
       <c r="M60" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>861.65751143253317</v>
       </c>
       <c r="N60" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>816.86770246853325</v>
       </c>
       <c r="O60" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>842.17837357269991</v>
       </c>
     </row>
@@ -13496,35 +14802,35 @@
         <v>4</v>
       </c>
       <c r="D64" s="4">
-        <f t="shared" ref="D64:K64" si="24">MAX(D57:D60)</f>
+        <f t="shared" ref="D64:K64" si="29">MAX(D57:D60)</f>
         <v>852.27819218586671</v>
       </c>
       <c r="E64" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>860.78198673386657</v>
       </c>
       <c r="F64" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>865.94553744380005</v>
       </c>
       <c r="G64" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>817.76137278586668</v>
       </c>
       <c r="H64" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>861.65751143253317</v>
       </c>
       <c r="I64" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>856.55641668319993</v>
       </c>
       <c r="J64" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>817.93160642986652</v>
       </c>
       <c r="K64" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>816.86770246853325</v>
       </c>
     </row>
@@ -13533,35 +14839,35 @@
         <v>5</v>
       </c>
       <c r="D65" s="4">
-        <f t="shared" ref="D65:K65" si="25">MIN(D57:D60)</f>
+        <f t="shared" ref="D65:K65" si="30">MIN(D57:D60)</f>
         <v>627.77118150166666</v>
       </c>
       <c r="E65" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>600.85723576333328</v>
       </c>
       <c r="F65" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>667.96269839000001</v>
       </c>
       <c r="G65" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>621.98156555666662</v>
       </c>
       <c r="H65" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>616.13799958560003</v>
       </c>
       <c r="I65" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>620.72012863760006</v>
       </c>
       <c r="J65" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>577.26012343000002</v>
       </c>
       <c r="K65" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>579.60908093360001</v>
       </c>
     </row>
@@ -13570,932 +14876,932 @@
         <v>6</v>
       </c>
       <c r="D66" s="4">
-        <f t="shared" ref="D66:K66" si="26">AVERAGE(D57:D60)</f>
+        <f t="shared" ref="D66:K66" si="31">AVERAGE(D57:D60)</f>
         <v>739.84215609173339</v>
       </c>
       <c r="E66" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>726.16703199264998</v>
       </c>
       <c r="F66" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>772.94693315681661</v>
       </c>
       <c r="G66" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>718.63824979248329</v>
       </c>
       <c r="H66" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>727.49260206598331</v>
       </c>
       <c r="I66" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>733.26663620406657</v>
       </c>
       <c r="J66" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>699.8039749853167</v>
       </c>
       <c r="K66" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>693.78056343973321</v>
       </c>
     </row>
     <row r="72" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A72" s="77"/>
-      <c r="B72" s="77"/>
-      <c r="C72" s="77"/>
-      <c r="D72" s="77" t="s">
+      <c r="A72" s="73"/>
+      <c r="B72" s="73"/>
+      <c r="C72" s="73"/>
+      <c r="D72" s="73" t="s">
         <v>192</v>
       </c>
-      <c r="E72" s="77" t="s">
+      <c r="E72" s="73" t="s">
         <v>193</v>
       </c>
-      <c r="F72" s="77"/>
-      <c r="G72" s="77"/>
-      <c r="H72" s="77"/>
-      <c r="I72" s="77" t="s">
+      <c r="F72" s="73"/>
+      <c r="G72" s="73"/>
+      <c r="H72" s="73"/>
+      <c r="I72" s="73" t="s">
         <v>192</v>
       </c>
-      <c r="J72" s="77" t="s">
+      <c r="J72" s="73" t="s">
         <v>193</v>
       </c>
-      <c r="K72" s="77"/>
-      <c r="L72" s="77"/>
-      <c r="M72" s="77"/>
-      <c r="N72" s="77" t="s">
+      <c r="K72" s="73"/>
+      <c r="L72" s="73"/>
+      <c r="M72" s="73"/>
+      <c r="N72" s="73" t="s">
         <v>192</v>
       </c>
-      <c r="O72" s="77" t="s">
+      <c r="O72" s="73" t="s">
         <v>193</v>
       </c>
-      <c r="P72" s="77"/>
-      <c r="Q72" s="77"/>
-      <c r="R72" s="77"/>
-      <c r="S72" s="77" t="s">
+      <c r="P72" s="73"/>
+      <c r="Q72" s="73"/>
+      <c r="R72" s="73"/>
+      <c r="S72" s="73" t="s">
         <v>192</v>
       </c>
-      <c r="T72" s="77" t="s">
+      <c r="T72" s="73" t="s">
         <v>193</v>
       </c>
-      <c r="U72" s="77"/>
-      <c r="V72" s="77"/>
+      <c r="U72" s="73"/>
+      <c r="V72" s="73"/>
     </row>
     <row r="73" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A73" s="77"/>
-      <c r="B73" s="77" t="s">
+      <c r="A73" s="73"/>
+      <c r="B73" s="73" t="s">
         <v>196</v>
       </c>
-      <c r="C73" s="77" t="s">
+      <c r="C73" s="73" t="s">
         <v>197</v>
       </c>
-      <c r="D73" s="77" t="s">
+      <c r="D73" s="73" t="s">
         <v>198</v>
       </c>
-      <c r="E73" s="77" t="s">
+      <c r="E73" s="73" t="s">
         <v>199</v>
       </c>
-      <c r="F73" s="77" t="s">
+      <c r="F73" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="G73" s="77" t="s">
+      <c r="G73" s="73" t="s">
         <v>196</v>
       </c>
-      <c r="H73" s="77" t="s">
+      <c r="H73" s="73" t="s">
         <v>197</v>
       </c>
-      <c r="I73" s="77" t="s">
+      <c r="I73" s="73" t="s">
         <v>198</v>
       </c>
-      <c r="J73" s="77" t="s">
+      <c r="J73" s="73" t="s">
         <v>199</v>
       </c>
-      <c r="K73" s="77" t="s">
+      <c r="K73" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="L73" s="77" t="s">
+      <c r="L73" s="73" t="s">
         <v>196</v>
       </c>
-      <c r="M73" s="77" t="s">
+      <c r="M73" s="73" t="s">
         <v>197</v>
       </c>
-      <c r="N73" s="77" t="s">
+      <c r="N73" s="73" t="s">
         <v>198</v>
       </c>
-      <c r="O73" s="77" t="s">
+      <c r="O73" s="73" t="s">
         <v>199</v>
       </c>
-      <c r="P73" s="77" t="s">
+      <c r="P73" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="Q73" s="77" t="s">
+      <c r="Q73" s="73" t="s">
         <v>196</v>
       </c>
-      <c r="R73" s="77" t="s">
+      <c r="R73" s="73" t="s">
         <v>197</v>
       </c>
-      <c r="S73" s="77" t="s">
+      <c r="S73" s="73" t="s">
         <v>198</v>
       </c>
-      <c r="T73" s="77" t="s">
+      <c r="T73" s="73" t="s">
         <v>199</v>
       </c>
-      <c r="U73" s="77" t="s">
+      <c r="U73" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="V73" s="77"/>
+      <c r="V73" s="73"/>
     </row>
     <row r="74" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A74" s="77"/>
-      <c r="B74" s="77">
+      <c r="A74" s="73"/>
+      <c r="B74" s="73">
         <v>1</v>
       </c>
-      <c r="C74" s="77">
+      <c r="C74" s="73">
         <v>3</v>
       </c>
-      <c r="D74" s="77">
+      <c r="D74" s="73">
         <v>1.7843621039999999</v>
       </c>
-      <c r="E74" s="77">
+      <c r="E74" s="73">
         <v>13.12447721</v>
       </c>
-      <c r="F74" s="77">
+      <c r="F74" s="73">
         <v>12.913345469999999</v>
       </c>
-      <c r="G74" s="77">
+      <c r="G74" s="73">
         <v>2</v>
       </c>
-      <c r="H74" s="77">
+      <c r="H74" s="73">
         <v>3</v>
       </c>
-      <c r="I74" s="77">
+      <c r="I74" s="73">
         <v>1.6121465399999999</v>
       </c>
-      <c r="J74" s="77">
+      <c r="J74" s="73">
         <v>11.00523155</v>
       </c>
-      <c r="K74" s="77">
+      <c r="K74" s="73">
         <v>10.60252912</v>
       </c>
-      <c r="L74" s="77">
+      <c r="L74" s="73">
         <v>3</v>
       </c>
-      <c r="M74" s="77">
+      <c r="M74" s="73">
         <v>3</v>
       </c>
-      <c r="N74" s="77">
+      <c r="N74" s="73">
         <v>1.8957573720000001</v>
       </c>
-      <c r="O74" s="77">
+      <c r="O74" s="73">
         <v>11.737313759999999</v>
       </c>
-      <c r="P74" s="77">
+      <c r="P74" s="73">
         <v>11.41887084</v>
       </c>
-      <c r="Q74" s="77">
+      <c r="Q74" s="73">
         <v>4</v>
       </c>
-      <c r="R74" s="77">
+      <c r="R74" s="73">
         <v>3</v>
       </c>
-      <c r="S74" s="77">
+      <c r="S74" s="73">
         <v>1.8694403660000001</v>
       </c>
-      <c r="T74" s="77">
+      <c r="T74" s="73">
         <v>10.98796596</v>
       </c>
-      <c r="U74" s="77">
+      <c r="U74" s="73">
         <v>11.078948069999999</v>
       </c>
-      <c r="V74" s="77"/>
+      <c r="V74" s="73"/>
     </row>
     <row r="75" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A75" s="77"/>
-      <c r="B75" s="77">
+      <c r="A75" s="73"/>
+      <c r="B75" s="73">
         <v>1</v>
       </c>
-      <c r="C75" s="77">
+      <c r="C75" s="73">
         <v>2</v>
       </c>
-      <c r="D75" s="77">
+      <c r="D75" s="73">
         <v>1.9533226530000001</v>
       </c>
-      <c r="E75" s="77">
+      <c r="E75" s="73">
         <v>11.698063429999999</v>
       </c>
-      <c r="F75" s="77">
+      <c r="F75" s="73">
         <v>11.91752514</v>
       </c>
-      <c r="G75" s="77">
+      <c r="G75" s="73">
         <v>2</v>
       </c>
-      <c r="H75" s="77">
+      <c r="H75" s="73">
         <v>2</v>
       </c>
-      <c r="I75" s="77">
+      <c r="I75" s="73">
         <v>1.6356537799999999</v>
       </c>
-      <c r="J75" s="77">
+      <c r="J75" s="73">
         <v>10.54304964</v>
       </c>
-      <c r="K75" s="77">
+      <c r="K75" s="73">
         <v>10.4326998</v>
       </c>
-      <c r="L75" s="77">
+      <c r="L75" s="73">
         <v>3</v>
       </c>
-      <c r="M75" s="77">
+      <c r="M75" s="73">
         <v>2</v>
       </c>
-      <c r="N75" s="77">
+      <c r="N75" s="73">
         <v>1.8451964569999999</v>
       </c>
-      <c r="O75" s="77">
+      <c r="O75" s="73">
         <v>11.37779744</v>
       </c>
-      <c r="P75" s="77">
+      <c r="P75" s="73">
         <v>11.05976031</v>
       </c>
-      <c r="Q75" s="77">
+      <c r="Q75" s="73">
         <v>4</v>
       </c>
-      <c r="R75" s="77">
+      <c r="R75" s="73">
         <v>2</v>
       </c>
-      <c r="S75" s="77">
+      <c r="S75" s="73">
         <v>1.698257736</v>
       </c>
-      <c r="T75" s="77">
+      <c r="T75" s="73">
         <v>10.901165600000001</v>
       </c>
-      <c r="U75" s="77">
+      <c r="U75" s="73">
         <v>10.59103932</v>
       </c>
-      <c r="V75" s="77"/>
+      <c r="V75" s="73"/>
     </row>
     <row r="76" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A76" s="77"/>
-      <c r="B76" s="77">
+      <c r="A76" s="73"/>
+      <c r="B76" s="73">
         <v>1</v>
       </c>
-      <c r="C76" s="77">
+      <c r="C76" s="73">
         <v>2</v>
       </c>
-      <c r="D76" s="77">
+      <c r="D76" s="73">
         <v>1.9533226530000001</v>
       </c>
-      <c r="E76" s="77">
+      <c r="E76" s="73">
         <v>12.01710959</v>
       </c>
-      <c r="F76" s="77">
+      <c r="F76" s="73">
         <v>11.531562429999999</v>
       </c>
-      <c r="G76" s="77">
+      <c r="G76" s="73">
         <v>2</v>
       </c>
-      <c r="H76" s="77">
+      <c r="H76" s="73">
         <v>2</v>
       </c>
-      <c r="I76" s="77">
+      <c r="I76" s="73">
         <v>1.6356537799999999</v>
       </c>
-      <c r="J76" s="77">
+      <c r="J76" s="73">
         <v>10.625908580000001</v>
       </c>
-      <c r="K76" s="77">
+      <c r="K76" s="73">
         <v>10.329453880000001</v>
       </c>
-      <c r="L76" s="77">
+      <c r="L76" s="73">
         <v>3</v>
       </c>
-      <c r="M76" s="77">
+      <c r="M76" s="73">
         <v>2</v>
       </c>
-      <c r="N76" s="77">
+      <c r="N76" s="73">
         <v>1.8451964569999999</v>
       </c>
-      <c r="O76" s="77">
+      <c r="O76" s="73">
         <v>11.31499011</v>
       </c>
-      <c r="P76" s="77">
+      <c r="P76" s="73">
         <v>10.668650830000001</v>
       </c>
-      <c r="Q76" s="77">
+      <c r="Q76" s="73">
         <v>4</v>
       </c>
-      <c r="R76" s="77">
+      <c r="R76" s="73">
         <v>2</v>
       </c>
-      <c r="S76" s="77">
+      <c r="S76" s="73">
         <v>1.698257736</v>
       </c>
-      <c r="T76" s="77">
+      <c r="T76" s="73">
         <v>11.25937878</v>
       </c>
-      <c r="U76" s="77">
+      <c r="U76" s="73">
         <v>10.48731806</v>
       </c>
-      <c r="V76" s="77"/>
+      <c r="V76" s="73"/>
     </row>
     <row r="77" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A77" s="77"/>
-      <c r="B77" s="77">
+      <c r="A77" s="73"/>
+      <c r="B77" s="73">
         <v>1</v>
       </c>
-      <c r="C77" s="77">
+      <c r="C77" s="73">
         <v>1</v>
       </c>
-      <c r="D77" s="77">
+      <c r="D77" s="73">
         <v>1.8314126049999999</v>
       </c>
-      <c r="E77" s="77">
+      <c r="E77" s="73">
         <v>11.832379469999999</v>
       </c>
-      <c r="F77" s="77">
+      <c r="F77" s="73">
         <v>11.70265908</v>
       </c>
-      <c r="G77" s="77">
+      <c r="G77" s="73">
         <v>2</v>
       </c>
-      <c r="H77" s="77">
+      <c r="H77" s="73">
         <v>1</v>
       </c>
-      <c r="I77" s="77">
+      <c r="I77" s="73">
         <v>1.577234099</v>
       </c>
-      <c r="J77" s="77">
+      <c r="J77" s="73">
         <v>10.75850441</v>
       </c>
-      <c r="K77" s="77">
+      <c r="K77" s="73">
         <v>10.937471029999999</v>
       </c>
-      <c r="L77" s="77">
+      <c r="L77" s="73">
         <v>3</v>
       </c>
-      <c r="M77" s="77">
+      <c r="M77" s="73">
         <v>1</v>
       </c>
-      <c r="N77" s="77">
+      <c r="N77" s="73">
         <v>1.6330105290000001</v>
       </c>
-      <c r="O77" s="77">
+      <c r="O77" s="73">
         <v>11.814252460000001</v>
       </c>
-      <c r="P77" s="77">
+      <c r="P77" s="73">
         <v>11.43216496</v>
       </c>
-      <c r="Q77" s="77">
+      <c r="Q77" s="73">
         <v>4</v>
       </c>
-      <c r="R77" s="77">
+      <c r="R77" s="73">
         <v>1</v>
       </c>
-      <c r="S77" s="77">
+      <c r="S77" s="73">
         <v>1.887225025</v>
       </c>
-      <c r="T77" s="77">
+      <c r="T77" s="73">
         <v>10.823476680000001</v>
       </c>
-      <c r="U77" s="77">
+      <c r="U77" s="73">
         <v>11.38139209</v>
       </c>
-      <c r="V77" s="77"/>
+      <c r="V77" s="73"/>
     </row>
     <row r="78" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A78" s="77"/>
-      <c r="B78" s="77">
+      <c r="A78" s="73"/>
+      <c r="B78" s="73">
         <v>1</v>
       </c>
-      <c r="C78" s="77">
+      <c r="C78" s="73">
         <v>1</v>
       </c>
-      <c r="D78" s="77">
+      <c r="D78" s="73">
         <v>1.8314126049999999</v>
       </c>
-      <c r="E78" s="77">
+      <c r="E78" s="73">
         <v>11.985200219999999</v>
       </c>
-      <c r="F78" s="77">
+      <c r="F78" s="73">
         <v>11.960113229999999</v>
       </c>
-      <c r="G78" s="77">
+      <c r="G78" s="73">
         <v>2</v>
       </c>
-      <c r="H78" s="77">
+      <c r="H78" s="73">
         <v>1</v>
       </c>
-      <c r="I78" s="77">
+      <c r="I78" s="73">
         <v>1.577234099</v>
       </c>
-      <c r="J78" s="77">
+      <c r="J78" s="73">
         <v>10.264696539999999</v>
       </c>
-      <c r="K78" s="77">
+      <c r="K78" s="73">
         <v>10.16197914</v>
       </c>
-      <c r="L78" s="77">
+      <c r="L78" s="73">
         <v>3</v>
       </c>
-      <c r="M78" s="77">
+      <c r="M78" s="73">
         <v>1</v>
       </c>
-      <c r="N78" s="77">
+      <c r="N78" s="73">
         <v>1.6330105290000001</v>
       </c>
-      <c r="O78" s="77">
+      <c r="O78" s="73">
         <v>11.33792416</v>
       </c>
-      <c r="P78" s="77">
+      <c r="P78" s="73">
         <v>11.511351449999999</v>
       </c>
-      <c r="Q78" s="77">
+      <c r="Q78" s="73">
         <v>4</v>
       </c>
-      <c r="R78" s="77">
+      <c r="R78" s="73">
         <v>1</v>
       </c>
-      <c r="S78" s="77">
+      <c r="S78" s="73">
         <v>1.887225025</v>
       </c>
-      <c r="T78" s="77">
+      <c r="T78" s="73">
         <v>10.649676060000001</v>
       </c>
-      <c r="U78" s="77">
+      <c r="U78" s="73">
         <v>10.95364814</v>
       </c>
-      <c r="V78" s="77"/>
+      <c r="V78" s="73"/>
     </row>
     <row r="79" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A79" s="77"/>
-      <c r="B79" s="77"/>
-      <c r="C79" s="77"/>
-      <c r="D79" s="77"/>
-      <c r="E79" s="77"/>
-      <c r="F79" s="77"/>
-      <c r="G79" s="77"/>
-      <c r="H79" s="77"/>
-      <c r="I79" s="77"/>
-      <c r="J79" s="77"/>
-      <c r="K79" s="77"/>
-      <c r="L79" s="77"/>
-      <c r="M79" s="77"/>
-      <c r="N79" s="77"/>
-      <c r="O79" s="77"/>
-      <c r="P79" s="77"/>
-      <c r="Q79" s="77"/>
-      <c r="R79" s="77"/>
-      <c r="S79" s="77"/>
-      <c r="T79" s="77"/>
-      <c r="U79" s="77"/>
-      <c r="V79" s="77"/>
+      <c r="A79" s="73"/>
+      <c r="B79" s="73"/>
+      <c r="C79" s="73"/>
+      <c r="D79" s="73"/>
+      <c r="E79" s="73"/>
+      <c r="F79" s="73"/>
+      <c r="G79" s="73"/>
+      <c r="H79" s="73"/>
+      <c r="I79" s="73"/>
+      <c r="J79" s="73"/>
+      <c r="K79" s="73"/>
+      <c r="L79" s="73"/>
+      <c r="M79" s="73"/>
+      <c r="N79" s="73"/>
+      <c r="O79" s="73"/>
+      <c r="P79" s="73"/>
+      <c r="Q79" s="73"/>
+      <c r="R79" s="73"/>
+      <c r="S79" s="73"/>
+      <c r="T79" s="73"/>
+      <c r="U79" s="73"/>
+      <c r="V79" s="73"/>
     </row>
     <row r="80" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A80" s="77"/>
-      <c r="B80" s="77"/>
-      <c r="C80" s="77" t="s">
+      <c r="A80" s="73"/>
+      <c r="B80" s="73"/>
+      <c r="C80" s="73" t="s">
         <v>308</v>
       </c>
-      <c r="D80" s="77">
+      <c r="D80" s="73">
         <f>AVERAGE(D74:D78)</f>
         <v>1.870766524</v>
       </c>
-      <c r="E80" s="77">
-        <f t="shared" ref="E80:F80" si="27">AVERAGE(E74:E78)</f>
+      <c r="E80" s="73">
+        <f t="shared" ref="E80:F80" si="32">AVERAGE(E74:E78)</f>
         <v>12.131445984000001</v>
       </c>
-      <c r="F80" s="77">
-        <f t="shared" si="27"/>
+      <c r="F80" s="73">
+        <f t="shared" si="32"/>
         <v>12.005041070000001</v>
       </c>
-      <c r="G80" s="77"/>
-      <c r="H80" s="77" t="s">
+      <c r="G80" s="73"/>
+      <c r="H80" s="73" t="s">
         <v>308</v>
       </c>
-      <c r="I80" s="77">
+      <c r="I80" s="73">
         <f>AVERAGE(I74:I78)</f>
         <v>1.6075844596</v>
       </c>
-      <c r="J80" s="77">
-        <f t="shared" ref="J80:K80" si="28">AVERAGE(J74:J78)</f>
+      <c r="J80" s="73">
+        <f t="shared" ref="J80:K80" si="33">AVERAGE(J74:J78)</f>
         <v>10.639478144</v>
       </c>
-      <c r="K80" s="77">
-        <f t="shared" si="28"/>
+      <c r="K80" s="73">
+        <f t="shared" si="33"/>
         <v>10.492826594</v>
       </c>
-      <c r="L80" s="77"/>
-      <c r="M80" s="77" t="s">
+      <c r="L80" s="73"/>
+      <c r="M80" s="73" t="s">
         <v>308</v>
       </c>
-      <c r="N80" s="77">
+      <c r="N80" s="73">
         <f>AVERAGE(N74:N78)</f>
         <v>1.7704342688000001</v>
       </c>
-      <c r="O80" s="77">
-        <f t="shared" ref="O80:P80" si="29">AVERAGE(O74:O78)</f>
+      <c r="O80" s="73">
+        <f t="shared" ref="O80:P80" si="34">AVERAGE(O74:O78)</f>
         <v>11.516455585999999</v>
       </c>
-      <c r="P80" s="77">
-        <f t="shared" si="29"/>
+      <c r="P80" s="73">
+        <f t="shared" si="34"/>
         <v>11.218159678000001</v>
       </c>
-      <c r="Q80" s="77"/>
-      <c r="R80" s="77" t="s">
+      <c r="Q80" s="73"/>
+      <c r="R80" s="73" t="s">
         <v>308</v>
       </c>
-      <c r="S80" s="77">
+      <c r="S80" s="73">
         <f>AVERAGE(S74:S78)</f>
         <v>1.8080811776000001</v>
       </c>
-      <c r="T80" s="77">
-        <f t="shared" ref="T80:U80" si="30">AVERAGE(T74:T78)</f>
+      <c r="T80" s="73">
+        <f t="shared" ref="T80:U80" si="35">AVERAGE(T74:T78)</f>
         <v>10.924332616000001</v>
       </c>
-      <c r="U80" s="77">
-        <f t="shared" si="30"/>
+      <c r="U80" s="73">
+        <f t="shared" si="35"/>
         <v>10.898469135999999</v>
       </c>
-      <c r="V80" s="77"/>
+      <c r="V80" s="73"/>
     </row>
     <row r="81" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A81" s="77"/>
-      <c r="B81" s="77"/>
-      <c r="C81" s="77" t="s">
+      <c r="A81" s="73"/>
+      <c r="B81" s="73"/>
+      <c r="C81" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="D81" s="77">
+      <c r="D81" s="73">
         <f>MIN(D74:D78)</f>
         <v>1.7843621039999999</v>
       </c>
-      <c r="E81" s="77">
-        <f t="shared" ref="E81:F81" si="31">MIN(E74:E78)</f>
+      <c r="E81" s="73">
+        <f t="shared" ref="E81:F81" si="36">MIN(E74:E78)</f>
         <v>11.698063429999999</v>
       </c>
-      <c r="F81" s="77">
-        <f t="shared" si="31"/>
+      <c r="F81" s="73">
+        <f t="shared" si="36"/>
         <v>11.531562429999999</v>
       </c>
-      <c r="G81" s="77"/>
-      <c r="H81" s="77" t="s">
+      <c r="G81" s="73"/>
+      <c r="H81" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="I81" s="77">
+      <c r="I81" s="73">
         <f>MIN(I74:I78)</f>
         <v>1.577234099</v>
       </c>
-      <c r="J81" s="77">
-        <f t="shared" ref="J81:K81" si="32">MIN(J74:J78)</f>
+      <c r="J81" s="73">
+        <f t="shared" ref="J81:K81" si="37">MIN(J74:J78)</f>
         <v>10.264696539999999</v>
       </c>
-      <c r="K81" s="77">
-        <f t="shared" si="32"/>
+      <c r="K81" s="73">
+        <f t="shared" si="37"/>
         <v>10.16197914</v>
       </c>
-      <c r="L81" s="77"/>
-      <c r="M81" s="77" t="s">
+      <c r="L81" s="73"/>
+      <c r="M81" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="N81" s="77">
+      <c r="N81" s="73">
         <f>MIN(N74:N78)</f>
         <v>1.6330105290000001</v>
       </c>
-      <c r="O81" s="77">
-        <f t="shared" ref="O81:P81" si="33">MIN(O74:O78)</f>
+      <c r="O81" s="73">
+        <f t="shared" ref="O81:P81" si="38">MIN(O74:O78)</f>
         <v>11.31499011</v>
       </c>
-      <c r="P81" s="77">
-        <f t="shared" si="33"/>
+      <c r="P81" s="73">
+        <f t="shared" si="38"/>
         <v>10.668650830000001</v>
       </c>
-      <c r="Q81" s="77"/>
-      <c r="R81" s="77" t="s">
+      <c r="Q81" s="73"/>
+      <c r="R81" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="S81" s="77">
+      <c r="S81" s="73">
         <f>MIN(S74:S78)</f>
         <v>1.698257736</v>
       </c>
-      <c r="T81" s="77">
-        <f t="shared" ref="T81:U81" si="34">MIN(T74:T78)</f>
+      <c r="T81" s="73">
+        <f t="shared" ref="T81:U81" si="39">MIN(T74:T78)</f>
         <v>10.649676060000001</v>
       </c>
-      <c r="U81" s="77">
-        <f t="shared" si="34"/>
+      <c r="U81" s="73">
+        <f t="shared" si="39"/>
         <v>10.48731806</v>
       </c>
-      <c r="V81" s="77"/>
+      <c r="V81" s="73"/>
     </row>
     <row r="82" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A82" s="77"/>
-      <c r="B82" s="77"/>
-      <c r="C82" s="77" t="s">
+      <c r="A82" s="73"/>
+      <c r="B82" s="73"/>
+      <c r="C82" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="D82" s="77">
+      <c r="D82" s="73">
         <f>MAX(D74:D78)</f>
         <v>1.9533226530000001</v>
       </c>
-      <c r="E82" s="77">
-        <f t="shared" ref="E82:F82" si="35">MAX(E74:E78)</f>
+      <c r="E82" s="73">
+        <f t="shared" ref="E82:F82" si="40">MAX(E74:E78)</f>
         <v>13.12447721</v>
       </c>
-      <c r="F82" s="77">
-        <f t="shared" si="35"/>
+      <c r="F82" s="73">
+        <f t="shared" si="40"/>
         <v>12.913345469999999</v>
       </c>
-      <c r="G82" s="77"/>
-      <c r="H82" s="77" t="s">
+      <c r="G82" s="73"/>
+      <c r="H82" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="I82" s="77">
+      <c r="I82" s="73">
         <f>MAX(I74:I78)</f>
         <v>1.6356537799999999</v>
       </c>
-      <c r="J82" s="77">
-        <f t="shared" ref="J82:K82" si="36">MAX(J74:J78)</f>
+      <c r="J82" s="73">
+        <f t="shared" ref="J82:K82" si="41">MAX(J74:J78)</f>
         <v>11.00523155</v>
       </c>
-      <c r="K82" s="77">
-        <f t="shared" si="36"/>
+      <c r="K82" s="73">
+        <f t="shared" si="41"/>
         <v>10.937471029999999</v>
       </c>
-      <c r="L82" s="77"/>
-      <c r="M82" s="77" t="s">
+      <c r="L82" s="73"/>
+      <c r="M82" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="N82" s="77">
+      <c r="N82" s="73">
         <f>MAX(N74:N78)</f>
         <v>1.8957573720000001</v>
       </c>
-      <c r="O82" s="77">
-        <f t="shared" ref="O82:P82" si="37">MAX(O74:O78)</f>
+      <c r="O82" s="73">
+        <f t="shared" ref="O82:P82" si="42">MAX(O74:O78)</f>
         <v>11.814252460000001</v>
       </c>
-      <c r="P82" s="77">
-        <f t="shared" si="37"/>
+      <c r="P82" s="73">
+        <f t="shared" si="42"/>
         <v>11.511351449999999</v>
       </c>
-      <c r="Q82" s="77"/>
-      <c r="R82" s="77" t="s">
+      <c r="Q82" s="73"/>
+      <c r="R82" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="S82" s="77">
+      <c r="S82" s="73">
         <f>MAX(S74:S78)</f>
         <v>1.887225025</v>
       </c>
-      <c r="T82" s="77">
-        <f t="shared" ref="T82:U82" si="38">MAX(T74:T78)</f>
+      <c r="T82" s="73">
+        <f t="shared" ref="T82:U82" si="43">MAX(T74:T78)</f>
         <v>11.25937878</v>
       </c>
-      <c r="U82" s="77">
-        <f t="shared" si="38"/>
+      <c r="U82" s="73">
+        <f t="shared" si="43"/>
         <v>11.38139209</v>
       </c>
-      <c r="V82" s="77"/>
+      <c r="V82" s="73"/>
     </row>
     <row r="83" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A83" s="77"/>
-      <c r="B83" s="77"/>
-      <c r="C83" s="77" t="s">
+      <c r="A83" s="73"/>
+      <c r="B83" s="73"/>
+      <c r="C83" s="73" t="s">
         <v>374</v>
       </c>
-      <c r="D83" s="77">
+      <c r="D83" s="73">
         <f>D82-D81</f>
         <v>0.16896054900000013</v>
       </c>
-      <c r="E83" s="77">
-        <f t="shared" ref="E83" si="39">E82-E81</f>
+      <c r="E83" s="73">
+        <f t="shared" ref="E83" si="44">E82-E81</f>
         <v>1.4264137800000007</v>
       </c>
-      <c r="F83" s="77">
-        <f t="shared" ref="F83" si="40">F82-F81</f>
+      <c r="F83" s="73">
+        <f t="shared" ref="F83" si="45">F82-F81</f>
         <v>1.3817830400000002</v>
       </c>
-      <c r="G83" s="77"/>
-      <c r="H83" s="77" t="s">
+      <c r="G83" s="73"/>
+      <c r="H83" s="73" t="s">
         <v>374</v>
       </c>
-      <c r="I83" s="77">
+      <c r="I83" s="73">
         <f>I82-I81</f>
         <v>5.8419680999999946E-2</v>
       </c>
-      <c r="J83" s="77">
-        <f t="shared" ref="J83" si="41">J82-J81</f>
+      <c r="J83" s="73">
+        <f t="shared" ref="J83" si="46">J82-J81</f>
         <v>0.74053501000000033</v>
       </c>
-      <c r="K83" s="77">
-        <f t="shared" ref="K83" si="42">K82-K81</f>
+      <c r="K83" s="73">
+        <f t="shared" ref="K83" si="47">K82-K81</f>
         <v>0.77549188999999963</v>
       </c>
-      <c r="L83" s="77"/>
-      <c r="M83" s="77" t="s">
+      <c r="L83" s="73"/>
+      <c r="M83" s="73" t="s">
         <v>374</v>
       </c>
-      <c r="N83" s="77">
+      <c r="N83" s="73">
         <f>N82-N81</f>
         <v>0.26274684299999995</v>
       </c>
-      <c r="O83" s="77">
-        <f t="shared" ref="O83" si="43">O82-O81</f>
+      <c r="O83" s="73">
+        <f t="shared" ref="O83" si="48">O82-O81</f>
         <v>0.49926235000000041</v>
       </c>
-      <c r="P83" s="77">
-        <f t="shared" ref="P83" si="44">P82-P81</f>
+      <c r="P83" s="73">
+        <f t="shared" ref="P83" si="49">P82-P81</f>
         <v>0.84270061999999868</v>
       </c>
-      <c r="Q83" s="77"/>
-      <c r="R83" s="77" t="s">
+      <c r="Q83" s="73"/>
+      <c r="R83" s="73" t="s">
         <v>374</v>
       </c>
-      <c r="S83" s="77">
+      <c r="S83" s="73">
         <f>S82-S81</f>
         <v>0.18896728900000004</v>
       </c>
-      <c r="T83" s="77">
-        <f t="shared" ref="T83:U83" si="45">T82-T81</f>
+      <c r="T83" s="73">
+        <f t="shared" ref="T83:U83" si="50">T82-T81</f>
         <v>0.60970271999999959</v>
       </c>
-      <c r="U83" s="77">
-        <f t="shared" si="45"/>
+      <c r="U83" s="73">
+        <f t="shared" si="50"/>
         <v>0.89407403000000052</v>
       </c>
-      <c r="V83" s="77"/>
+      <c r="V83" s="73"/>
     </row>
     <row r="84" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A84" s="77"/>
-      <c r="B84" s="77"/>
-      <c r="C84" s="79" t="s">
+      <c r="A84" s="73"/>
+      <c r="B84" s="73"/>
+      <c r="C84" s="75" t="s">
         <v>378</v>
       </c>
-      <c r="D84" s="77">
+      <c r="D84" s="73">
         <f>_xlfn.STDEV.P(D74:D78)</f>
         <v>6.9561792023758062E-2</v>
       </c>
-      <c r="E84" s="77">
-        <f t="shared" ref="E84:U84" si="46">_xlfn.STDEV.P(E74:E78)</f>
+      <c r="E84" s="73">
+        <f t="shared" ref="E84:U84" si="51">_xlfn.STDEV.P(E74:E78)</f>
         <v>0.50947676457314639</v>
       </c>
-      <c r="F84" s="77">
-        <f t="shared" si="46"/>
+      <c r="F84" s="73">
+        <f t="shared" si="51"/>
         <v>0.47964806312186858</v>
       </c>
-      <c r="G84" s="77">
-        <f t="shared" si="46"/>
+      <c r="G84" s="73">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
-      <c r="H84" s="77">
-        <f t="shared" si="46"/>
+      <c r="H84" s="73">
+        <f t="shared" si="51"/>
         <v>0.74833147735478833</v>
       </c>
-      <c r="I84" s="77">
-        <f t="shared" si="46"/>
+      <c r="I84" s="73">
+        <f t="shared" si="51"/>
         <v>2.6225464152658324E-2</v>
       </c>
-      <c r="J84" s="77">
-        <f t="shared" si="46"/>
+      <c r="J84" s="73">
+        <f t="shared" si="51"/>
         <v>0.24408467635070619</v>
       </c>
-      <c r="K84" s="77">
-        <f t="shared" si="46"/>
+      <c r="K84" s="73">
+        <f t="shared" si="51"/>
         <v>0.26438957299079113</v>
       </c>
-      <c r="L84" s="77">
-        <f t="shared" si="46"/>
+      <c r="L84" s="73">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
-      <c r="M84" s="77">
-        <f t="shared" si="46"/>
+      <c r="M84" s="73">
+        <f t="shared" si="51"/>
         <v>0.74833147735478833</v>
       </c>
-      <c r="N84" s="77">
-        <f t="shared" si="46"/>
+      <c r="N84" s="73">
+        <f t="shared" si="51"/>
         <v>0.11371474687639985</v>
       </c>
-      <c r="O84" s="77">
-        <f t="shared" si="46"/>
+      <c r="O84" s="73">
+        <f t="shared" si="51"/>
         <v>0.21407905116028678</v>
       </c>
-      <c r="P84" s="77">
-        <f t="shared" si="46"/>
+      <c r="P84" s="73">
+        <f t="shared" si="51"/>
         <v>0.31594144402305796</v>
       </c>
-      <c r="Q84" s="77">
-        <f t="shared" si="46"/>
+      <c r="Q84" s="73">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
-      <c r="R84" s="77">
-        <f t="shared" si="46"/>
+      <c r="R84" s="73">
+        <f t="shared" si="51"/>
         <v>0.74833147735478833</v>
       </c>
-      <c r="S84" s="77">
-        <f t="shared" si="46"/>
+      <c r="S84" s="73">
+        <f t="shared" si="51"/>
         <v>8.990530998043765E-2</v>
       </c>
-      <c r="T84" s="77">
-        <f t="shared" si="46"/>
+      <c r="T84" s="73">
+        <f t="shared" si="51"/>
         <v>0.20122126562085751</v>
       </c>
-      <c r="U84" s="77">
-        <f t="shared" si="46"/>
+      <c r="U84" s="73">
+        <f t="shared" si="51"/>
         <v>0.32630974446438044</v>
       </c>
     </row>
     <row r="85" spans="1:27" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A85" s="77"/>
-      <c r="B85" s="77"/>
-      <c r="C85" s="77"/>
-      <c r="D85" s="77"/>
-      <c r="E85" s="77"/>
-      <c r="F85" s="77"/>
-      <c r="G85" s="77"/>
-      <c r="H85" s="77"/>
-      <c r="I85" s="77"/>
-      <c r="J85" s="77"/>
-      <c r="K85" s="77"/>
-      <c r="L85" s="77"/>
-      <c r="M85" s="77"/>
-      <c r="N85" s="77"/>
-      <c r="O85" s="77"/>
-      <c r="P85" s="77"/>
-      <c r="Q85" s="77"/>
-      <c r="R85" s="77"/>
-      <c r="S85" s="77"/>
-      <c r="T85" s="77"/>
+      <c r="A85" s="73"/>
+      <c r="B85" s="73"/>
+      <c r="C85" s="73"/>
+      <c r="D85" s="73"/>
+      <c r="E85" s="73"/>
+      <c r="F85" s="73"/>
+      <c r="G85" s="73"/>
+      <c r="H85" s="73"/>
+      <c r="I85" s="73"/>
+      <c r="J85" s="73"/>
+      <c r="K85" s="73"/>
+      <c r="L85" s="73"/>
+      <c r="M85" s="73"/>
+      <c r="N85" s="73"/>
+      <c r="O85" s="73"/>
+      <c r="P85" s="73"/>
+      <c r="Q85" s="73"/>
+      <c r="R85" s="73"/>
+      <c r="S85" s="73"/>
+      <c r="T85" s="73"/>
     </row>
     <row r="86" spans="1:27" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A86" s="77"/>
-      <c r="B86" s="78" t="s">
+      <c r="A86" s="73"/>
+      <c r="B86" s="74" t="s">
         <v>196</v>
       </c>
-      <c r="C86" s="79" t="s">
+      <c r="C86" s="75" t="s">
         <v>377</v>
       </c>
-      <c r="D86" s="79" t="s">
+      <c r="D86" s="75" t="s">
         <v>375</v>
       </c>
-      <c r="E86" s="78" t="s">
+      <c r="E86" s="74" t="s">
         <v>376</v>
       </c>
-      <c r="F86" s="77"/>
-      <c r="G86" s="77"/>
-      <c r="H86" s="77"/>
-      <c r="I86" s="77"/>
-      <c r="J86" s="77"/>
-      <c r="K86" s="77"/>
-      <c r="L86" s="77"/>
-      <c r="M86" s="77"/>
-      <c r="N86" s="77"/>
-      <c r="O86" s="77"/>
-      <c r="P86" s="77"/>
-      <c r="Q86" s="77"/>
-      <c r="R86" s="77"/>
-      <c r="S86" s="77"/>
-      <c r="T86" s="77"/>
-      <c r="U86" s="77"/>
-      <c r="V86" s="77"/>
-      <c r="W86" s="77"/>
-      <c r="X86" s="77"/>
-      <c r="Y86" s="77"/>
-      <c r="Z86" s="77"/>
-      <c r="AA86" s="76"/>
+      <c r="F86" s="73"/>
+      <c r="G86" s="73"/>
+      <c r="H86" s="73"/>
+      <c r="I86" s="73"/>
+      <c r="J86" s="73"/>
+      <c r="K86" s="73"/>
+      <c r="L86" s="73"/>
+      <c r="M86" s="73"/>
+      <c r="N86" s="73"/>
+      <c r="O86" s="73"/>
+      <c r="P86" s="73"/>
+      <c r="Q86" s="73"/>
+      <c r="R86" s="73"/>
+      <c r="S86" s="73"/>
+      <c r="T86" s="73"/>
+      <c r="U86" s="73"/>
+      <c r="V86" s="73"/>
+      <c r="W86" s="73"/>
+      <c r="X86" s="73"/>
+      <c r="Y86" s="73"/>
+      <c r="Z86" s="73"/>
+      <c r="AA86" s="72"/>
     </row>
     <row r="87" spans="1:27" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A87" s="77"/>
-      <c r="B87" s="77">
+      <c r="A87" s="73"/>
+      <c r="B87" s="73">
         <v>1</v>
       </c>
-      <c r="C87" s="77">
+      <c r="C87" s="73">
         <v>0.16896054900000013</v>
       </c>
-      <c r="D87" s="77">
+      <c r="D87" s="73">
         <v>1.4264137800000007</v>
       </c>
-      <c r="E87" s="77">
+      <c r="E87" s="73">
         <v>1.3817830400000002</v>
       </c>
-      <c r="F87" s="77"/>
-      <c r="G87" s="77"/>
-      <c r="H87" s="77"/>
-      <c r="I87" s="77"/>
-      <c r="J87" s="77"/>
-      <c r="K87" s="77"/>
-      <c r="L87" s="77"/>
-      <c r="M87" s="77"/>
-      <c r="N87" s="77"/>
-      <c r="O87" s="77"/>
-      <c r="P87" s="77"/>
-      <c r="Q87" s="77"/>
-      <c r="R87" s="77"/>
-      <c r="S87" s="77"/>
-      <c r="T87" s="77"/>
-      <c r="U87" s="77"/>
-      <c r="V87" s="77"/>
-      <c r="W87" s="77"/>
-      <c r="X87" s="77"/>
-      <c r="Y87" s="77"/>
-      <c r="Z87" s="77"/>
-      <c r="AA87" s="76"/>
+      <c r="F87" s="73"/>
+      <c r="G87" s="73"/>
+      <c r="H87" s="73"/>
+      <c r="I87" s="73"/>
+      <c r="J87" s="73"/>
+      <c r="K87" s="73"/>
+      <c r="L87" s="73"/>
+      <c r="M87" s="73"/>
+      <c r="N87" s="73"/>
+      <c r="O87" s="73"/>
+      <c r="P87" s="73"/>
+      <c r="Q87" s="73"/>
+      <c r="R87" s="73"/>
+      <c r="S87" s="73"/>
+      <c r="T87" s="73"/>
+      <c r="U87" s="73"/>
+      <c r="V87" s="73"/>
+      <c r="W87" s="73"/>
+      <c r="X87" s="73"/>
+      <c r="Y87" s="73"/>
+      <c r="Z87" s="73"/>
+      <c r="AA87" s="72"/>
     </row>
     <row r="88" spans="1:27" ht="15.75" customHeight="1">
       <c r="B88">
@@ -14510,20 +15816,20 @@
       <c r="E88">
         <v>0.77549188999999963</v>
       </c>
-      <c r="H88" s="77"/>
-      <c r="I88" s="77"/>
-      <c r="J88" s="77"/>
-      <c r="K88" s="77"/>
-      <c r="L88" s="77"/>
-      <c r="M88" s="77"/>
-      <c r="N88" s="77"/>
-      <c r="O88" s="77"/>
-      <c r="P88" s="77"/>
-      <c r="Q88" s="77"/>
-      <c r="R88" s="77"/>
-      <c r="S88" s="77"/>
-      <c r="T88" s="77"/>
-      <c r="U88" s="77"/>
+      <c r="H88" s="73"/>
+      <c r="I88" s="73"/>
+      <c r="J88" s="73"/>
+      <c r="K88" s="73"/>
+      <c r="L88" s="73"/>
+      <c r="M88" s="73"/>
+      <c r="N88" s="73"/>
+      <c r="O88" s="73"/>
+      <c r="P88" s="73"/>
+      <c r="Q88" s="73"/>
+      <c r="R88" s="73"/>
+      <c r="S88" s="73"/>
+      <c r="T88" s="73"/>
+      <c r="U88" s="73"/>
     </row>
     <row r="89" spans="1:27" ht="15.75" customHeight="1">
       <c r="B89">
@@ -14538,20 +15844,20 @@
       <c r="E89">
         <v>0.84270061999999868</v>
       </c>
-      <c r="G89" s="77"/>
-      <c r="H89" s="77"/>
-      <c r="I89" s="77"/>
-      <c r="J89" s="77"/>
-      <c r="K89" s="77"/>
-      <c r="L89" s="77"/>
-      <c r="M89" s="77"/>
-      <c r="N89" s="77"/>
-      <c r="O89" s="77"/>
-      <c r="P89" s="77"/>
-      <c r="Q89" s="77"/>
-      <c r="R89" s="77"/>
-      <c r="S89" s="77"/>
-      <c r="T89" s="77"/>
+      <c r="G89" s="73"/>
+      <c r="H89" s="73"/>
+      <c r="I89" s="73"/>
+      <c r="J89" s="73"/>
+      <c r="K89" s="73"/>
+      <c r="L89" s="73"/>
+      <c r="M89" s="73"/>
+      <c r="N89" s="73"/>
+      <c r="O89" s="73"/>
+      <c r="P89" s="73"/>
+      <c r="Q89" s="73"/>
+      <c r="R89" s="73"/>
+      <c r="S89" s="73"/>
+      <c r="T89" s="73"/>
     </row>
     <row r="90" spans="1:27" ht="15.75" customHeight="1">
       <c r="B90">
@@ -14566,160 +15872,284 @@
       <c r="E90">
         <v>0.89407403000000052</v>
       </c>
-      <c r="G90" s="77"/>
-      <c r="H90" s="77"/>
-      <c r="I90" s="77"/>
-      <c r="J90" s="77"/>
-      <c r="K90" s="77"/>
-      <c r="L90" s="77"/>
-      <c r="M90" s="77"/>
-      <c r="N90" s="77"/>
-      <c r="O90" s="77"/>
-      <c r="P90" s="77"/>
-      <c r="Q90" s="77"/>
-      <c r="R90" s="77"/>
-      <c r="S90" s="77"/>
-      <c r="T90" s="77"/>
+      <c r="G90" s="73"/>
+      <c r="H90" s="73"/>
+      <c r="I90" s="73"/>
+      <c r="J90" s="73"/>
+      <c r="K90" s="73"/>
+      <c r="L90" s="80" t="s">
+        <v>383</v>
+      </c>
+      <c r="M90" s="73"/>
+      <c r="N90" s="73"/>
+      <c r="O90" s="73"/>
+      <c r="P90" s="73"/>
+      <c r="Q90" s="73"/>
+      <c r="R90" s="73"/>
+      <c r="S90" s="73"/>
+      <c r="T90" s="73"/>
     </row>
     <row r="91" spans="1:27" ht="15.75" customHeight="1">
-      <c r="G91" s="77"/>
-      <c r="H91" s="77"/>
-      <c r="I91" s="77"/>
-      <c r="J91" s="77"/>
-      <c r="K91" s="77"/>
-      <c r="L91" s="77"/>
-      <c r="M91" s="77"/>
-      <c r="N91" s="77"/>
-      <c r="O91" s="77"/>
-      <c r="P91" s="77"/>
-      <c r="Q91" s="77"/>
-      <c r="R91" s="77"/>
-      <c r="S91" s="77"/>
-      <c r="T91" s="77"/>
+      <c r="G91" s="73"/>
+      <c r="H91" s="73"/>
+      <c r="I91" s="73"/>
+      <c r="J91" s="73"/>
+      <c r="K91" s="73" t="s">
+        <v>196</v>
+      </c>
+      <c r="L91" s="73" t="s">
+        <v>379</v>
+      </c>
+      <c r="M91" s="73" t="s">
+        <v>380</v>
+      </c>
+      <c r="N91" s="73" t="s">
+        <v>381</v>
+      </c>
+      <c r="O91" s="73" t="s">
+        <v>382</v>
+      </c>
+      <c r="P91" s="73" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q91" s="73" t="s">
+        <v>385</v>
+      </c>
+      <c r="R91" s="73" t="s">
+        <v>386</v>
+      </c>
+      <c r="S91" s="73" t="s">
+        <v>387</v>
+      </c>
+      <c r="T91" s="73"/>
     </row>
     <row r="92" spans="1:27" ht="15.75" customHeight="1">
-      <c r="G92" s="77"/>
-      <c r="H92" s="77"/>
-      <c r="I92" s="77"/>
-      <c r="J92" s="77"/>
-      <c r="K92" s="77"/>
-      <c r="L92" s="77"/>
-      <c r="M92" s="77"/>
-      <c r="N92" s="77"/>
-      <c r="O92" s="77"/>
-      <c r="P92" s="77"/>
-      <c r="Q92" s="77"/>
-      <c r="R92" s="77"/>
-      <c r="S92" s="77"/>
-      <c r="T92" s="77"/>
+      <c r="G92" s="73"/>
+      <c r="H92" s="73"/>
+      <c r="I92" s="73"/>
+      <c r="J92" s="73"/>
+      <c r="K92" s="73">
+        <v>1</v>
+      </c>
+      <c r="L92" s="73">
+        <f>AVERAGE(E77:E78)</f>
+        <v>11.908789844999999</v>
+      </c>
+      <c r="M92" s="73">
+        <f>AVERAGE(E75:E76)</f>
+        <v>11.857586510000001</v>
+      </c>
+      <c r="N92" s="73">
+        <f>E74</f>
+        <v>13.12447721</v>
+      </c>
+      <c r="O92" s="73">
+        <f>AVERAGE(11.79,11.97)</f>
+        <v>11.879999999999999</v>
+      </c>
+      <c r="P92" s="73">
+        <f>AVERAGE(F77:F78)</f>
+        <v>11.831386155000001</v>
+      </c>
+      <c r="Q92" s="73">
+        <f>AVERAGE(F75:F76)</f>
+        <v>11.724543785</v>
+      </c>
+      <c r="R92">
+        <f>F74</f>
+        <v>12.913345469999999</v>
+      </c>
+      <c r="S92" s="73">
+        <f>AVERAGE(11.05,11.59)</f>
+        <v>11.32</v>
+      </c>
+      <c r="T92" s="73"/>
     </row>
     <row r="93" spans="1:27" ht="15.75" customHeight="1">
-      <c r="G93" s="77"/>
-      <c r="H93" s="77"/>
-      <c r="I93" s="77"/>
-      <c r="J93" s="77"/>
-      <c r="K93" s="77"/>
-      <c r="L93" s="77"/>
-      <c r="M93" s="77"/>
-      <c r="N93" s="77"/>
-      <c r="O93" s="77"/>
-      <c r="P93" s="77"/>
-      <c r="Q93" s="77"/>
-      <c r="R93" s="77"/>
-      <c r="S93" s="77"/>
-      <c r="T93" s="77"/>
+      <c r="G93" s="73"/>
+      <c r="H93" s="73"/>
+      <c r="I93" s="73"/>
+      <c r="J93" s="73"/>
+      <c r="K93" s="73">
+        <v>2</v>
+      </c>
+      <c r="L93" s="73">
+        <f>AVERAGE(J77:J78)</f>
+        <v>10.511600475</v>
+      </c>
+      <c r="M93" s="73">
+        <f>AVERAGE(J75:J76)</f>
+        <v>10.58447911</v>
+      </c>
+      <c r="N93" s="73">
+        <f>J74</f>
+        <v>11.00523155</v>
+      </c>
+      <c r="O93" s="73">
+        <f>AVERAGE(11.91,12.88)</f>
+        <v>12.395</v>
+      </c>
+      <c r="P93" s="73">
+        <f>AVERAGE(K77:K78)</f>
+        <v>10.549725084999999</v>
+      </c>
+      <c r="Q93" s="73">
+        <f>AVERAGE(K75:K76)</f>
+        <v>10.38107684</v>
+      </c>
+      <c r="R93" s="73">
+        <f>K74</f>
+        <v>10.60252912</v>
+      </c>
+      <c r="S93" s="73">
+        <f>AVERAGE(11.51,11.41)</f>
+        <v>11.46</v>
+      </c>
+      <c r="T93" s="73"/>
     </row>
     <row r="94" spans="1:27" ht="15.75" customHeight="1">
-      <c r="G94" s="77"/>
-      <c r="H94" s="77"/>
-      <c r="I94" s="77"/>
-      <c r="J94" s="77"/>
-      <c r="K94" s="77"/>
-      <c r="L94" s="77"/>
-      <c r="M94" s="77"/>
-      <c r="N94" s="77"/>
-      <c r="O94" s="77"/>
-      <c r="P94" s="77"/>
-      <c r="Q94" s="77"/>
-      <c r="R94" s="77"/>
-      <c r="S94" s="77"/>
-      <c r="T94" s="77"/>
+      <c r="G94" s="73"/>
+      <c r="H94" s="73"/>
+      <c r="I94" s="73"/>
+      <c r="J94" s="73"/>
+      <c r="K94" s="73">
+        <v>3</v>
+      </c>
+      <c r="L94" s="73">
+        <f>AVERAGE(O77:O78)</f>
+        <v>11.576088309999999</v>
+      </c>
+      <c r="M94" s="73">
+        <f>AVERAGE(O75:O76)</f>
+        <v>11.346393774999999</v>
+      </c>
+      <c r="N94" s="73">
+        <f>O74</f>
+        <v>11.737313759999999</v>
+      </c>
+      <c r="O94" s="73">
+        <f>AVERAGE(11.43,11.51)</f>
+        <v>11.469999999999999</v>
+      </c>
+      <c r="P94" s="73">
+        <f>AVERAGE(P77:P78)</f>
+        <v>11.471758205</v>
+      </c>
+      <c r="Q94" s="73">
+        <f>AVERAGE(P75:P76)</f>
+        <v>10.864205569999999</v>
+      </c>
+      <c r="R94" s="73">
+        <f>P74</f>
+        <v>11.41887084</v>
+      </c>
+      <c r="S94" s="73">
+        <f>AVERAGE(10.93,10.98)</f>
+        <v>10.955</v>
+      </c>
+      <c r="T94" s="73"/>
     </row>
     <row r="95" spans="1:27" ht="15.75" customHeight="1">
-      <c r="G95" s="77"/>
-      <c r="H95" s="77"/>
-      <c r="I95" s="77"/>
-      <c r="J95" s="77"/>
-      <c r="K95" s="77"/>
-      <c r="L95" s="77"/>
-      <c r="M95" s="77"/>
-      <c r="N95" s="77"/>
-      <c r="O95" s="77"/>
-      <c r="P95" s="77"/>
-      <c r="Q95" s="77"/>
-      <c r="R95" s="77"/>
-      <c r="S95" s="77"/>
-      <c r="T95" s="77"/>
+      <c r="G95" s="73"/>
+      <c r="H95" s="73"/>
+      <c r="I95" s="73"/>
+      <c r="J95" s="73"/>
+      <c r="K95" s="73">
+        <v>4</v>
+      </c>
+      <c r="L95" s="73">
+        <f>AVERAGE(T77:T78)</f>
+        <v>10.736576370000002</v>
+      </c>
+      <c r="M95" s="73">
+        <f>AVERAGE(T75:T76)</f>
+        <v>11.080272190000001</v>
+      </c>
+      <c r="N95" s="73">
+        <f>T74</f>
+        <v>10.98796596</v>
+      </c>
+      <c r="O95" s="73">
+        <f>AVERAGE(11.63,11.26)</f>
+        <v>11.445</v>
+      </c>
+      <c r="P95" s="73">
+        <f>AVERAGE(U77:U78)</f>
+        <v>11.167520115</v>
+      </c>
+      <c r="Q95" s="73">
+        <f>AVERAGE(U75:U76)</f>
+        <v>10.53917869</v>
+      </c>
+      <c r="R95" s="73">
+        <f>U74</f>
+        <v>11.078948069999999</v>
+      </c>
+      <c r="S95" s="73">
+        <f>AVERAGE(10.93,10.9)</f>
+        <v>10.914999999999999</v>
+      </c>
+      <c r="T95" s="73"/>
     </row>
     <row r="96" spans="1:27" ht="15.75" customHeight="1">
-      <c r="G96" s="77"/>
-      <c r="H96" s="77"/>
-      <c r="I96" s="77"/>
-      <c r="J96" s="77"/>
-      <c r="K96" s="77"/>
-      <c r="L96" s="77"/>
-      <c r="M96" s="77"/>
-      <c r="N96" s="77"/>
-      <c r="O96" s="77"/>
-      <c r="P96" s="77"/>
-      <c r="Q96" s="77"/>
-      <c r="R96" s="77"/>
-      <c r="S96" s="77"/>
-      <c r="T96" s="77"/>
+      <c r="G96" s="73"/>
+      <c r="H96" s="73"/>
+      <c r="I96" s="73"/>
+      <c r="J96" s="73"/>
+      <c r="K96" s="73"/>
+      <c r="L96" s="73"/>
+      <c r="M96" s="73"/>
+      <c r="N96" s="73"/>
+      <c r="O96" s="73"/>
+      <c r="P96" s="73"/>
+      <c r="Q96" s="73"/>
+      <c r="R96" s="73"/>
+      <c r="S96" s="73"/>
+      <c r="T96" s="73"/>
     </row>
     <row r="97" spans="7:20" ht="15.75" customHeight="1">
-      <c r="G97" s="77"/>
-      <c r="H97" s="77"/>
-      <c r="I97" s="77"/>
-      <c r="J97" s="77"/>
-      <c r="K97" s="77"/>
-      <c r="L97" s="77"/>
-      <c r="M97" s="77"/>
-      <c r="N97" s="77"/>
-      <c r="O97" s="77"/>
-      <c r="P97" s="77"/>
-      <c r="Q97" s="77"/>
-      <c r="R97" s="77"/>
-      <c r="S97" s="77"/>
-      <c r="T97" s="77"/>
+      <c r="G97" s="73"/>
+      <c r="H97" s="73"/>
+      <c r="I97" s="73"/>
+      <c r="J97" s="73"/>
+      <c r="K97" s="73"/>
+      <c r="L97" s="73"/>
+      <c r="M97" s="73"/>
+      <c r="N97" s="73"/>
+      <c r="O97" s="73"/>
+      <c r="P97" s="73"/>
+      <c r="Q97" s="73"/>
+      <c r="R97" s="73"/>
+      <c r="S97" s="73"/>
+      <c r="T97" s="73"/>
     </row>
     <row r="98" spans="7:20" ht="15.75" customHeight="1">
-      <c r="G98" s="77"/>
-      <c r="H98" s="77"/>
-      <c r="I98" s="77"/>
-      <c r="J98" s="77"/>
-      <c r="K98" s="77"/>
-      <c r="L98" s="77"/>
-      <c r="M98" s="77"/>
-      <c r="N98" s="77"/>
-      <c r="O98" s="77"/>
-      <c r="P98" s="77"/>
-      <c r="Q98" s="77"/>
-      <c r="R98" s="77"/>
-      <c r="S98" s="77"/>
-      <c r="T98" s="77"/>
+      <c r="G98" s="73"/>
+      <c r="H98" s="73"/>
+      <c r="I98" s="73"/>
+      <c r="J98" s="73"/>
+      <c r="K98" s="73"/>
+      <c r="L98" s="73"/>
+      <c r="M98" s="73"/>
+      <c r="N98" s="73"/>
+      <c r="O98" s="73"/>
+      <c r="P98" s="73"/>
+      <c r="Q98" s="73"/>
+      <c r="R98" s="73"/>
+      <c r="S98" s="73"/>
+      <c r="T98" s="73"/>
     </row>
     <row r="99" spans="7:20" ht="15.75" customHeight="1">
-      <c r="K99" s="77"/>
-      <c r="L99" s="77"/>
-      <c r="M99" s="77"/>
-      <c r="N99" s="77"/>
-      <c r="O99" s="77"/>
-      <c r="P99" s="77"/>
-      <c r="Q99" s="77"/>
-      <c r="R99" s="77"/>
-      <c r="S99" s="77"/>
-      <c r="T99" s="77"/>
+      <c r="K99" s="73"/>
+      <c r="L99" s="73"/>
+      <c r="M99" s="73"/>
+      <c r="N99" s="73"/>
+      <c r="O99" s="73"/>
+      <c r="P99" s="73"/>
+      <c r="Q99" s="73"/>
+      <c r="R99" s="73"/>
+      <c r="S99" s="73"/>
+      <c r="T99" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -14796,36 +16226,36 @@
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="77"/>
+      <c r="K9" s="77"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="77"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="76" t="s">
         <v>225</v>
       </c>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="75" t="s">
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="79" t="s">
         <v>226</v>
       </c>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
+      <c r="J10" s="77"/>
+      <c r="K10" s="77"/>
+      <c r="L10" s="77"/>
+      <c r="M10" s="77"/>
       <c r="O10" s="1" t="s">
         <v>227</v>
       </c>
@@ -15501,36 +16931,36 @@
       </c>
     </row>
     <row r="31" spans="1:17">
-      <c r="C31" s="72" t="s">
+      <c r="C31" s="76" t="s">
         <v>230</v>
       </c>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="73"/>
-      <c r="I31" s="73"/>
-      <c r="J31" s="73"/>
-      <c r="K31" s="73"/>
-      <c r="L31" s="73"/>
-      <c r="M31" s="73"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="77"/>
+      <c r="J31" s="77"/>
+      <c r="K31" s="77"/>
+      <c r="L31" s="77"/>
+      <c r="M31" s="77"/>
     </row>
     <row r="32" spans="1:17">
-      <c r="C32" s="72" t="s">
+      <c r="C32" s="76" t="s">
         <v>225</v>
       </c>
-      <c r="D32" s="73"/>
-      <c r="E32" s="73"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="73"/>
-      <c r="I32" s="75" t="s">
+      <c r="D32" s="77"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="77"/>
+      <c r="I32" s="79" t="s">
         <v>226</v>
       </c>
-      <c r="J32" s="73"/>
-      <c r="K32" s="73"/>
-      <c r="L32" s="73"/>
-      <c r="M32" s="73"/>
+      <c r="J32" s="77"/>
+      <c r="K32" s="77"/>
+      <c r="L32" s="77"/>
+      <c r="M32" s="77"/>
       <c r="O32" s="1" t="s">
         <v>227</v>
       </c>

</xml_diff>

<commit_message>
working on sorting out the experimental values once and for all
</commit_message>
<xml_diff>
--- a/metabolicsData_revised.xlsx
+++ b/metabolicsData_revised.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2134A4-D220-4903-B4C0-ED848356537E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854A4B31-F920-42BD-B08E-D686D7E80E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1125" yWindow="1125" windowWidth="14625" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="key" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="sild" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2649" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2655" uniqueCount="391">
   <si>
     <t>Metabolic power [W/kg]</t>
   </si>
@@ -1237,6 +1238,15 @@
   <si>
     <t>exo sim</t>
   </si>
+  <si>
+    <t>All data</t>
+  </si>
+  <si>
+    <t>full</t>
+  </si>
+  <si>
+    <t>partial</t>
+  </si>
 </sst>
 </file>
 
@@ -1407,7 +1417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1548,6 +1558,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1556,7 +1567,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2356,16 +2368,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>13.12447721</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.00523155</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.737313759999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.98796596</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2530,16 +2542,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>12.913345469999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.60252912</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.41887084</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.078948069999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4118,15 +4130,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>321129</xdr:colOff>
-      <xdr:row>95</xdr:row>
-      <xdr:rowOff>96613</xdr:rowOff>
+      <xdr:colOff>8164</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>42185</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>140153</xdr:colOff>
-      <xdr:row>121</xdr:row>
-      <xdr:rowOff>10886</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>793295</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>160565</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4369,12 +4381,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="D1" s="76"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
@@ -12868,8 +12880,8 @@
   </sheetPr>
   <dimension ref="A1:AA99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T92" sqref="T92"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -12894,12 +12906,12 @@
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
-      <c r="G3" s="78" t="s">
+      <c r="G3" s="79" t="s">
         <v>170</v>
       </c>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
       <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" customHeight="1">
@@ -14908,6 +14920,77 @@
         <v>693.78056343973321</v>
       </c>
     </row>
+    <row r="68" spans="1:22" ht="15.75" customHeight="1">
+      <c r="D68" s="82" t="s">
+        <v>389</v>
+      </c>
+      <c r="N68" s="82" t="s">
+        <v>389</v>
+      </c>
+      <c r="S68" s="82" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" ht="15.75" customHeight="1">
+      <c r="D69" s="74">
+        <v>1.7843621039999999</v>
+      </c>
+      <c r="E69" s="74">
+        <v>13.12447721</v>
+      </c>
+      <c r="F69" s="74">
+        <v>12.913345469999999</v>
+      </c>
+      <c r="N69" s="74">
+        <v>1.964192763</v>
+      </c>
+      <c r="O69" s="74">
+        <v>11.914036019999999</v>
+      </c>
+      <c r="P69" s="74">
+        <v>11.509005480000001</v>
+      </c>
+      <c r="S69" s="73">
+        <v>1.8694403660000001</v>
+      </c>
+      <c r="T69" s="73">
+        <v>10.98796596</v>
+      </c>
+      <c r="U69" s="73">
+        <v>11.078948069999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" ht="15.75" customHeight="1">
+      <c r="I70" s="82" t="s">
+        <v>390</v>
+      </c>
+      <c r="N70" s="82" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" ht="15.75" customHeight="1">
+      <c r="B71" s="81" t="s">
+        <v>388</v>
+      </c>
+      <c r="I71" s="74">
+        <v>1.6121465399999999</v>
+      </c>
+      <c r="J71" s="74">
+        <v>11.00523155</v>
+      </c>
+      <c r="K71" s="74">
+        <v>10.60252912</v>
+      </c>
+      <c r="N71" s="73">
+        <v>1.8957573720000001</v>
+      </c>
+      <c r="O71" s="73">
+        <v>11.737313759999999</v>
+      </c>
+      <c r="P71" s="73">
+        <v>11.41887084</v>
+      </c>
+    </row>
     <row r="72" spans="1:22" ht="15.75" customHeight="1">
       <c r="A72" s="73"/>
       <c r="B72" s="73"/>
@@ -15020,60 +15103,36 @@
       <c r="C74" s="73">
         <v>3</v>
       </c>
-      <c r="D74" s="73">
-        <v>1.7843621039999999</v>
-      </c>
-      <c r="E74" s="73">
-        <v>13.12447721</v>
-      </c>
-      <c r="F74" s="73">
-        <v>12.913345469999999</v>
-      </c>
+      <c r="D74" s="74"/>
+      <c r="E74" s="74"/>
+      <c r="F74" s="74"/>
       <c r="G74" s="73">
         <v>2</v>
       </c>
       <c r="H74" s="73">
         <v>3</v>
       </c>
-      <c r="I74" s="73">
-        <v>1.6121465399999999</v>
-      </c>
-      <c r="J74" s="73">
-        <v>11.00523155</v>
-      </c>
-      <c r="K74" s="73">
-        <v>10.60252912</v>
-      </c>
+      <c r="I74" s="74"/>
+      <c r="J74" s="74"/>
+      <c r="K74" s="74"/>
       <c r="L74" s="73">
         <v>3</v>
       </c>
       <c r="M74" s="73">
         <v>3</v>
       </c>
-      <c r="N74" s="73">
-        <v>1.8957573720000001</v>
-      </c>
-      <c r="O74" s="73">
-        <v>11.737313759999999</v>
-      </c>
-      <c r="P74" s="73">
-        <v>11.41887084</v>
-      </c>
+      <c r="N74" s="74"/>
+      <c r="O74" s="74"/>
+      <c r="P74" s="74"/>
       <c r="Q74" s="73">
         <v>4</v>
       </c>
       <c r="R74" s="73">
         <v>3</v>
       </c>
-      <c r="S74" s="73">
-        <v>1.8694403660000001</v>
-      </c>
-      <c r="T74" s="73">
-        <v>10.98796596</v>
-      </c>
-      <c r="U74" s="73">
-        <v>11.078948069999999</v>
-      </c>
+      <c r="S74" s="73"/>
+      <c r="T74" s="73"/>
+      <c r="U74" s="73"/>
       <c r="V74" s="73"/>
     </row>
     <row r="75" spans="1:22" ht="15.75" customHeight="1">
@@ -15084,13 +15143,13 @@
       <c r="C75" s="73">
         <v>2</v>
       </c>
-      <c r="D75" s="73">
+      <c r="D75" s="76">
         <v>1.9533226530000001</v>
       </c>
-      <c r="E75" s="73">
+      <c r="E75" s="76">
         <v>11.698063429999999</v>
       </c>
-      <c r="F75" s="73">
+      <c r="F75" s="76">
         <v>11.91752514</v>
       </c>
       <c r="G75" s="73">
@@ -15099,13 +15158,13 @@
       <c r="H75" s="73">
         <v>2</v>
       </c>
-      <c r="I75" s="73">
+      <c r="I75" s="76">
         <v>1.6356537799999999</v>
       </c>
-      <c r="J75" s="73">
+      <c r="J75" s="76">
         <v>10.54304964</v>
       </c>
-      <c r="K75" s="73">
+      <c r="K75" s="76">
         <v>10.4326998</v>
       </c>
       <c r="L75" s="73">
@@ -15114,13 +15173,13 @@
       <c r="M75" s="73">
         <v>2</v>
       </c>
-      <c r="N75" s="73">
+      <c r="N75" s="76">
         <v>1.8451964569999999</v>
       </c>
-      <c r="O75" s="73">
+      <c r="O75" s="76">
         <v>11.37779744</v>
       </c>
-      <c r="P75" s="73">
+      <c r="P75" s="76">
         <v>11.05976031</v>
       </c>
       <c r="Q75" s="73">
@@ -15129,13 +15188,13 @@
       <c r="R75" s="73">
         <v>2</v>
       </c>
-      <c r="S75" s="73">
+      <c r="S75" s="76">
         <v>1.698257736</v>
       </c>
-      <c r="T75" s="73">
+      <c r="T75" s="76">
         <v>10.901165600000001</v>
       </c>
-      <c r="U75" s="73">
+      <c r="U75" s="76">
         <v>10.59103932</v>
       </c>
       <c r="V75" s="73"/>
@@ -15148,13 +15207,13 @@
       <c r="C76" s="73">
         <v>2</v>
       </c>
-      <c r="D76" s="73">
+      <c r="D76" s="76">
         <v>1.9533226530000001</v>
       </c>
-      <c r="E76" s="73">
+      <c r="E76" s="76">
         <v>12.01710959</v>
       </c>
-      <c r="F76" s="73">
+      <c r="F76" s="76">
         <v>11.531562429999999</v>
       </c>
       <c r="G76" s="73">
@@ -15163,13 +15222,13 @@
       <c r="H76" s="73">
         <v>2</v>
       </c>
-      <c r="I76" s="73">
+      <c r="I76" s="76">
         <v>1.6356537799999999</v>
       </c>
-      <c r="J76" s="73">
+      <c r="J76" s="76">
         <v>10.625908580000001</v>
       </c>
-      <c r="K76" s="73">
+      <c r="K76" s="76">
         <v>10.329453880000001</v>
       </c>
       <c r="L76" s="73">
@@ -15178,13 +15237,13 @@
       <c r="M76" s="73">
         <v>2</v>
       </c>
-      <c r="N76" s="73">
+      <c r="N76" s="76">
         <v>1.8451964569999999</v>
       </c>
-      <c r="O76" s="73">
+      <c r="O76" s="76">
         <v>11.31499011</v>
       </c>
-      <c r="P76" s="73">
+      <c r="P76" s="76">
         <v>10.668650830000001</v>
       </c>
       <c r="Q76" s="73">
@@ -15193,13 +15252,13 @@
       <c r="R76" s="73">
         <v>2</v>
       </c>
-      <c r="S76" s="73">
+      <c r="S76" s="76">
         <v>1.698257736</v>
       </c>
-      <c r="T76" s="73">
+      <c r="T76" s="76">
         <v>11.25937878</v>
       </c>
-      <c r="U76" s="73">
+      <c r="U76" s="76">
         <v>10.48731806</v>
       </c>
       <c r="V76" s="73"/>
@@ -15212,13 +15271,13 @@
       <c r="C77" s="73">
         <v>1</v>
       </c>
-      <c r="D77" s="73">
+      <c r="D77" s="76">
         <v>1.8314126049999999</v>
       </c>
-      <c r="E77" s="73">
+      <c r="E77" s="76">
         <v>11.832379469999999</v>
       </c>
-      <c r="F77" s="73">
+      <c r="F77" s="76">
         <v>11.70265908</v>
       </c>
       <c r="G77" s="73">
@@ -15227,13 +15286,13 @@
       <c r="H77" s="73">
         <v>1</v>
       </c>
-      <c r="I77" s="73">
+      <c r="I77" s="76">
         <v>1.577234099</v>
       </c>
-      <c r="J77" s="73">
+      <c r="J77" s="76">
         <v>10.75850441</v>
       </c>
-      <c r="K77" s="73">
+      <c r="K77" s="76">
         <v>10.937471029999999</v>
       </c>
       <c r="L77" s="73">
@@ -15242,13 +15301,13 @@
       <c r="M77" s="73">
         <v>1</v>
       </c>
-      <c r="N77" s="73">
+      <c r="N77" s="76">
         <v>1.6330105290000001</v>
       </c>
-      <c r="O77" s="73">
+      <c r="O77" s="76">
         <v>11.814252460000001</v>
       </c>
-      <c r="P77" s="73">
+      <c r="P77" s="76">
         <v>11.43216496</v>
       </c>
       <c r="Q77" s="73">
@@ -15257,13 +15316,13 @@
       <c r="R77" s="73">
         <v>1</v>
       </c>
-      <c r="S77" s="73">
+      <c r="S77" s="76">
         <v>1.887225025</v>
       </c>
-      <c r="T77" s="73">
+      <c r="T77" s="76">
         <v>10.823476680000001</v>
       </c>
-      <c r="U77" s="73">
+      <c r="U77" s="76">
         <v>11.38139209</v>
       </c>
       <c r="V77" s="73"/>
@@ -15276,13 +15335,13 @@
       <c r="C78" s="73">
         <v>1</v>
       </c>
-      <c r="D78" s="73">
+      <c r="D78" s="76">
         <v>1.8314126049999999</v>
       </c>
-      <c r="E78" s="73">
+      <c r="E78" s="76">
         <v>11.985200219999999</v>
       </c>
-      <c r="F78" s="73">
+      <c r="F78" s="76">
         <v>11.960113229999999</v>
       </c>
       <c r="G78" s="73">
@@ -15291,13 +15350,13 @@
       <c r="H78" s="73">
         <v>1</v>
       </c>
-      <c r="I78" s="73">
+      <c r="I78" s="76">
         <v>1.577234099</v>
       </c>
-      <c r="J78" s="73">
+      <c r="J78" s="76">
         <v>10.264696539999999</v>
       </c>
-      <c r="K78" s="73">
+      <c r="K78" s="76">
         <v>10.16197914</v>
       </c>
       <c r="L78" s="73">
@@ -15306,13 +15365,13 @@
       <c r="M78" s="73">
         <v>1</v>
       </c>
-      <c r="N78" s="73">
+      <c r="N78" s="76">
         <v>1.6330105290000001</v>
       </c>
-      <c r="O78" s="73">
+      <c r="O78" s="76">
         <v>11.33792416</v>
       </c>
-      <c r="P78" s="73">
+      <c r="P78" s="76">
         <v>11.511351449999999</v>
       </c>
       <c r="Q78" s="73">
@@ -15321,13 +15380,13 @@
       <c r="R78" s="73">
         <v>1</v>
       </c>
-      <c r="S78" s="73">
+      <c r="S78" s="76">
         <v>1.887225025</v>
       </c>
-      <c r="T78" s="73">
+      <c r="T78" s="76">
         <v>10.649676060000001</v>
       </c>
-      <c r="U78" s="73">
+      <c r="U78" s="76">
         <v>10.95364814</v>
       </c>
       <c r="V78" s="73"/>
@@ -15364,15 +15423,15 @@
       </c>
       <c r="D80" s="73">
         <f>AVERAGE(D74:D78)</f>
-        <v>1.870766524</v>
+        <v>1.892367629</v>
       </c>
       <c r="E80" s="73">
         <f t="shared" ref="E80:F80" si="32">AVERAGE(E74:E78)</f>
-        <v>12.131445984000001</v>
+        <v>11.883188177499999</v>
       </c>
       <c r="F80" s="73">
         <f t="shared" si="32"/>
-        <v>12.005041070000001</v>
+        <v>11.777964969999999</v>
       </c>
       <c r="G80" s="73"/>
       <c r="H80" s="73" t="s">
@@ -15380,15 +15439,15 @@
       </c>
       <c r="I80" s="73">
         <f>AVERAGE(I74:I78)</f>
-        <v>1.6075844596</v>
+        <v>1.6064439395000001</v>
       </c>
       <c r="J80" s="73">
         <f t="shared" ref="J80:K80" si="33">AVERAGE(J74:J78)</f>
-        <v>10.639478144</v>
+        <v>10.548039792499999</v>
       </c>
       <c r="K80" s="73">
         <f t="shared" si="33"/>
-        <v>10.492826594</v>
+        <v>10.4654009625</v>
       </c>
       <c r="L80" s="73"/>
       <c r="M80" s="73" t="s">
@@ -15396,15 +15455,15 @@
       </c>
       <c r="N80" s="73">
         <f>AVERAGE(N74:N78)</f>
-        <v>1.7704342688000001</v>
+        <v>1.739103493</v>
       </c>
       <c r="O80" s="73">
         <f t="shared" ref="O80:P80" si="34">AVERAGE(O74:O78)</f>
-        <v>11.516455585999999</v>
+        <v>11.461241042499999</v>
       </c>
       <c r="P80" s="73">
         <f t="shared" si="34"/>
-        <v>11.218159678000001</v>
+        <v>11.1679818875</v>
       </c>
       <c r="Q80" s="73"/>
       <c r="R80" s="73" t="s">
@@ -15412,15 +15471,15 @@
       </c>
       <c r="S80" s="73">
         <f>AVERAGE(S74:S78)</f>
-        <v>1.8080811776000001</v>
+        <v>1.7927413805000001</v>
       </c>
       <c r="T80" s="73">
         <f t="shared" ref="T80:U80" si="35">AVERAGE(T74:T78)</f>
-        <v>10.924332616000001</v>
+        <v>10.908424280000002</v>
       </c>
       <c r="U80" s="73">
         <f t="shared" si="35"/>
-        <v>10.898469135999999</v>
+        <v>10.853349402499999</v>
       </c>
       <c r="V80" s="73"/>
     </row>
@@ -15432,7 +15491,7 @@
       </c>
       <c r="D81" s="73">
         <f>MIN(D74:D78)</f>
-        <v>1.7843621039999999</v>
+        <v>1.8314126049999999</v>
       </c>
       <c r="E81" s="73">
         <f t="shared" ref="E81:F81" si="36">MIN(E74:E78)</f>
@@ -15504,11 +15563,11 @@
       </c>
       <c r="E82" s="73">
         <f t="shared" ref="E82:F82" si="40">MAX(E74:E78)</f>
-        <v>13.12447721</v>
+        <v>12.01710959</v>
       </c>
       <c r="F82" s="73">
         <f t="shared" si="40"/>
-        <v>12.913345469999999</v>
+        <v>11.960113229999999</v>
       </c>
       <c r="G82" s="73"/>
       <c r="H82" s="73" t="s">
@@ -15520,7 +15579,7 @@
       </c>
       <c r="J82" s="73">
         <f t="shared" ref="J82:K82" si="41">MAX(J74:J78)</f>
-        <v>11.00523155</v>
+        <v>10.75850441</v>
       </c>
       <c r="K82" s="73">
         <f t="shared" si="41"/>
@@ -15532,7 +15591,7 @@
       </c>
       <c r="N82" s="73">
         <f>MAX(N74:N78)</f>
-        <v>1.8957573720000001</v>
+        <v>1.8451964569999999</v>
       </c>
       <c r="O82" s="73">
         <f t="shared" ref="O82:P82" si="42">MAX(O74:O78)</f>
@@ -15568,15 +15627,15 @@
       </c>
       <c r="D83" s="73">
         <f>D82-D81</f>
-        <v>0.16896054900000013</v>
+        <v>0.12191004800000016</v>
       </c>
       <c r="E83" s="73">
         <f t="shared" ref="E83" si="44">E82-E81</f>
-        <v>1.4264137800000007</v>
+        <v>0.31904616000000097</v>
       </c>
       <c r="F83" s="73">
         <f t="shared" ref="F83" si="45">F82-F81</f>
-        <v>1.3817830400000002</v>
+        <v>0.42855080000000001</v>
       </c>
       <c r="G83" s="73"/>
       <c r="H83" s="73" t="s">
@@ -15588,7 +15647,7 @@
       </c>
       <c r="J83" s="73">
         <f t="shared" ref="J83" si="46">J82-J81</f>
-        <v>0.74053501000000033</v>
+        <v>0.49380787000000126</v>
       </c>
       <c r="K83" s="73">
         <f t="shared" ref="K83" si="47">K82-K81</f>
@@ -15600,7 +15659,7 @@
       </c>
       <c r="N83" s="73">
         <f>N82-N81</f>
-        <v>0.26274684299999995</v>
+        <v>0.2121859279999998</v>
       </c>
       <c r="O83" s="73">
         <f t="shared" ref="O83" si="48">O82-O81</f>
@@ -15636,15 +15695,15 @@
       </c>
       <c r="D84" s="73">
         <f>_xlfn.STDEV.P(D74:D78)</f>
-        <v>6.9561792023758062E-2</v>
+        <v>6.095502400000008E-2</v>
       </c>
       <c r="E84" s="73">
         <f t="shared" ref="E84:U84" si="51">_xlfn.STDEV.P(E74:E78)</f>
-        <v>0.50947676457314639</v>
+        <v>0.12766567513996913</v>
       </c>
       <c r="F84" s="73">
         <f t="shared" si="51"/>
-        <v>0.47964806312186858</v>
+        <v>0.17251102751606953</v>
       </c>
       <c r="G84" s="73">
         <f t="shared" si="51"/>
@@ -15656,15 +15715,15 @@
       </c>
       <c r="I84" s="73">
         <f t="shared" si="51"/>
-        <v>2.6225464152658324E-2</v>
+        <v>2.9209840499999973E-2</v>
       </c>
       <c r="J84" s="73">
         <f t="shared" si="51"/>
-        <v>0.24408467635070619</v>
+        <v>0.18073959419935789</v>
       </c>
       <c r="K84" s="73">
         <f t="shared" si="51"/>
-        <v>0.26438957299079113</v>
+        <v>0.28916514583702363</v>
       </c>
       <c r="L84" s="73">
         <f t="shared" si="51"/>
@@ -15676,15 +15735,15 @@
       </c>
       <c r="N84" s="73">
         <f t="shared" si="51"/>
-        <v>0.11371474687639985</v>
+        <v>0.1060929639999999</v>
       </c>
       <c r="O84" s="73">
         <f t="shared" si="51"/>
-        <v>0.21407905116028678</v>
+        <v>0.2050465096326782</v>
       </c>
       <c r="P84" s="73">
         <f t="shared" si="51"/>
-        <v>0.31594144402305796</v>
+        <v>0.33493983305499708</v>
       </c>
       <c r="Q84" s="73">
         <f t="shared" si="51"/>
@@ -15696,15 +15755,15 @@
       </c>
       <c r="S84" s="73">
         <f t="shared" si="51"/>
-        <v>8.990530998043765E-2</v>
+        <v>9.4483644500000019E-2</v>
       </c>
       <c r="T84" s="73">
         <f t="shared" si="51"/>
-        <v>0.20122126562085751</v>
+        <v>0.22214211982676796</v>
       </c>
       <c r="U84" s="73">
         <f t="shared" si="51"/>
-        <v>0.32630974446438044</v>
+        <v>0.35059750414108276</v>
       </c>
     </row>
     <row r="85" spans="1:27" ht="15.75" customHeight="1" thickBot="1">
@@ -15877,7 +15936,7 @@
       <c r="I90" s="73"/>
       <c r="J90" s="73"/>
       <c r="K90" s="73"/>
-      <c r="L90" s="80" t="s">
+      <c r="L90" s="76" t="s">
         <v>383</v>
       </c>
       <c r="M90" s="73"/>
@@ -15941,7 +16000,7 @@
       </c>
       <c r="N92" s="73">
         <f>E74</f>
-        <v>13.12447721</v>
+        <v>0</v>
       </c>
       <c r="O92" s="73">
         <f>AVERAGE(11.79,11.97)</f>
@@ -15957,7 +16016,7 @@
       </c>
       <c r="R92">
         <f>F74</f>
-        <v>12.913345469999999</v>
+        <v>0</v>
       </c>
       <c r="S92" s="73">
         <f>AVERAGE(11.05,11.59)</f>
@@ -15983,7 +16042,7 @@
       </c>
       <c r="N93" s="73">
         <f>J74</f>
-        <v>11.00523155</v>
+        <v>0</v>
       </c>
       <c r="O93" s="73">
         <f>AVERAGE(11.91,12.88)</f>
@@ -15999,7 +16058,7 @@
       </c>
       <c r="R93" s="73">
         <f>K74</f>
-        <v>10.60252912</v>
+        <v>0</v>
       </c>
       <c r="S93" s="73">
         <f>AVERAGE(11.51,11.41)</f>
@@ -16025,7 +16084,7 @@
       </c>
       <c r="N94" s="73">
         <f>O74</f>
-        <v>11.737313759999999</v>
+        <v>0</v>
       </c>
       <c r="O94" s="73">
         <f>AVERAGE(11.43,11.51)</f>
@@ -16041,7 +16100,7 @@
       </c>
       <c r="R94" s="73">
         <f>P74</f>
-        <v>11.41887084</v>
+        <v>0</v>
       </c>
       <c r="S94" s="73">
         <f>AVERAGE(10.93,10.98)</f>
@@ -16067,7 +16126,7 @@
       </c>
       <c r="N95" s="73">
         <f>T74</f>
-        <v>10.98796596</v>
+        <v>0</v>
       </c>
       <c r="O95" s="73">
         <f>AVERAGE(11.63,11.26)</f>
@@ -16083,7 +16142,7 @@
       </c>
       <c r="R95" s="73">
         <f>U74</f>
-        <v>11.078948069999999</v>
+        <v>0</v>
       </c>
       <c r="S95" s="73">
         <f>AVERAGE(10.93,10.9)</f>
@@ -16226,36 +16285,36 @@
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="C9" s="76" t="s">
+      <c r="C9" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="77"/>
-      <c r="K9" s="77"/>
-      <c r="L9" s="77"/>
-      <c r="M9" s="77"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="78"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="C10" s="76" t="s">
+      <c r="C10" s="77" t="s">
         <v>225</v>
       </c>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="79" t="s">
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="80" t="s">
         <v>226</v>
       </c>
-      <c r="J10" s="77"/>
-      <c r="K10" s="77"/>
-      <c r="L10" s="77"/>
-      <c r="M10" s="77"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="78"/>
       <c r="O10" s="1" t="s">
         <v>227</v>
       </c>
@@ -16931,36 +16990,36 @@
       </c>
     </row>
     <row r="31" spans="1:17">
-      <c r="C31" s="76" t="s">
+      <c r="C31" s="77" t="s">
         <v>230</v>
       </c>
-      <c r="D31" s="77"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="77"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="77"/>
-      <c r="J31" s="77"/>
-      <c r="K31" s="77"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="77"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="78"/>
+      <c r="G31" s="78"/>
+      <c r="H31" s="78"/>
+      <c r="I31" s="78"/>
+      <c r="J31" s="78"/>
+      <c r="K31" s="78"/>
+      <c r="L31" s="78"/>
+      <c r="M31" s="78"/>
     </row>
     <row r="32" spans="1:17">
-      <c r="C32" s="76" t="s">
+      <c r="C32" s="77" t="s">
         <v>225</v>
       </c>
-      <c r="D32" s="77"/>
-      <c r="E32" s="77"/>
-      <c r="F32" s="77"/>
-      <c r="G32" s="77"/>
-      <c r="H32" s="77"/>
-      <c r="I32" s="79" t="s">
+      <c r="D32" s="78"/>
+      <c r="E32" s="78"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="78"/>
+      <c r="H32" s="78"/>
+      <c r="I32" s="80" t="s">
         <v>226</v>
       </c>
-      <c r="J32" s="77"/>
-      <c r="K32" s="77"/>
-      <c r="L32" s="77"/>
-      <c r="M32" s="77"/>
+      <c r="J32" s="78"/>
+      <c r="K32" s="78"/>
+      <c r="L32" s="78"/>
+      <c r="M32" s="78"/>
       <c r="O32" s="1" t="s">
         <v>227</v>
       </c>

</xml_diff>

<commit_message>
have all the gross values for all the subjects now... going to go through the rest of the sheet, and other sheets to make sure things are up-to-date
</commit_message>
<xml_diff>
--- a/metabolicsData_revised.xlsx
+++ b/metabolicsData_revised.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854A4B31-F920-42BD-B08E-D686D7E80E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C181825C-C9F9-4B71-8CBE-3E2817F86D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1125" yWindow="1125" windowWidth="14625" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="key" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2655" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2650" uniqueCount="389">
   <si>
     <t>Metabolic power [W/kg]</t>
   </si>
@@ -1241,12 +1241,6 @@
   <si>
     <t>All data</t>
   </si>
-  <si>
-    <t>full</t>
-  </si>
-  <si>
-    <t>partial</t>
-  </si>
 </sst>
 </file>
 
@@ -1255,7 +1249,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m\-d"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1342,8 +1336,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1380,6 +1381,11 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1414,10 +1420,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1559,6 +1566,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1567,10 +1576,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1718,16 +1731,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.16896054900000013</c:v>
+                  <c:v>0.17421305799999987</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.8419680999999946E-2</c:v>
+                  <c:v>0.10115337700000016</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.26274684299999995</c:v>
+                  <c:v>0.32648271800000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.18896728900000004</c:v>
+                  <c:v>0.12857113099999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1796,16 +1809,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.4264137800000007</c:v>
+                  <c:v>1.5342937600000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.74053501000000033</c:v>
+                  <c:v>0.90151375000000122</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.49926235000000041</c:v>
+                  <c:v>0.59257189000000032</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.60970271999999959</c:v>
+                  <c:v>0.59759501999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1874,16 +1887,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.3817830400000002</c:v>
+                  <c:v>1.4378871599999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.77549188999999963</c:v>
+                  <c:v>0.73048421999999924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.84270061999999868</c:v>
+                  <c:v>0.84198493999999968</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.89407403000000052</c:v>
+                  <c:v>0.84118643999999954</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2282,16 +2295,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11.908789844999999</c:v>
+                  <c:v>11.7544605</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.511600475</c:v>
+                  <c:v>10.38771596</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.576088309999999</c:v>
+                  <c:v>11.489311234999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.736576370000002</c:v>
+                  <c:v>10.57791746</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2325,16 +2338,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11.857586510000001</c:v>
+                  <c:v>11.691313415</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.58447911</c:v>
+                  <c:v>10.463576085</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.346393774999999</c:v>
+                  <c:v>11.216629624999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.080272190000001</c:v>
+                  <c:v>10.936670769999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2368,16 +2381,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>13.027399920000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>11.0059532</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>11.734510090000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>10.807169289999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2410,18 +2423,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>11.879999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12.395</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.469999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.445</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2454,16 +2455,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11.831386155000001</c:v>
+                  <c:v>11.645599149999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.549725084999999</c:v>
+                  <c:v>10.441008180000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.471758205</c:v>
+                  <c:v>11.271648604999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.167520115</c:v>
+                  <c:v>10.98816105</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2497,16 +2498,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11.724543785</c:v>
+                  <c:v>11.593726929999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.38107684</c:v>
+                  <c:v>10.294050915</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.864205569999999</c:v>
+                  <c:v>10.740147685</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.53917869</c:v>
+                  <c:v>10.401058115000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2542,16 +2543,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>12.812353359999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>10.588295240000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>11.42584708</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>10.923264469999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2586,18 +2587,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>11.32</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.46</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.955</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.914999999999999</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4381,12 +4370,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="D1" s="77"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
@@ -12880,8 +12869,8 @@
   </sheetPr>
   <dimension ref="A1:AA99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I70" sqref="I70"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -12906,12 +12895,12 @@
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
-      <c r="G3" s="79" t="s">
+      <c r="G3" s="81" t="s">
         <v>170</v>
       </c>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
       <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" customHeight="1">
@@ -14921,475 +14910,459 @@
       </c>
     </row>
     <row r="68" spans="1:22" ht="15.75" customHeight="1">
-      <c r="D68" s="82" t="s">
-        <v>389</v>
-      </c>
-      <c r="N68" s="82" t="s">
-        <v>389</v>
-      </c>
-      <c r="S68" s="82" t="s">
-        <v>389</v>
-      </c>
+      <c r="D68" s="77"/>
+      <c r="N68" s="77"/>
+      <c r="S68" s="77"/>
     </row>
     <row r="69" spans="1:22" ht="15.75" customHeight="1">
-      <c r="D69" s="74">
-        <v>1.7843621039999999</v>
-      </c>
-      <c r="E69" s="74">
-        <v>13.12447721</v>
-      </c>
-      <c r="F69" s="74">
-        <v>12.913345469999999</v>
-      </c>
-      <c r="N69" s="74">
-        <v>1.964192763</v>
-      </c>
-      <c r="O69" s="74">
-        <v>11.914036019999999</v>
-      </c>
-      <c r="P69" s="74">
-        <v>11.509005480000001</v>
-      </c>
-      <c r="S69" s="73">
-        <v>1.8694403660000001</v>
-      </c>
-      <c r="T69" s="73">
-        <v>10.98796596</v>
-      </c>
-      <c r="U69" s="73">
-        <v>11.078948069999999</v>
-      </c>
+      <c r="D69" s="74"/>
+      <c r="E69" s="74"/>
+      <c r="F69" s="74"/>
+      <c r="N69" s="74"/>
+      <c r="O69" s="74"/>
+      <c r="P69" s="74"/>
+      <c r="S69" s="73"/>
+      <c r="T69" s="73"/>
+      <c r="U69" s="73"/>
     </row>
     <row r="70" spans="1:22" ht="15.75" customHeight="1">
-      <c r="I70" s="82" t="s">
-        <v>390</v>
-      </c>
-      <c r="N70" s="82" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="71" spans="1:22" ht="15.75" customHeight="1">
-      <c r="B71" s="81" t="s">
+      <c r="I70" s="77"/>
+      <c r="N70" s="77"/>
+    </row>
+    <row r="71" spans="1:22" s="83" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B71" s="83" t="s">
         <v>388</v>
       </c>
-      <c r="I71" s="74">
-        <v>1.6121465399999999</v>
-      </c>
-      <c r="J71" s="74">
-        <v>11.00523155</v>
-      </c>
-      <c r="K71" s="74">
-        <v>10.60252912</v>
-      </c>
-      <c r="N71" s="73">
-        <v>1.8957573720000001</v>
-      </c>
-      <c r="O71" s="73">
-        <v>11.737313759999999</v>
-      </c>
-      <c r="P71" s="73">
-        <v>11.41887084</v>
-      </c>
-    </row>
-    <row r="72" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A72" s="73"/>
-      <c r="B72" s="73"/>
-      <c r="C72" s="73"/>
-      <c r="D72" s="73" t="s">
+      <c r="I71" s="84"/>
+      <c r="J71" s="84"/>
+      <c r="K71" s="84"/>
+      <c r="N71" s="84"/>
+      <c r="O71" s="84"/>
+      <c r="P71" s="84"/>
+    </row>
+    <row r="72" spans="1:22" s="83" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A72" s="84"/>
+      <c r="B72" s="84"/>
+      <c r="C72" s="84"/>
+      <c r="D72" s="84" t="s">
         <v>192</v>
       </c>
-      <c r="E72" s="73" t="s">
+      <c r="E72" s="84" t="s">
         <v>193</v>
       </c>
-      <c r="F72" s="73"/>
-      <c r="G72" s="73"/>
-      <c r="H72" s="73"/>
-      <c r="I72" s="73" t="s">
+      <c r="F72" s="84"/>
+      <c r="G72" s="84"/>
+      <c r="H72" s="84"/>
+      <c r="I72" s="84" t="s">
         <v>192</v>
       </c>
-      <c r="J72" s="73" t="s">
+      <c r="J72" s="84" t="s">
         <v>193</v>
       </c>
-      <c r="K72" s="73"/>
-      <c r="L72" s="73"/>
-      <c r="M72" s="73"/>
-      <c r="N72" s="73" t="s">
+      <c r="K72" s="84"/>
+      <c r="L72" s="84"/>
+      <c r="M72" s="84"/>
+      <c r="N72" s="84" t="s">
         <v>192</v>
       </c>
-      <c r="O72" s="73" t="s">
+      <c r="O72" s="84" t="s">
         <v>193</v>
       </c>
-      <c r="P72" s="73"/>
-      <c r="Q72" s="73"/>
-      <c r="R72" s="73"/>
-      <c r="S72" s="73" t="s">
+      <c r="P72" s="84"/>
+      <c r="Q72" s="84"/>
+      <c r="R72" s="84"/>
+      <c r="S72" s="84" t="s">
         <v>192</v>
       </c>
-      <c r="T72" s="73" t="s">
+      <c r="T72" s="84" t="s">
         <v>193</v>
       </c>
-      <c r="U72" s="73"/>
-      <c r="V72" s="73"/>
-    </row>
-    <row r="73" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A73" s="73"/>
-      <c r="B73" s="73" t="s">
+      <c r="U72" s="84"/>
+      <c r="V72" s="84"/>
+    </row>
+    <row r="73" spans="1:22" s="83" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A73" s="84"/>
+      <c r="B73" s="84" t="s">
         <v>196</v>
       </c>
-      <c r="C73" s="73" t="s">
+      <c r="C73" s="84" t="s">
         <v>197</v>
       </c>
-      <c r="D73" s="73" t="s">
+      <c r="D73" s="84" t="s">
         <v>198</v>
       </c>
-      <c r="E73" s="73" t="s">
+      <c r="E73" s="84" t="s">
         <v>199</v>
       </c>
-      <c r="F73" s="73" t="s">
+      <c r="F73" s="84" t="s">
         <v>200</v>
       </c>
-      <c r="G73" s="73" t="s">
+      <c r="G73" s="84" t="s">
         <v>196</v>
       </c>
-      <c r="H73" s="73" t="s">
+      <c r="H73" s="84" t="s">
         <v>197</v>
       </c>
-      <c r="I73" s="73" t="s">
+      <c r="I73" s="84" t="s">
         <v>198</v>
       </c>
-      <c r="J73" s="73" t="s">
+      <c r="J73" s="84" t="s">
         <v>199</v>
       </c>
-      <c r="K73" s="73" t="s">
+      <c r="K73" s="84" t="s">
         <v>200</v>
       </c>
-      <c r="L73" s="73" t="s">
+      <c r="L73" s="84" t="s">
         <v>196</v>
       </c>
-      <c r="M73" s="73" t="s">
+      <c r="M73" s="84" t="s">
         <v>197</v>
       </c>
-      <c r="N73" s="73" t="s">
+      <c r="N73" s="84" t="s">
         <v>198</v>
       </c>
-      <c r="O73" s="73" t="s">
+      <c r="O73" s="84" t="s">
         <v>199</v>
       </c>
-      <c r="P73" s="73" t="s">
+      <c r="P73" s="84" t="s">
         <v>200</v>
       </c>
-      <c r="Q73" s="73" t="s">
+      <c r="Q73" s="84" t="s">
         <v>196</v>
       </c>
-      <c r="R73" s="73" t="s">
+      <c r="R73" s="84" t="s">
         <v>197</v>
       </c>
-      <c r="S73" s="73" t="s">
+      <c r="S73" s="84" t="s">
         <v>198</v>
       </c>
-      <c r="T73" s="73" t="s">
+      <c r="T73" s="84" t="s">
         <v>199</v>
       </c>
-      <c r="U73" s="73" t="s">
+      <c r="U73" s="84" t="s">
         <v>200</v>
       </c>
-      <c r="V73" s="73"/>
-    </row>
-    <row r="74" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A74" s="73"/>
-      <c r="B74" s="73">
+      <c r="V73" s="84"/>
+    </row>
+    <row r="74" spans="1:22" s="83" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A74" s="84"/>
+      <c r="B74" s="84">
         <v>1</v>
       </c>
-      <c r="C74" s="73">
+      <c r="C74" s="84">
         <v>3</v>
       </c>
-      <c r="D74" s="74"/>
-      <c r="E74" s="74"/>
-      <c r="F74" s="74"/>
-      <c r="G74" s="73">
+      <c r="D74" s="83">
+        <v>1.751345334</v>
+      </c>
+      <c r="E74" s="83">
+        <v>13.027399920000001</v>
+      </c>
+      <c r="F74" s="83">
+        <v>12.812353359999999</v>
+      </c>
+      <c r="G74" s="84">
         <v>2</v>
       </c>
-      <c r="H74" s="73">
+      <c r="H74" s="84">
         <v>3</v>
       </c>
-      <c r="I74" s="74"/>
-      <c r="J74" s="74"/>
-      <c r="K74" s="74"/>
-      <c r="L74" s="73">
+      <c r="I74" s="83">
+        <v>1.6153839210000001</v>
+      </c>
+      <c r="J74" s="83">
+        <v>11.0059532</v>
+      </c>
+      <c r="K74" s="83">
+        <v>10.588295240000001</v>
+      </c>
+      <c r="L74" s="84">
         <v>3</v>
       </c>
-      <c r="M74" s="73">
+      <c r="M74" s="84">
         <v>3</v>
       </c>
-      <c r="N74" s="74"/>
-      <c r="O74" s="74"/>
-      <c r="P74" s="74"/>
-      <c r="Q74" s="73">
+      <c r="N74" s="83">
+        <v>1.9051938390000001</v>
+      </c>
+      <c r="O74" s="83">
+        <v>11.734510090000001</v>
+      </c>
+      <c r="P74" s="83">
+        <v>11.42584708</v>
+      </c>
+      <c r="Q74" s="84">
         <v>4</v>
       </c>
-      <c r="R74" s="73">
+      <c r="R74" s="84">
         <v>3</v>
       </c>
-      <c r="S74" s="73"/>
-      <c r="T74" s="73"/>
-      <c r="U74" s="73"/>
-      <c r="V74" s="73"/>
-    </row>
-    <row r="75" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A75" s="73"/>
-      <c r="B75" s="73">
+      <c r="S74" s="83">
+        <v>1.797774521</v>
+      </c>
+      <c r="T74" s="83">
+        <v>10.807169289999999</v>
+      </c>
+      <c r="U74" s="83">
+        <v>10.923264469999999</v>
+      </c>
+      <c r="V74" s="84"/>
+    </row>
+    <row r="75" spans="1:22" s="83" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A75" s="84"/>
+      <c r="B75" s="84">
         <v>1</v>
       </c>
-      <c r="C75" s="73">
+      <c r="C75" s="84">
         <v>2</v>
       </c>
-      <c r="D75" s="76">
-        <v>1.9533226530000001</v>
-      </c>
-      <c r="E75" s="76">
-        <v>11.698063429999999</v>
-      </c>
-      <c r="F75" s="76">
-        <v>11.91752514</v>
-      </c>
-      <c r="G75" s="73">
+      <c r="D75" s="83">
+        <v>1.8857474729999999</v>
+      </c>
+      <c r="E75" s="83">
+        <v>11.88952067</v>
+      </c>
+      <c r="F75" s="83">
+        <v>11.374466200000001</v>
+      </c>
+      <c r="G75" s="84">
         <v>2</v>
       </c>
-      <c r="H75" s="73">
+      <c r="H75" s="84">
         <v>2</v>
       </c>
-      <c r="I75" s="76">
-        <v>1.6356537799999999</v>
-      </c>
-      <c r="J75" s="76">
-        <v>10.54304964</v>
-      </c>
-      <c r="K75" s="76">
-        <v>10.4326998</v>
-      </c>
-      <c r="L75" s="73">
+      <c r="I75" s="83">
+        <v>1.582638532</v>
+      </c>
+      <c r="J75" s="83">
+        <v>10.466353270000001</v>
+      </c>
+      <c r="K75" s="83">
+        <v>10.248913780000001</v>
+      </c>
+      <c r="L75" s="84">
         <v>3</v>
       </c>
-      <c r="M75" s="73">
+      <c r="M75" s="84">
         <v>2</v>
       </c>
-      <c r="N75" s="76">
-        <v>1.8451964569999999</v>
-      </c>
-      <c r="O75" s="76">
-        <v>11.37779744</v>
-      </c>
-      <c r="P75" s="76">
-        <v>11.05976031</v>
-      </c>
-      <c r="Q75" s="73">
+      <c r="N75" s="83">
+        <v>1.791405567</v>
+      </c>
+      <c r="O75" s="83">
+        <v>11.1419382</v>
+      </c>
+      <c r="P75" s="83">
+        <v>10.583862140000001</v>
+      </c>
+      <c r="Q75" s="84">
         <v>4</v>
       </c>
-      <c r="R75" s="73">
+      <c r="R75" s="84">
         <v>2</v>
       </c>
-      <c r="S75" s="76">
-        <v>1.698257736</v>
-      </c>
-      <c r="T75" s="76">
-        <v>10.901165600000001</v>
-      </c>
-      <c r="U75" s="76">
-        <v>10.59103932</v>
-      </c>
-      <c r="V75" s="73"/>
-    </row>
-    <row r="76" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A76" s="73"/>
-      <c r="B76" s="73">
+      <c r="S75" s="83">
+        <v>1.6692033900000001</v>
+      </c>
+      <c r="T75" s="83">
+        <v>11.08524332</v>
+      </c>
+      <c r="U75" s="83">
+        <v>10.360162170000001</v>
+      </c>
+      <c r="V75" s="84"/>
+    </row>
+    <row r="76" spans="1:22" s="83" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A76" s="84"/>
+      <c r="B76" s="84">
         <v>1</v>
       </c>
-      <c r="C76" s="73">
+      <c r="C76" s="84">
         <v>2</v>
       </c>
-      <c r="D76" s="76">
-        <v>1.9533226530000001</v>
-      </c>
-      <c r="E76" s="76">
-        <v>12.01710959</v>
-      </c>
-      <c r="F76" s="76">
-        <v>11.531562429999999</v>
-      </c>
-      <c r="G76" s="73">
+      <c r="D76" s="83">
+        <v>1.8857474729999999</v>
+      </c>
+      <c r="E76" s="83">
+        <v>11.49310616</v>
+      </c>
+      <c r="F76" s="83">
+        <v>11.812987659999999</v>
+      </c>
+      <c r="G76" s="84">
         <v>2</v>
       </c>
-      <c r="H76" s="73">
+      <c r="H76" s="84">
         <v>2</v>
       </c>
-      <c r="I76" s="76">
-        <v>1.6356537799999999</v>
-      </c>
-      <c r="J76" s="76">
-        <v>10.625908580000001</v>
-      </c>
-      <c r="K76" s="76">
-        <v>10.329453880000001</v>
-      </c>
-      <c r="L76" s="73">
+      <c r="I76" s="83">
+        <v>1.582638532</v>
+      </c>
+      <c r="J76" s="83">
+        <v>10.4607989</v>
+      </c>
+      <c r="K76" s="83">
+        <v>10.339188050000001</v>
+      </c>
+      <c r="L76" s="84">
         <v>3</v>
       </c>
-      <c r="M76" s="73">
+      <c r="M76" s="84">
         <v>2</v>
       </c>
-      <c r="N76" s="76">
-        <v>1.8451964569999999</v>
-      </c>
-      <c r="O76" s="76">
-        <v>11.31499011</v>
-      </c>
-      <c r="P76" s="76">
-        <v>10.668650830000001</v>
-      </c>
-      <c r="Q76" s="73">
+      <c r="N76" s="83">
+        <v>1.791405567</v>
+      </c>
+      <c r="O76" s="83">
+        <v>11.291321050000001</v>
+      </c>
+      <c r="P76" s="83">
+        <v>10.89643323</v>
+      </c>
+      <c r="Q76" s="84">
         <v>4</v>
       </c>
-      <c r="R76" s="73">
+      <c r="R76" s="84">
         <v>2</v>
       </c>
-      <c r="S76" s="76">
-        <v>1.698257736</v>
-      </c>
-      <c r="T76" s="76">
-        <v>11.25937878</v>
-      </c>
-      <c r="U76" s="76">
-        <v>10.48731806</v>
-      </c>
-      <c r="V76" s="73"/>
-    </row>
-    <row r="77" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A77" s="73"/>
-      <c r="B77" s="73">
+      <c r="S76" s="83">
+        <v>1.6692033900000001</v>
+      </c>
+      <c r="T76" s="83">
+        <v>10.78809822</v>
+      </c>
+      <c r="U76" s="83">
+        <v>10.44195406</v>
+      </c>
+      <c r="V76" s="84"/>
+    </row>
+    <row r="77" spans="1:22" s="83" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A77" s="84"/>
+      <c r="B77" s="84">
         <v>1</v>
       </c>
-      <c r="C77" s="73">
+      <c r="C77" s="84">
         <v>1</v>
       </c>
-      <c r="D77" s="76">
-        <v>1.8314126049999999</v>
-      </c>
-      <c r="E77" s="76">
-        <v>11.832379469999999</v>
-      </c>
-      <c r="F77" s="76">
-        <v>11.70265908</v>
-      </c>
-      <c r="G77" s="73">
+      <c r="D77" s="83">
+        <v>1.711534415</v>
+      </c>
+      <c r="E77" s="83">
+        <v>11.77550426</v>
+      </c>
+      <c r="F77" s="83">
+        <v>11.760609199999999</v>
+      </c>
+      <c r="G77" s="84">
         <v>2</v>
       </c>
-      <c r="H77" s="73">
+      <c r="H77" s="84">
         <v>1</v>
       </c>
-      <c r="I77" s="76">
-        <v>1.577234099</v>
-      </c>
-      <c r="J77" s="76">
-        <v>10.75850441</v>
-      </c>
-      <c r="K77" s="76">
-        <v>10.937471029999999</v>
-      </c>
-      <c r="L77" s="73">
+      <c r="I77" s="83">
+        <v>1.5142305439999999</v>
+      </c>
+      <c r="J77" s="85">
+        <v>10.104439449999999</v>
+      </c>
+      <c r="K77" s="85">
+        <v>10.07576607</v>
+      </c>
+      <c r="L77" s="84">
         <v>3</v>
       </c>
-      <c r="M77" s="73">
+      <c r="M77" s="84">
         <v>1</v>
       </c>
-      <c r="N77" s="76">
-        <v>1.6330105290000001</v>
-      </c>
-      <c r="O77" s="76">
-        <v>11.814252460000001</v>
-      </c>
-      <c r="P77" s="76">
-        <v>11.43216496</v>
-      </c>
-      <c r="Q77" s="73">
+      <c r="N77" s="83">
+        <v>1.578711121</v>
+      </c>
+      <c r="O77" s="83">
+        <v>11.25170795</v>
+      </c>
+      <c r="P77" s="83">
+        <v>11.321315609999999</v>
+      </c>
+      <c r="Q77" s="84">
         <v>4</v>
       </c>
-      <c r="R77" s="73">
+      <c r="R77" s="84">
         <v>1</v>
       </c>
-      <c r="S77" s="76">
-        <v>1.887225025</v>
-      </c>
-      <c r="T77" s="76">
-        <v>10.823476680000001</v>
-      </c>
-      <c r="U77" s="76">
-        <v>11.38139209</v>
-      </c>
-      <c r="V77" s="73"/>
-    </row>
-    <row r="78" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A78" s="73"/>
-      <c r="B78" s="73">
+      <c r="S77" s="83">
+        <v>1.7902534109999999</v>
+      </c>
+      <c r="T77" s="83">
+        <v>10.4876483</v>
+      </c>
+      <c r="U77" s="83">
+        <v>10.774973490000001</v>
+      </c>
+      <c r="V77" s="84"/>
+    </row>
+    <row r="78" spans="1:22" s="83" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A78" s="84"/>
+      <c r="B78" s="84">
         <v>1</v>
       </c>
-      <c r="C78" s="73">
+      <c r="C78" s="84">
         <v>1</v>
       </c>
-      <c r="D78" s="76">
-        <v>1.8314126049999999</v>
-      </c>
-      <c r="E78" s="76">
-        <v>11.985200219999999</v>
-      </c>
-      <c r="F78" s="76">
-        <v>11.960113229999999</v>
-      </c>
-      <c r="G78" s="73">
+      <c r="D78" s="83">
+        <v>1.711534415</v>
+      </c>
+      <c r="E78" s="83">
+        <v>11.733416739999999</v>
+      </c>
+      <c r="F78" s="83">
+        <v>11.5305891</v>
+      </c>
+      <c r="G78" s="84">
         <v>2</v>
       </c>
-      <c r="H78" s="73">
+      <c r="H78" s="84">
         <v>1</v>
       </c>
-      <c r="I78" s="76">
-        <v>1.577234099</v>
-      </c>
-      <c r="J78" s="76">
-        <v>10.264696539999999</v>
-      </c>
-      <c r="K78" s="76">
-        <v>10.16197914</v>
-      </c>
-      <c r="L78" s="73">
+      <c r="I78" s="83">
+        <v>1.5142305439999999</v>
+      </c>
+      <c r="J78" s="85">
+        <v>10.67099247</v>
+      </c>
+      <c r="K78" s="85">
+        <v>10.806250289999999</v>
+      </c>
+      <c r="L78" s="84">
         <v>3</v>
       </c>
-      <c r="M78" s="73">
+      <c r="M78" s="84">
         <v>1</v>
       </c>
-      <c r="N78" s="76">
-        <v>1.6330105290000001</v>
-      </c>
-      <c r="O78" s="76">
-        <v>11.33792416</v>
-      </c>
-      <c r="P78" s="76">
-        <v>11.511351449999999</v>
-      </c>
-      <c r="Q78" s="73">
+      <c r="N78" s="83">
+        <v>1.578711121</v>
+      </c>
+      <c r="O78" s="83">
+        <v>11.726914519999999</v>
+      </c>
+      <c r="P78" s="83">
+        <v>11.221981599999999</v>
+      </c>
+      <c r="Q78" s="84">
         <v>4</v>
       </c>
-      <c r="R78" s="73">
+      <c r="R78" s="84">
         <v>1</v>
       </c>
-      <c r="S78" s="76">
-        <v>1.887225025</v>
-      </c>
-      <c r="T78" s="76">
-        <v>10.649676060000001</v>
-      </c>
-      <c r="U78" s="76">
-        <v>10.95364814</v>
-      </c>
-      <c r="V78" s="73"/>
+      <c r="S78" s="83">
+        <v>1.7902534109999999</v>
+      </c>
+      <c r="T78" s="83">
+        <v>10.66818662</v>
+      </c>
+      <c r="U78" s="83">
+        <v>11.20134861</v>
+      </c>
+      <c r="V78" s="84"/>
     </row>
     <row r="79" spans="1:22" ht="15.75" customHeight="1">
       <c r="A79" s="73"/>
@@ -15423,15 +15396,15 @@
       </c>
       <c r="D80" s="73">
         <f>AVERAGE(D74:D78)</f>
-        <v>1.892367629</v>
+        <v>1.7891818220000002</v>
       </c>
       <c r="E80" s="73">
         <f t="shared" ref="E80:F80" si="32">AVERAGE(E74:E78)</f>
-        <v>11.883188177499999</v>
+        <v>11.983789550000001</v>
       </c>
       <c r="F80" s="73">
         <f t="shared" si="32"/>
-        <v>11.777964969999999</v>
+        <v>11.858201103999999</v>
       </c>
       <c r="G80" s="73"/>
       <c r="H80" s="73" t="s">
@@ -15439,15 +15412,15 @@
       </c>
       <c r="I80" s="73">
         <f>AVERAGE(I74:I78)</f>
-        <v>1.6064439395000001</v>
+        <v>1.5618244146</v>
       </c>
       <c r="J80" s="73">
         <f t="shared" ref="J80:K80" si="33">AVERAGE(J74:J78)</f>
-        <v>10.548039792499999</v>
+        <v>10.541707458000001</v>
       </c>
       <c r="K80" s="73">
         <f t="shared" si="33"/>
-        <v>10.4654009625</v>
+        <v>10.411682686000002</v>
       </c>
       <c r="L80" s="73"/>
       <c r="M80" s="73" t="s">
@@ -15455,15 +15428,15 @@
       </c>
       <c r="N80" s="73">
         <f>AVERAGE(N74:N78)</f>
-        <v>1.739103493</v>
+        <v>1.729085443</v>
       </c>
       <c r="O80" s="73">
         <f t="shared" ref="O80:P80" si="34">AVERAGE(O74:O78)</f>
-        <v>11.461241042499999</v>
+        <v>11.429278362000002</v>
       </c>
       <c r="P80" s="73">
         <f t="shared" si="34"/>
-        <v>11.1679818875</v>
+        <v>11.089887932</v>
       </c>
       <c r="Q80" s="73"/>
       <c r="R80" s="73" t="s">
@@ -15471,15 +15444,15 @@
       </c>
       <c r="S80" s="73">
         <f>AVERAGE(S74:S78)</f>
-        <v>1.7927413805000001</v>
+        <v>1.7433376245999999</v>
       </c>
       <c r="T80" s="73">
         <f t="shared" ref="T80:U80" si="35">AVERAGE(T74:T78)</f>
-        <v>10.908424280000002</v>
+        <v>10.767269150000001</v>
       </c>
       <c r="U80" s="73">
         <f t="shared" si="35"/>
-        <v>10.853349402499999</v>
+        <v>10.740340560000002</v>
       </c>
       <c r="V80" s="73"/>
     </row>
@@ -15491,15 +15464,15 @@
       </c>
       <c r="D81" s="73">
         <f>MIN(D74:D78)</f>
-        <v>1.8314126049999999</v>
+        <v>1.711534415</v>
       </c>
       <c r="E81" s="73">
         <f t="shared" ref="E81:F81" si="36">MIN(E74:E78)</f>
-        <v>11.698063429999999</v>
+        <v>11.49310616</v>
       </c>
       <c r="F81" s="73">
         <f t="shared" si="36"/>
-        <v>11.531562429999999</v>
+        <v>11.374466200000001</v>
       </c>
       <c r="G81" s="73"/>
       <c r="H81" s="73" t="s">
@@ -15507,15 +15480,15 @@
       </c>
       <c r="I81" s="73">
         <f>MIN(I74:I78)</f>
-        <v>1.577234099</v>
+        <v>1.5142305439999999</v>
       </c>
       <c r="J81" s="73">
         <f t="shared" ref="J81:K81" si="37">MIN(J74:J78)</f>
-        <v>10.264696539999999</v>
+        <v>10.104439449999999</v>
       </c>
       <c r="K81" s="73">
         <f t="shared" si="37"/>
-        <v>10.16197914</v>
+        <v>10.07576607</v>
       </c>
       <c r="L81" s="73"/>
       <c r="M81" s="73" t="s">
@@ -15523,15 +15496,15 @@
       </c>
       <c r="N81" s="73">
         <f>MIN(N74:N78)</f>
-        <v>1.6330105290000001</v>
+        <v>1.578711121</v>
       </c>
       <c r="O81" s="73">
         <f t="shared" ref="O81:P81" si="38">MIN(O74:O78)</f>
-        <v>11.31499011</v>
+        <v>11.1419382</v>
       </c>
       <c r="P81" s="73">
         <f t="shared" si="38"/>
-        <v>10.668650830000001</v>
+        <v>10.583862140000001</v>
       </c>
       <c r="Q81" s="73"/>
       <c r="R81" s="73" t="s">
@@ -15539,15 +15512,15 @@
       </c>
       <c r="S81" s="73">
         <f>MIN(S74:S78)</f>
-        <v>1.698257736</v>
+        <v>1.6692033900000001</v>
       </c>
       <c r="T81" s="73">
         <f t="shared" ref="T81:U81" si="39">MIN(T74:T78)</f>
-        <v>10.649676060000001</v>
+        <v>10.4876483</v>
       </c>
       <c r="U81" s="73">
         <f t="shared" si="39"/>
-        <v>10.48731806</v>
+        <v>10.360162170000001</v>
       </c>
       <c r="V81" s="73"/>
     </row>
@@ -15559,15 +15532,15 @@
       </c>
       <c r="D82" s="73">
         <f>MAX(D74:D78)</f>
-        <v>1.9533226530000001</v>
+        <v>1.8857474729999999</v>
       </c>
       <c r="E82" s="73">
         <f t="shared" ref="E82:F82" si="40">MAX(E74:E78)</f>
-        <v>12.01710959</v>
+        <v>13.027399920000001</v>
       </c>
       <c r="F82" s="73">
         <f t="shared" si="40"/>
-        <v>11.960113229999999</v>
+        <v>12.812353359999999</v>
       </c>
       <c r="G82" s="73"/>
       <c r="H82" s="73" t="s">
@@ -15575,15 +15548,15 @@
       </c>
       <c r="I82" s="73">
         <f>MAX(I74:I78)</f>
-        <v>1.6356537799999999</v>
+        <v>1.6153839210000001</v>
       </c>
       <c r="J82" s="73">
         <f t="shared" ref="J82:K82" si="41">MAX(J74:J78)</f>
-        <v>10.75850441</v>
+        <v>11.0059532</v>
       </c>
       <c r="K82" s="73">
         <f t="shared" si="41"/>
-        <v>10.937471029999999</v>
+        <v>10.806250289999999</v>
       </c>
       <c r="L82" s="73"/>
       <c r="M82" s="73" t="s">
@@ -15591,15 +15564,15 @@
       </c>
       <c r="N82" s="73">
         <f>MAX(N74:N78)</f>
-        <v>1.8451964569999999</v>
+        <v>1.9051938390000001</v>
       </c>
       <c r="O82" s="73">
         <f t="shared" ref="O82:P82" si="42">MAX(O74:O78)</f>
-        <v>11.814252460000001</v>
+        <v>11.734510090000001</v>
       </c>
       <c r="P82" s="73">
         <f t="shared" si="42"/>
-        <v>11.511351449999999</v>
+        <v>11.42584708</v>
       </c>
       <c r="Q82" s="73"/>
       <c r="R82" s="73" t="s">
@@ -15607,15 +15580,15 @@
       </c>
       <c r="S82" s="73">
         <f>MAX(S74:S78)</f>
-        <v>1.887225025</v>
+        <v>1.797774521</v>
       </c>
       <c r="T82" s="73">
         <f t="shared" ref="T82:U82" si="43">MAX(T74:T78)</f>
-        <v>11.25937878</v>
+        <v>11.08524332</v>
       </c>
       <c r="U82" s="73">
         <f t="shared" si="43"/>
-        <v>11.38139209</v>
+        <v>11.20134861</v>
       </c>
       <c r="V82" s="73"/>
     </row>
@@ -15627,15 +15600,15 @@
       </c>
       <c r="D83" s="73">
         <f>D82-D81</f>
-        <v>0.12191004800000016</v>
+        <v>0.17421305799999987</v>
       </c>
       <c r="E83" s="73">
         <f t="shared" ref="E83" si="44">E82-E81</f>
-        <v>0.31904616000000097</v>
+        <v>1.5342937600000006</v>
       </c>
       <c r="F83" s="73">
         <f t="shared" ref="F83" si="45">F82-F81</f>
-        <v>0.42855080000000001</v>
+        <v>1.4378871599999989</v>
       </c>
       <c r="G83" s="73"/>
       <c r="H83" s="73" t="s">
@@ -15643,15 +15616,15 @@
       </c>
       <c r="I83" s="73">
         <f>I82-I81</f>
-        <v>5.8419680999999946E-2</v>
+        <v>0.10115337700000016</v>
       </c>
       <c r="J83" s="73">
         <f t="shared" ref="J83" si="46">J82-J81</f>
-        <v>0.49380787000000126</v>
+        <v>0.90151375000000122</v>
       </c>
       <c r="K83" s="73">
         <f t="shared" ref="K83" si="47">K82-K81</f>
-        <v>0.77549188999999963</v>
+        <v>0.73048421999999924</v>
       </c>
       <c r="L83" s="73"/>
       <c r="M83" s="73" t="s">
@@ -15659,15 +15632,15 @@
       </c>
       <c r="N83" s="73">
         <f>N82-N81</f>
-        <v>0.2121859279999998</v>
+        <v>0.32648271800000006</v>
       </c>
       <c r="O83" s="73">
         <f t="shared" ref="O83" si="48">O82-O81</f>
-        <v>0.49926235000000041</v>
+        <v>0.59257189000000032</v>
       </c>
       <c r="P83" s="73">
         <f t="shared" ref="P83" si="49">P82-P81</f>
-        <v>0.84270061999999868</v>
+        <v>0.84198493999999968</v>
       </c>
       <c r="Q83" s="73"/>
       <c r="R83" s="73" t="s">
@@ -15675,15 +15648,15 @@
       </c>
       <c r="S83" s="73">
         <f>S82-S81</f>
-        <v>0.18896728900000004</v>
+        <v>0.12857113099999995</v>
       </c>
       <c r="T83" s="73">
         <f t="shared" ref="T83:U83" si="50">T82-T81</f>
-        <v>0.60970271999999959</v>
+        <v>0.59759501999999998</v>
       </c>
       <c r="U83" s="73">
         <f t="shared" si="50"/>
-        <v>0.89407403000000052</v>
+        <v>0.84118643999999954</v>
       </c>
       <c r="V83" s="73"/>
     </row>
@@ -15695,15 +15668,15 @@
       </c>
       <c r="D84" s="73">
         <f>_xlfn.STDEV.P(D74:D78)</f>
-        <v>6.095502400000008E-2</v>
+        <v>8.01744215544197E-2</v>
       </c>
       <c r="E84" s="73">
         <f t="shared" ref="E84:U84" si="51">_xlfn.STDEV.P(E74:E78)</f>
-        <v>0.12766567513996913</v>
+        <v>0.53755906119189645</v>
       </c>
       <c r="F84" s="73">
         <f t="shared" si="51"/>
-        <v>0.17251102751606953</v>
+        <v>0.50265376660030303</v>
       </c>
       <c r="G84" s="73">
         <f t="shared" si="51"/>
@@ -15715,15 +15688,15 @@
       </c>
       <c r="I84" s="73">
         <f t="shared" si="51"/>
-        <v>2.9209840499999973E-2</v>
+        <v>4.0658157187636344E-2</v>
       </c>
       <c r="J84" s="73">
         <f t="shared" si="51"/>
-        <v>0.18073959419935789</v>
+        <v>0.29518349632729751</v>
       </c>
       <c r="K84" s="73">
         <f t="shared" si="51"/>
-        <v>0.28916514583702363</v>
+        <v>0.25747417356729352</v>
       </c>
       <c r="L84" s="73">
         <f t="shared" si="51"/>
@@ -15735,15 +15708,15 @@
       </c>
       <c r="N84" s="73">
         <f t="shared" si="51"/>
-        <v>0.1060929639999999</v>
+        <v>0.12961993387312226</v>
       </c>
       <c r="O84" s="73">
         <f t="shared" si="51"/>
-        <v>0.2050465096326782</v>
+        <v>0.25095080401431985</v>
       </c>
       <c r="P84" s="73">
         <f t="shared" si="51"/>
-        <v>0.33493983305499708</v>
+        <v>0.3089863687252844</v>
       </c>
       <c r="Q84" s="73">
         <f t="shared" si="51"/>
@@ -15755,15 +15728,15 @@
       </c>
       <c r="S84" s="73">
         <f t="shared" si="51"/>
-        <v>9.4483644500000019E-2</v>
+        <v>6.0592618686075655E-2</v>
       </c>
       <c r="T84" s="73">
         <f t="shared" si="51"/>
-        <v>0.22214211982676796</v>
+        <v>0.19551910987021023</v>
       </c>
       <c r="U84" s="73">
         <f t="shared" si="51"/>
-        <v>0.35059750414108276</v>
+        <v>0.31008357920409679</v>
       </c>
     </row>
     <row r="85" spans="1:27" ht="15.75" customHeight="1" thickBot="1">
@@ -15831,13 +15804,16 @@
         <v>1</v>
       </c>
       <c r="C87" s="73">
-        <v>0.16896054900000013</v>
+        <f>D83</f>
+        <v>0.17421305799999987</v>
       </c>
       <c r="D87" s="73">
-        <v>1.4264137800000007</v>
+        <f t="shared" ref="D87:E87" si="52">E83</f>
+        <v>1.5342937600000006</v>
       </c>
       <c r="E87" s="73">
-        <v>1.3817830400000002</v>
+        <f t="shared" si="52"/>
+        <v>1.4378871599999989</v>
       </c>
       <c r="F87" s="73"/>
       <c r="G87" s="73"/>
@@ -15867,13 +15843,16 @@
         <v>2</v>
       </c>
       <c r="C88" s="70">
-        <v>5.8419680999999946E-2</v>
-      </c>
-      <c r="D88">
-        <v>0.74053501000000033</v>
-      </c>
-      <c r="E88">
-        <v>0.77549188999999963</v>
+        <f>I83</f>
+        <v>0.10115337700000016</v>
+      </c>
+      <c r="D88" s="78">
+        <f t="shared" ref="D88:E88" si="53">J83</f>
+        <v>0.90151375000000122</v>
+      </c>
+      <c r="E88" s="78">
+        <f t="shared" si="53"/>
+        <v>0.73048421999999924</v>
       </c>
       <c r="H88" s="73"/>
       <c r="I88" s="73"/>
@@ -15895,13 +15874,16 @@
         <v>3</v>
       </c>
       <c r="C89">
-        <v>0.26274684299999995</v>
-      </c>
-      <c r="D89">
-        <v>0.49926235000000041</v>
-      </c>
-      <c r="E89">
-        <v>0.84270061999999868</v>
+        <f>N83</f>
+        <v>0.32648271800000006</v>
+      </c>
+      <c r="D89" s="78">
+        <f t="shared" ref="D89:E89" si="54">O83</f>
+        <v>0.59257189000000032</v>
+      </c>
+      <c r="E89" s="78">
+        <f t="shared" si="54"/>
+        <v>0.84198493999999968</v>
       </c>
       <c r="G89" s="73"/>
       <c r="H89" s="73"/>
@@ -15923,13 +15905,16 @@
         <v>4</v>
       </c>
       <c r="C90">
-        <v>0.18896728900000004</v>
-      </c>
-      <c r="D90">
-        <v>0.60970271999999959</v>
-      </c>
-      <c r="E90">
-        <v>0.89407403000000052</v>
+        <f>S83</f>
+        <v>0.12857113099999995</v>
+      </c>
+      <c r="D90" s="78">
+        <f t="shared" ref="D90:E90" si="55">T83</f>
+        <v>0.59759501999999998</v>
+      </c>
+      <c r="E90" s="78">
+        <f t="shared" si="55"/>
+        <v>0.84118643999999954</v>
       </c>
       <c r="G90" s="73"/>
       <c r="H90" s="73"/>
@@ -15992,36 +15977,30 @@
       </c>
       <c r="L92" s="73">
         <f>AVERAGE(E77:E78)</f>
-        <v>11.908789844999999</v>
+        <v>11.7544605</v>
       </c>
       <c r="M92" s="73">
         <f>AVERAGE(E75:E76)</f>
-        <v>11.857586510000001</v>
+        <v>11.691313415</v>
       </c>
       <c r="N92" s="73">
         <f>E74</f>
-        <v>0</v>
-      </c>
-      <c r="O92" s="73">
-        <f>AVERAGE(11.79,11.97)</f>
-        <v>11.879999999999999</v>
-      </c>
+        <v>13.027399920000001</v>
+      </c>
+      <c r="O92" s="73"/>
       <c r="P92" s="73">
         <f>AVERAGE(F77:F78)</f>
-        <v>11.831386155000001</v>
+        <v>11.645599149999999</v>
       </c>
       <c r="Q92" s="73">
         <f>AVERAGE(F75:F76)</f>
-        <v>11.724543785</v>
+        <v>11.593726929999999</v>
       </c>
       <c r="R92">
         <f>F74</f>
-        <v>0</v>
-      </c>
-      <c r="S92" s="73">
-        <f>AVERAGE(11.05,11.59)</f>
-        <v>11.32</v>
-      </c>
+        <v>12.812353359999999</v>
+      </c>
+      <c r="S92" s="73"/>
       <c r="T92" s="73"/>
     </row>
     <row r="93" spans="1:27" ht="15.75" customHeight="1">
@@ -16034,36 +16013,30 @@
       </c>
       <c r="L93" s="73">
         <f>AVERAGE(J77:J78)</f>
-        <v>10.511600475</v>
+        <v>10.38771596</v>
       </c>
       <c r="M93" s="73">
         <f>AVERAGE(J75:J76)</f>
-        <v>10.58447911</v>
+        <v>10.463576085</v>
       </c>
       <c r="N93" s="73">
         <f>J74</f>
-        <v>0</v>
-      </c>
-      <c r="O93" s="73">
-        <f>AVERAGE(11.91,12.88)</f>
-        <v>12.395</v>
-      </c>
+        <v>11.0059532</v>
+      </c>
+      <c r="O93" s="73"/>
       <c r="P93" s="73">
         <f>AVERAGE(K77:K78)</f>
-        <v>10.549725084999999</v>
+        <v>10.441008180000001</v>
       </c>
       <c r="Q93" s="73">
         <f>AVERAGE(K75:K76)</f>
-        <v>10.38107684</v>
+        <v>10.294050915</v>
       </c>
       <c r="R93" s="73">
         <f>K74</f>
-        <v>0</v>
-      </c>
-      <c r="S93" s="73">
-        <f>AVERAGE(11.51,11.41)</f>
-        <v>11.46</v>
-      </c>
+        <v>10.588295240000001</v>
+      </c>
+      <c r="S93" s="73"/>
       <c r="T93" s="73"/>
     </row>
     <row r="94" spans="1:27" ht="15.75" customHeight="1">
@@ -16076,36 +16049,30 @@
       </c>
       <c r="L94" s="73">
         <f>AVERAGE(O77:O78)</f>
-        <v>11.576088309999999</v>
+        <v>11.489311234999999</v>
       </c>
       <c r="M94" s="73">
         <f>AVERAGE(O75:O76)</f>
-        <v>11.346393774999999</v>
+        <v>11.216629624999999</v>
       </c>
       <c r="N94" s="73">
         <f>O74</f>
-        <v>0</v>
-      </c>
-      <c r="O94" s="73">
-        <f>AVERAGE(11.43,11.51)</f>
-        <v>11.469999999999999</v>
-      </c>
+        <v>11.734510090000001</v>
+      </c>
+      <c r="O94" s="73"/>
       <c r="P94" s="73">
         <f>AVERAGE(P77:P78)</f>
-        <v>11.471758205</v>
+        <v>11.271648604999999</v>
       </c>
       <c r="Q94" s="73">
         <f>AVERAGE(P75:P76)</f>
-        <v>10.864205569999999</v>
+        <v>10.740147685</v>
       </c>
       <c r="R94" s="73">
         <f>P74</f>
-        <v>0</v>
-      </c>
-      <c r="S94" s="73">
-        <f>AVERAGE(10.93,10.98)</f>
-        <v>10.955</v>
-      </c>
+        <v>11.42584708</v>
+      </c>
+      <c r="S94" s="73"/>
       <c r="T94" s="73"/>
     </row>
     <row r="95" spans="1:27" ht="15.75" customHeight="1">
@@ -16118,36 +16085,30 @@
       </c>
       <c r="L95" s="73">
         <f>AVERAGE(T77:T78)</f>
-        <v>10.736576370000002</v>
+        <v>10.57791746</v>
       </c>
       <c r="M95" s="73">
         <f>AVERAGE(T75:T76)</f>
-        <v>11.080272190000001</v>
+        <v>10.936670769999999</v>
       </c>
       <c r="N95" s="73">
         <f>T74</f>
-        <v>0</v>
-      </c>
-      <c r="O95" s="73">
-        <f>AVERAGE(11.63,11.26)</f>
-        <v>11.445</v>
-      </c>
+        <v>10.807169289999999</v>
+      </c>
+      <c r="O95" s="73"/>
       <c r="P95" s="73">
         <f>AVERAGE(U77:U78)</f>
-        <v>11.167520115</v>
+        <v>10.98816105</v>
       </c>
       <c r="Q95" s="73">
         <f>AVERAGE(U75:U76)</f>
-        <v>10.53917869</v>
+        <v>10.401058115000001</v>
       </c>
       <c r="R95" s="73">
         <f>U74</f>
-        <v>0</v>
-      </c>
-      <c r="S95" s="73">
-        <f>AVERAGE(10.93,10.9)</f>
-        <v>10.914999999999999</v>
-      </c>
+        <v>10.923264469999999</v>
+      </c>
+      <c r="S95" s="73"/>
       <c r="T95" s="73"/>
     </row>
     <row r="96" spans="1:27" ht="15.75" customHeight="1">
@@ -16285,36 +16246,36 @@
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="C9" s="77" t="s">
+      <c r="C9" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="78"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="79" t="s">
         <v>225</v>
       </c>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="78"/>
-      <c r="I10" s="80" t="s">
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="82" t="s">
         <v>226</v>
       </c>
-      <c r="J10" s="78"/>
-      <c r="K10" s="78"/>
-      <c r="L10" s="78"/>
-      <c r="M10" s="78"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="80"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="80"/>
       <c r="O10" s="1" t="s">
         <v>227</v>
       </c>
@@ -16990,36 +16951,36 @@
       </c>
     </row>
     <row r="31" spans="1:17">
-      <c r="C31" s="77" t="s">
+      <c r="C31" s="79" t="s">
         <v>230</v>
       </c>
-      <c r="D31" s="78"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="78"/>
-      <c r="I31" s="78"/>
-      <c r="J31" s="78"/>
-      <c r="K31" s="78"/>
-      <c r="L31" s="78"/>
-      <c r="M31" s="78"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="80"/>
+      <c r="I31" s="80"/>
+      <c r="J31" s="80"/>
+      <c r="K31" s="80"/>
+      <c r="L31" s="80"/>
+      <c r="M31" s="80"/>
     </row>
     <row r="32" spans="1:17">
-      <c r="C32" s="77" t="s">
+      <c r="C32" s="79" t="s">
         <v>225</v>
       </c>
-      <c r="D32" s="78"/>
-      <c r="E32" s="78"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
-      <c r="H32" s="78"/>
-      <c r="I32" s="80" t="s">
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="80"/>
+      <c r="I32" s="82" t="s">
         <v>226</v>
       </c>
-      <c r="J32" s="78"/>
-      <c r="K32" s="78"/>
-      <c r="L32" s="78"/>
-      <c r="M32" s="78"/>
+      <c r="J32" s="80"/>
+      <c r="K32" s="80"/>
+      <c r="L32" s="80"/>
+      <c r="M32" s="80"/>
       <c r="O32" s="1" t="s">
         <v>227</v>
       </c>

</xml_diff>

<commit_message>
all the data should now be correct on the welk tab. There was some fishy stuff happening on the metabolics calculations in the google drive, I have revised them and added them to this sheet
</commit_message>
<xml_diff>
--- a/metabolicsData_revised.xlsx
+++ b/metabolicsData_revised.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C181825C-C9F9-4B71-8CBE-3E2817F86D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A21749-EACE-41DD-8152-6581364E9DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="key" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,6 @@
     <sheet name="sild" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1424,7 +1423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1568,6 +1567,12 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1576,11 +1581,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -4370,12 +4370,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="D1" s="79"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
@@ -12869,8 +12869,8 @@
   </sheetPr>
   <dimension ref="A1:AA99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L92" sqref="L92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -12895,12 +12895,12 @@
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
-      <c r="G3" s="81" t="s">
+      <c r="G3" s="85" t="s">
         <v>170</v>
       </c>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
       <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" customHeight="1">
@@ -13216,204 +13216,204 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" ht="15">
       <c r="A15" s="3">
         <v>1</v>
       </c>
       <c r="B15" s="3">
         <v>3</v>
       </c>
-      <c r="C15" s="3">
-        <v>1.7843621039999999</v>
-      </c>
-      <c r="D15" s="26">
-        <v>13.12447721</v>
-      </c>
-      <c r="E15" s="26">
-        <v>12.913345469999999</v>
-      </c>
-      <c r="F15" s="26">
-        <v>13.43907997</v>
-      </c>
-      <c r="G15" s="26">
-        <v>12.6698953</v>
-      </c>
-      <c r="H15" s="26">
-        <v>12.738848109999999</v>
-      </c>
-      <c r="I15" s="26">
-        <v>12.943077819999999</v>
-      </c>
-      <c r="J15" s="26">
-        <v>12.516079510000001</v>
-      </c>
-      <c r="K15" s="26">
-        <v>12.488343179999999</v>
+      <c r="C15" s="79">
+        <v>1.751345334</v>
+      </c>
+      <c r="D15" s="79">
+        <v>13.027399920000001</v>
+      </c>
+      <c r="E15" s="79">
+        <v>12.812353359999999</v>
+      </c>
+      <c r="F15" s="79">
+        <v>13.310797470000001</v>
+      </c>
+      <c r="G15" s="79">
+        <v>12.367950560000001</v>
+      </c>
+      <c r="H15" s="79">
+        <v>12.62920433</v>
+      </c>
+      <c r="I15" s="79">
+        <v>12.72295995</v>
+      </c>
+      <c r="J15" s="79">
+        <v>12.33160528</v>
+      </c>
+      <c r="K15" s="79">
+        <v>12.392633</v>
       </c>
       <c r="M15" s="4">
-        <f t="shared" ref="M15:M18" si="1">MAX(D15:K15)</f>
-        <v>13.43907997</v>
+        <f>MAX(D15:K15)</f>
+        <v>13.310797470000001</v>
       </c>
       <c r="N15" s="4">
-        <f t="shared" ref="N15:N18" si="2">MIN(D15:K15)</f>
-        <v>12.488343179999999</v>
+        <f t="shared" ref="N15:N18" si="1">MIN(D15:K15)</f>
+        <v>12.33160528</v>
       </c>
       <c r="O15" s="4">
-        <f t="shared" ref="O15:O18" si="3">AVERAGE(D15:K15)</f>
-        <v>12.85414332125</v>
+        <f t="shared" ref="O15:O18" si="2">AVERAGE(D15:K15)</f>
+        <v>12.699362983750001</v>
       </c>
       <c r="Q15" s="4">
         <f>MAX(D15:K18)</f>
-        <v>13.43907997</v>
+        <v>13.310797470000001</v>
       </c>
       <c r="R15" s="4">
         <f>MIN(D15:K18)</f>
-        <v>10.24945512</v>
+        <v>10.24386281</v>
       </c>
       <c r="S15" s="4">
         <f>AVERAGE(D15:K18)</f>
-        <v>11.530962407500001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19">
+        <v>11.447995978124998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15">
       <c r="A16" s="3">
         <v>2</v>
       </c>
       <c r="B16" s="3">
         <v>3</v>
       </c>
-      <c r="C16" s="26">
-        <v>1.6121465399999999</v>
-      </c>
-      <c r="D16" s="28">
-        <v>11.00523155</v>
-      </c>
-      <c r="E16" s="28">
-        <v>10.60252912</v>
-      </c>
-      <c r="F16" s="28">
-        <v>11.60660088</v>
-      </c>
-      <c r="G16" s="28">
-        <v>10.918603879999999</v>
-      </c>
-      <c r="H16" s="28">
-        <v>10.862868539999999</v>
-      </c>
-      <c r="I16" s="28">
-        <v>10.98916532</v>
-      </c>
-      <c r="J16" s="26">
-        <v>10.24945512</v>
-      </c>
-      <c r="K16" s="28">
-        <v>10.340420999999999</v>
+      <c r="C16" s="79">
+        <v>1.6153839210000001</v>
+      </c>
+      <c r="D16" s="79">
+        <v>11.0059532</v>
+      </c>
+      <c r="E16" s="79">
+        <v>10.588295240000001</v>
+      </c>
+      <c r="F16" s="79">
+        <v>11.55513827</v>
+      </c>
+      <c r="G16" s="79">
+        <v>10.92502738</v>
+      </c>
+      <c r="H16" s="79">
+        <v>10.86090008</v>
+      </c>
+      <c r="I16" s="79">
+        <v>10.98918377</v>
+      </c>
+      <c r="J16" s="79">
+        <v>10.24386281</v>
+      </c>
+      <c r="K16" s="79">
+        <v>10.336277819999999</v>
       </c>
       <c r="M16" s="4">
+        <f t="shared" ref="M15:M18" si="3">MAX(D16:K16)</f>
+        <v>11.55513827</v>
+      </c>
+      <c r="N16" s="4">
         <f t="shared" si="1"/>
-        <v>11.60660088</v>
-      </c>
-      <c r="N16" s="4">
+        <v>10.24386281</v>
+      </c>
+      <c r="O16" s="4">
         <f t="shared" si="2"/>
-        <v>10.24945512</v>
-      </c>
-      <c r="O16" s="4">
-        <f t="shared" si="3"/>
-        <v>10.821859426250001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19">
+        <v>10.81307982125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="15">
       <c r="A17" s="3">
         <v>3</v>
       </c>
       <c r="B17" s="3">
         <v>3</v>
       </c>
-      <c r="C17" s="26">
-        <v>1.8957573720000001</v>
-      </c>
-      <c r="D17" s="28">
-        <v>11.737313759999999</v>
-      </c>
-      <c r="E17" s="26">
-        <v>11.41887084</v>
-      </c>
-      <c r="F17" s="28">
-        <v>12.781186999999999</v>
-      </c>
-      <c r="G17" s="28">
-        <v>11.57141339</v>
-      </c>
-      <c r="H17" s="28">
-        <v>11.418755819999999</v>
-      </c>
-      <c r="I17" s="28">
-        <v>11.489576980000001</v>
-      </c>
-      <c r="J17" s="28">
-        <v>11.272226720000001</v>
-      </c>
-      <c r="K17" s="28">
-        <v>10.854166660000001</v>
+      <c r="C17" s="79">
+        <v>1.9051938390000001</v>
+      </c>
+      <c r="D17" s="79">
+        <v>11.734510090000001</v>
+      </c>
+      <c r="E17" s="79">
+        <v>11.42584708</v>
+      </c>
+      <c r="F17" s="79">
+        <v>12.60082197</v>
+      </c>
+      <c r="G17" s="79">
+        <v>11.57117963</v>
+      </c>
+      <c r="H17" s="79">
+        <v>11.42935855</v>
+      </c>
+      <c r="I17" s="79">
+        <v>11.49916747</v>
+      </c>
+      <c r="J17" s="79">
+        <v>11.23061113</v>
+      </c>
+      <c r="K17" s="79">
+        <v>10.855900719999999</v>
       </c>
       <c r="M17" s="4">
+        <f t="shared" si="3"/>
+        <v>12.60082197</v>
+      </c>
+      <c r="N17" s="4">
         <f t="shared" si="1"/>
-        <v>12.781186999999999</v>
-      </c>
-      <c r="N17" s="4">
+        <v>10.855900719999999</v>
+      </c>
+      <c r="O17" s="4">
         <f t="shared" si="2"/>
-        <v>10.854166660000001</v>
-      </c>
-      <c r="O17" s="4">
-        <f t="shared" si="3"/>
-        <v>11.56793889625</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19">
+        <v>11.54342458</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="15">
       <c r="A18" s="3">
         <v>4</v>
       </c>
       <c r="B18" s="3">
         <v>3</v>
       </c>
-      <c r="C18" s="26">
-        <v>1.8694403660000001</v>
-      </c>
-      <c r="D18" s="26">
-        <v>10.98796596</v>
-      </c>
-      <c r="E18" s="26">
-        <v>11.078948069999999</v>
-      </c>
-      <c r="F18" s="26">
-        <v>11.00202453</v>
-      </c>
-      <c r="G18" s="26">
-        <v>10.618670460000001</v>
-      </c>
-      <c r="H18" s="26">
-        <v>11.08831531</v>
-      </c>
-      <c r="I18" s="26">
-        <v>11.03373869</v>
-      </c>
-      <c r="J18" s="26">
-        <v>10.620491790000001</v>
-      </c>
-      <c r="K18" s="26">
-        <v>10.60910908</v>
+      <c r="C18" s="79">
+        <v>1.797774521</v>
+      </c>
+      <c r="D18" s="79">
+        <v>10.807169289999999</v>
+      </c>
+      <c r="E18" s="79">
+        <v>10.923264469999999</v>
+      </c>
+      <c r="F18" s="79">
+        <v>10.83669117</v>
+      </c>
+      <c r="G18" s="79">
+        <v>10.449408869999999</v>
+      </c>
+      <c r="H18" s="79">
+        <v>10.92302059</v>
+      </c>
+      <c r="I18" s="79">
+        <v>10.89053167</v>
+      </c>
+      <c r="J18" s="79">
+        <v>10.536766350000001</v>
+      </c>
+      <c r="K18" s="79">
+        <v>10.522079809999999</v>
       </c>
       <c r="M18" s="4">
+        <f t="shared" si="3"/>
+        <v>10.923264469999999</v>
+      </c>
+      <c r="N18" s="4">
         <f t="shared" si="1"/>
-        <v>11.08831531</v>
-      </c>
-      <c r="N18" s="4">
+        <v>10.449408869999999</v>
+      </c>
+      <c r="O18" s="4">
         <f t="shared" si="2"/>
-        <v>10.60910908</v>
-      </c>
-      <c r="O18" s="4">
-        <f t="shared" si="3"/>
-        <v>10.879907986249998</v>
+        <v>10.7361165275</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="12.75">
@@ -13438,39 +13438,39 @@
       </c>
       <c r="C21" s="3">
         <f t="shared" ref="C21:K21" si="4">MAX(C15:C18)</f>
-        <v>1.8957573720000001</v>
+        <v>1.9051938390000001</v>
       </c>
       <c r="D21" s="3">
         <f t="shared" si="4"/>
-        <v>13.12447721</v>
+        <v>13.027399920000001</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" si="4"/>
-        <v>12.913345469999999</v>
+        <v>12.812353359999999</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="4"/>
-        <v>13.43907997</v>
+        <v>13.310797470000001</v>
       </c>
       <c r="G21" s="3">
         <f t="shared" si="4"/>
-        <v>12.6698953</v>
+        <v>12.367950560000001</v>
       </c>
       <c r="H21" s="3">
         <f t="shared" si="4"/>
-        <v>12.738848109999999</v>
+        <v>12.62920433</v>
       </c>
       <c r="I21" s="3">
         <f t="shared" si="4"/>
-        <v>12.943077819999999</v>
+        <v>12.72295995</v>
       </c>
       <c r="J21" s="3">
         <f t="shared" si="4"/>
-        <v>12.516079510000001</v>
+        <v>12.33160528</v>
       </c>
       <c r="K21" s="3">
         <f t="shared" si="4"/>
-        <v>12.488343179999999</v>
+        <v>12.392633</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="12.75">
@@ -13480,39 +13480,39 @@
       </c>
       <c r="C22" s="3">
         <f t="shared" ref="C22:K22" si="5">MIN(C15:C18)</f>
-        <v>1.6121465399999999</v>
+        <v>1.6153839210000001</v>
       </c>
       <c r="D22" s="3">
         <f t="shared" si="5"/>
-        <v>10.98796596</v>
+        <v>10.807169289999999</v>
       </c>
       <c r="E22" s="3">
         <f t="shared" si="5"/>
-        <v>10.60252912</v>
+        <v>10.588295240000001</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="5"/>
-        <v>11.00202453</v>
+        <v>10.83669117</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="5"/>
-        <v>10.618670460000001</v>
+        <v>10.449408869999999</v>
       </c>
       <c r="H22" s="3">
         <f t="shared" si="5"/>
-        <v>10.862868539999999</v>
+        <v>10.86090008</v>
       </c>
       <c r="I22" s="3">
         <f t="shared" si="5"/>
-        <v>10.98916532</v>
+        <v>10.89053167</v>
       </c>
       <c r="J22" s="3">
         <f t="shared" si="5"/>
-        <v>10.24945512</v>
+        <v>10.24386281</v>
       </c>
       <c r="K22" s="3">
         <f t="shared" si="5"/>
-        <v>10.340420999999999</v>
+        <v>10.336277819999999</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="12.75">
@@ -13522,39 +13522,39 @@
       </c>
       <c r="C23" s="3">
         <f t="shared" ref="C23:K23" si="6">AVERAGE(C15:C18)</f>
-        <v>1.7904265955000001</v>
+        <v>1.76742440375</v>
       </c>
       <c r="D23" s="3">
         <f t="shared" si="6"/>
-        <v>11.713747120000001</v>
+        <v>11.643758125</v>
       </c>
       <c r="E23" s="3">
         <f t="shared" si="6"/>
-        <v>11.503423375000001</v>
+        <v>11.4374400375</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="6"/>
-        <v>12.207223095</v>
+        <v>12.075862220000001</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" si="6"/>
-        <v>11.444645757500002</v>
+        <v>11.328391610000001</v>
       </c>
       <c r="H23" s="3">
         <f t="shared" si="6"/>
-        <v>11.527196945</v>
+        <v>11.460620887500001</v>
       </c>
       <c r="I23" s="3">
         <f t="shared" si="6"/>
-        <v>11.6138897025</v>
+        <v>11.525460715000001</v>
       </c>
       <c r="J23" s="3">
         <f t="shared" si="6"/>
-        <v>11.164563285000002</v>
+        <v>11.0857113925</v>
       </c>
       <c r="K23" s="3">
         <f t="shared" si="6"/>
-        <v>11.073009979999998</v>
+        <v>11.026722837499999</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="12.75">
@@ -13670,59 +13670,59 @@
       </c>
       <c r="D28" s="3">
         <f>D15-$C15</f>
-        <v>11.340115106000001</v>
+        <v>11.276054586000001</v>
       </c>
       <c r="E28" s="71">
         <f t="shared" ref="E28:K28" si="7">E15-$C15</f>
-        <v>11.128983366</v>
+        <v>11.061008026</v>
       </c>
       <c r="F28" s="71">
         <f t="shared" si="7"/>
-        <v>11.654717866</v>
+        <v>11.559452136000001</v>
       </c>
       <c r="G28" s="71">
         <f t="shared" si="7"/>
-        <v>10.885533196000001</v>
+        <v>10.616605226000001</v>
       </c>
       <c r="H28" s="71">
         <f t="shared" si="7"/>
-        <v>10.954486006</v>
+        <v>10.877858996000001</v>
       </c>
       <c r="I28" s="71">
         <f t="shared" si="7"/>
-        <v>11.158715716</v>
+        <v>10.971614616</v>
       </c>
       <c r="J28" s="71">
         <f t="shared" si="7"/>
-        <v>10.731717406000001</v>
+        <v>10.580259946</v>
       </c>
       <c r="K28" s="71">
         <f t="shared" si="7"/>
-        <v>10.703981076</v>
+        <v>10.641287666</v>
       </c>
       <c r="M28" s="4">
         <f t="shared" ref="M28:M31" si="8">MAX(D28:K28)</f>
-        <v>11.654717866</v>
+        <v>11.559452136000001</v>
       </c>
       <c r="N28" s="4">
         <f t="shared" ref="N28:N31" si="9">MIN(D28:K28)</f>
-        <v>10.703981076</v>
+        <v>10.580259946</v>
       </c>
       <c r="O28" s="4">
         <f t="shared" ref="O28:O31" si="10">AVERAGE(D28:K28)</f>
-        <v>11.06978121725</v>
+        <v>10.94801764975</v>
       </c>
       <c r="Q28" s="4">
         <f>MAX(D28:K31)</f>
-        <v>11.654717866</v>
+        <v>11.559452136000001</v>
       </c>
       <c r="R28" s="4">
         <f>MIN(D28:K31)</f>
-        <v>8.6373085800000009</v>
+        <v>8.6284788890000002</v>
       </c>
       <c r="S28" s="4">
         <f>AVERAGE(D28:K31)</f>
-        <v>9.7405358119999992</v>
+        <v>9.6805715743750014</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="12.75">
@@ -13734,47 +13734,47 @@
       </c>
       <c r="D29" s="71">
         <f t="shared" ref="D29:K31" si="11">D16-$C16</f>
-        <v>9.3930850100000001</v>
+        <v>9.390569279000001</v>
       </c>
       <c r="E29" s="71">
         <f t="shared" si="11"/>
-        <v>8.9903825800000003</v>
+        <v>8.9729113190000014</v>
       </c>
       <c r="F29" s="71">
         <f t="shared" si="11"/>
-        <v>9.9944543400000008</v>
+        <v>9.9397543490000011</v>
       </c>
       <c r="G29" s="71">
         <f t="shared" si="11"/>
-        <v>9.3064573399999997</v>
+        <v>9.3096434590000001</v>
       </c>
       <c r="H29" s="71">
         <f t="shared" si="11"/>
-        <v>9.2507219999999997</v>
+        <v>9.245516159000001</v>
       </c>
       <c r="I29" s="71">
         <f t="shared" si="11"/>
-        <v>9.3770187800000002</v>
+        <v>9.373799849000001</v>
       </c>
       <c r="J29" s="71">
         <f t="shared" si="11"/>
-        <v>8.6373085800000009</v>
+        <v>8.6284788890000002</v>
       </c>
       <c r="K29" s="71">
         <f t="shared" si="11"/>
-        <v>8.7282744599999997</v>
+        <v>8.720893899</v>
       </c>
       <c r="M29" s="4">
         <f t="shared" si="8"/>
-        <v>9.9944543400000008</v>
+        <v>9.9397543490000011</v>
       </c>
       <c r="N29" s="4">
         <f t="shared" si="9"/>
-        <v>8.6373085800000009</v>
+        <v>8.6284788890000002</v>
       </c>
       <c r="O29" s="4">
         <f t="shared" si="10"/>
-        <v>9.2097128862499993</v>
+        <v>9.1976959002500021</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="12.75">
@@ -13786,47 +13786,47 @@
       </c>
       <c r="D30" s="71">
         <f t="shared" si="11"/>
-        <v>9.841556387999999</v>
+        <v>9.8293162509999998</v>
       </c>
       <c r="E30" s="71">
         <f t="shared" si="11"/>
-        <v>9.523113468</v>
+        <v>9.5206532409999998</v>
       </c>
       <c r="F30" s="71">
         <f t="shared" si="11"/>
-        <v>10.885429627999999</v>
+        <v>10.695628130999999</v>
       </c>
       <c r="G30" s="71">
         <f t="shared" si="11"/>
-        <v>9.6756560179999997</v>
+        <v>9.6659857909999989</v>
       </c>
       <c r="H30" s="71">
         <f t="shared" si="11"/>
-        <v>9.5229984479999992</v>
+        <v>9.5241647109999992</v>
       </c>
       <c r="I30" s="71">
         <f t="shared" si="11"/>
-        <v>9.5938196080000004</v>
+        <v>9.593973630999999</v>
       </c>
       <c r="J30" s="71">
         <f t="shared" si="11"/>
-        <v>9.3764693480000005</v>
+        <v>9.3254172909999991</v>
       </c>
       <c r="K30" s="71">
         <f t="shared" si="11"/>
-        <v>8.9584092880000004</v>
+        <v>8.9507068809999986</v>
       </c>
       <c r="M30" s="4">
         <f t="shared" si="8"/>
-        <v>10.885429627999999</v>
+        <v>10.695628130999999</v>
       </c>
       <c r="N30" s="4">
         <f t="shared" si="9"/>
-        <v>8.9584092880000004</v>
+        <v>8.9507068809999986</v>
       </c>
       <c r="O30" s="4">
         <f t="shared" si="10"/>
-        <v>9.67218152425</v>
+        <v>9.6382307409999992</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="12.75">
@@ -13838,47 +13838,47 @@
       </c>
       <c r="D31" s="71">
         <f t="shared" si="11"/>
-        <v>9.1185255940000012</v>
+        <v>9.009394769</v>
       </c>
       <c r="E31" s="71">
         <f t="shared" si="11"/>
-        <v>9.209507704</v>
+        <v>9.1254899489999985</v>
       </c>
       <c r="F31" s="71">
         <f t="shared" si="11"/>
-        <v>9.1325841640000007</v>
+        <v>9.0389166490000008</v>
       </c>
       <c r="G31" s="71">
         <f t="shared" si="11"/>
-        <v>8.7492300940000014</v>
+        <v>8.6516343489999983</v>
       </c>
       <c r="H31" s="71">
         <f t="shared" si="11"/>
-        <v>9.2188749439999995</v>
+        <v>9.1252460689999992</v>
       </c>
       <c r="I31" s="71">
         <f t="shared" si="11"/>
-        <v>9.1642983240000007</v>
+        <v>9.0927571490000005</v>
       </c>
       <c r="J31" s="71">
         <f t="shared" si="11"/>
-        <v>8.7510514239999999</v>
+        <v>8.7389918289999997</v>
       </c>
       <c r="K31" s="71">
         <f t="shared" si="11"/>
-        <v>8.7396687140000004</v>
+        <v>8.7243052890000001</v>
       </c>
       <c r="M31" s="4">
         <f t="shared" si="8"/>
-        <v>9.2188749439999995</v>
+        <v>9.1254899489999985</v>
       </c>
       <c r="N31" s="4">
         <f t="shared" si="9"/>
-        <v>8.7396687140000004</v>
+        <v>8.6516343489999983</v>
       </c>
       <c r="O31" s="4">
         <f t="shared" si="10"/>
-        <v>9.0104676202500009</v>
+        <v>8.938342006500001</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="12.75">
@@ -13892,35 +13892,35 @@
       </c>
       <c r="D35" s="4">
         <f t="shared" ref="D35:K35" si="12">MAX(D28:D31)</f>
-        <v>11.340115106000001</v>
+        <v>11.276054586000001</v>
       </c>
       <c r="E35" s="4">
         <f t="shared" si="12"/>
-        <v>11.128983366</v>
+        <v>11.061008026</v>
       </c>
       <c r="F35" s="4">
         <f t="shared" si="12"/>
-        <v>11.654717866</v>
+        <v>11.559452136000001</v>
       </c>
       <c r="G35" s="4">
         <f t="shared" si="12"/>
-        <v>10.885533196000001</v>
+        <v>10.616605226000001</v>
       </c>
       <c r="H35" s="4">
         <f t="shared" si="12"/>
-        <v>10.954486006</v>
+        <v>10.877858996000001</v>
       </c>
       <c r="I35" s="4">
         <f t="shared" si="12"/>
-        <v>11.158715716</v>
+        <v>10.971614616</v>
       </c>
       <c r="J35" s="4">
         <f t="shared" si="12"/>
-        <v>10.731717406000001</v>
+        <v>10.580259946</v>
       </c>
       <c r="K35" s="4">
         <f t="shared" si="12"/>
-        <v>10.703981076</v>
+        <v>10.641287666</v>
       </c>
     </row>
     <row r="36" spans="1:19" ht="12.75">
@@ -13929,35 +13929,35 @@
       </c>
       <c r="D36" s="4">
         <f t="shared" ref="D36:K36" si="13">MIN(D28:D31)</f>
-        <v>9.1185255940000012</v>
+        <v>9.009394769</v>
       </c>
       <c r="E36" s="4">
         <f t="shared" si="13"/>
-        <v>8.9903825800000003</v>
+        <v>8.9729113190000014</v>
       </c>
       <c r="F36" s="4">
         <f t="shared" si="13"/>
-        <v>9.1325841640000007</v>
+        <v>9.0389166490000008</v>
       </c>
       <c r="G36" s="4">
         <f t="shared" si="13"/>
-        <v>8.7492300940000014</v>
+        <v>8.6516343489999983</v>
       </c>
       <c r="H36" s="4">
         <f t="shared" si="13"/>
-        <v>9.2188749439999995</v>
+        <v>9.1252460689999992</v>
       </c>
       <c r="I36" s="4">
         <f t="shared" si="13"/>
-        <v>9.1642983240000007</v>
+        <v>9.0927571490000005</v>
       </c>
       <c r="J36" s="4">
         <f t="shared" si="13"/>
-        <v>8.6373085800000009</v>
+        <v>8.6284788890000002</v>
       </c>
       <c r="K36" s="4">
         <f t="shared" si="13"/>
-        <v>8.7282744599999997</v>
+        <v>8.720893899</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="12.75">
@@ -13966,35 +13966,35 @@
       </c>
       <c r="D37" s="4">
         <f t="shared" ref="D37:K37" si="14">AVERAGE(D28:D31)</f>
-        <v>9.9233205244999994</v>
+        <v>9.8763337212499991</v>
       </c>
       <c r="E37" s="4">
         <f t="shared" si="14"/>
-        <v>9.7129967794999992</v>
+        <v>9.6700156337499994</v>
       </c>
       <c r="F37" s="4">
         <f t="shared" si="14"/>
-        <v>10.4167964995</v>
+        <v>10.308437816250001</v>
       </c>
       <c r="G37" s="4">
         <f t="shared" si="14"/>
-        <v>9.6542191620000004</v>
+        <v>9.56096720625</v>
       </c>
       <c r="H37" s="4">
         <f t="shared" si="14"/>
-        <v>9.7367703494999986</v>
+        <v>9.6931964837500004</v>
       </c>
       <c r="I37" s="4">
         <f t="shared" si="14"/>
-        <v>9.8234631070000002</v>
+        <v>9.7580363112500006</v>
       </c>
       <c r="J37" s="4">
         <f t="shared" si="14"/>
-        <v>9.374136689500002</v>
+        <v>9.3182869887499997</v>
       </c>
       <c r="K37" s="4">
         <f t="shared" si="14"/>
-        <v>9.2825833845000005</v>
+        <v>9.2592984337500006</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="12.75">
@@ -14103,63 +14103,63 @@
       </c>
       <c r="C44" s="4">
         <f t="shared" ref="C44:K44" si="15">C15*$J6</f>
-        <v>132.57810432719998</v>
+        <v>130.12495831620001</v>
       </c>
       <c r="D44" s="4">
         <f t="shared" si="15"/>
-        <v>975.14865670300003</v>
+        <v>967.93581405600003</v>
       </c>
       <c r="E44" s="4">
         <f t="shared" si="15"/>
-        <v>959.46156842099992</v>
+        <v>951.95785464799997</v>
       </c>
       <c r="F44" s="4">
         <f t="shared" si="15"/>
-        <v>998.52364177099992</v>
+        <v>988.99225202100001</v>
       </c>
       <c r="G44" s="4">
         <f t="shared" si="15"/>
-        <v>941.37322079</v>
+        <v>918.93872660800002</v>
       </c>
       <c r="H44" s="4">
         <f t="shared" si="15"/>
-        <v>946.49641457299992</v>
+        <v>938.349881719</v>
       </c>
       <c r="I44" s="4">
         <f t="shared" si="15"/>
-        <v>961.67068202599989</v>
+        <v>945.31592428499994</v>
       </c>
       <c r="J44" s="4">
         <f t="shared" si="15"/>
-        <v>929.94470759299998</v>
+        <v>916.23827230399991</v>
       </c>
       <c r="K44" s="4">
         <f t="shared" si="15"/>
-        <v>927.88389827399988</v>
+        <v>920.77263189999996</v>
       </c>
       <c r="M44" s="4">
         <f t="shared" ref="M44:M47" si="16">MAX(D44:K44)</f>
-        <v>998.52364177099992</v>
+        <v>988.99225202100001</v>
       </c>
       <c r="N44" s="4">
         <f t="shared" ref="N44:N47" si="17">MIN(D44:K44)</f>
-        <v>927.88389827399988</v>
+        <v>916.23827230399991</v>
       </c>
       <c r="O44" s="4">
         <f t="shared" ref="O44:O47" si="18">AVERAGE(D44:K44)</f>
-        <v>955.06284876887491</v>
+        <v>943.56266969262504</v>
       </c>
       <c r="Q44" s="4">
         <f>MAX(D44:K47)</f>
-        <v>1036.3878709746666</v>
+        <v>1020.9611191293332</v>
       </c>
       <c r="R44" s="4">
         <f>MIN(D44:K47)</f>
-        <v>685.00525052</v>
+        <v>684.63149780166657</v>
       </c>
       <c r="S44" s="4">
         <f>AVERAGE(D44:K47)</f>
-        <v>860.91954169803114</v>
+        <v>854.14135821062484</v>
       </c>
     </row>
     <row r="45" spans="1:19" ht="12.75">
@@ -14171,51 +14171,51 @@
       </c>
       <c r="C45" s="4">
         <f t="shared" ref="C45:K45" si="19">C16*$J7</f>
-        <v>107.74512708999998</v>
+        <v>107.9614920535</v>
       </c>
       <c r="D45" s="4">
         <f t="shared" si="19"/>
-        <v>735.51630859166653</v>
+        <v>735.56453886666668</v>
       </c>
       <c r="E45" s="4">
         <f t="shared" si="19"/>
-        <v>708.60236285333326</v>
+        <v>707.65106520666666</v>
       </c>
       <c r="F45" s="4">
         <f t="shared" si="19"/>
-        <v>775.70782548</v>
+        <v>772.26840771166667</v>
       </c>
       <c r="G45" s="4">
         <f t="shared" si="19"/>
-        <v>729.72669264666661</v>
+        <v>730.15599656333325</v>
       </c>
       <c r="H45" s="4">
         <f t="shared" si="19"/>
-        <v>726.00171408999984</v>
+        <v>725.87015534666659</v>
       </c>
       <c r="I45" s="4">
         <f t="shared" si="19"/>
-        <v>734.4425488866666</v>
+        <v>734.44378196166667</v>
       </c>
       <c r="J45" s="4">
         <f t="shared" si="19"/>
-        <v>685.00525052</v>
+        <v>684.63149780166657</v>
       </c>
       <c r="K45" s="4">
         <f t="shared" si="19"/>
-        <v>691.08480349999991</v>
+        <v>690.80790096999988</v>
       </c>
       <c r="M45" s="4">
         <f t="shared" si="16"/>
-        <v>775.70782548</v>
+        <v>772.26840771166667</v>
       </c>
       <c r="N45" s="4">
         <f t="shared" si="17"/>
-        <v>685.00525052</v>
+        <v>684.63149780166657</v>
       </c>
       <c r="O45" s="4">
         <f t="shared" si="18"/>
-        <v>723.26093832104164</v>
+        <v>722.67416805354151</v>
       </c>
     </row>
     <row r="46" spans="1:19" ht="12.75">
@@ -14227,51 +14227,51 @@
       </c>
       <c r="C46" s="4">
         <f t="shared" ref="C46:K46" si="20">C17*$J8</f>
-        <v>122.6555019684</v>
+        <v>123.26604138330001</v>
       </c>
       <c r="D46" s="4">
         <f t="shared" si="20"/>
-        <v>759.40420027200003</v>
+        <v>759.22280282300005</v>
       </c>
       <c r="E46" s="4">
         <f t="shared" si="20"/>
-        <v>738.80094334800003</v>
+        <v>739.25230607600008</v>
       </c>
       <c r="F46" s="4">
         <f t="shared" si="20"/>
-        <v>826.94279889999996</v>
+        <v>815.27318145900006</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" si="20"/>
-        <v>748.67044633300009</v>
+        <v>748.65532206099999</v>
       </c>
       <c r="H46" s="4">
         <f t="shared" si="20"/>
-        <v>738.79350155400004</v>
+        <v>739.47949818500001</v>
       </c>
       <c r="I46" s="4">
         <f t="shared" si="20"/>
-        <v>743.37563060600007</v>
+        <v>743.99613530900001</v>
       </c>
       <c r="J46" s="4">
         <f t="shared" si="20"/>
-        <v>729.31306878400005</v>
+        <v>726.62054011099997</v>
       </c>
       <c r="K46" s="4">
         <f t="shared" si="20"/>
-        <v>702.26458290200003</v>
+        <v>702.37677658400003</v>
       </c>
       <c r="M46" s="4">
         <f t="shared" si="16"/>
-        <v>826.94279889999996</v>
+        <v>815.27318145900006</v>
       </c>
       <c r="N46" s="4">
         <f t="shared" si="17"/>
-        <v>702.26458290200003</v>
+        <v>702.37677658400003</v>
       </c>
       <c r="O46" s="4">
         <f t="shared" si="18"/>
-        <v>748.44564658737511</v>
+        <v>746.85957032600004</v>
       </c>
     </row>
     <row r="47" spans="1:19" ht="12.75">
@@ -14283,51 +14283,51 @@
       </c>
       <c r="C47" s="4">
         <f t="shared" ref="C47:K47" si="21">C18*$J9</f>
-        <v>174.73035954213333</v>
+        <v>168.03199189613332</v>
       </c>
       <c r="D47" s="4">
         <f t="shared" si="21"/>
-        <v>1027.0085517279999</v>
+        <v>1010.1100896386664</v>
       </c>
       <c r="E47" s="4">
         <f t="shared" si="21"/>
-        <v>1035.5123462759998</v>
+        <v>1020.9611191293332</v>
       </c>
       <c r="F47" s="4">
         <f t="shared" si="21"/>
-        <v>1028.3225594039998</v>
+        <v>1012.8694013559999</v>
       </c>
       <c r="G47" s="4">
         <f t="shared" si="21"/>
-        <v>992.4917323279999</v>
+        <v>976.67141571599984</v>
       </c>
       <c r="H47" s="4">
         <f t="shared" si="21"/>
-        <v>1036.3878709746666</v>
+        <v>1020.9383244786666</v>
       </c>
       <c r="I47" s="4">
         <f t="shared" si="21"/>
-        <v>1031.2867762253331</v>
+        <v>1017.9016934226665</v>
       </c>
       <c r="J47" s="4">
         <f t="shared" si="21"/>
-        <v>992.66196597199996</v>
+        <v>984.83642817999998</v>
       </c>
       <c r="K47" s="4">
         <f t="shared" si="21"/>
-        <v>991.59806201066647</v>
+        <v>983.46372624133312</v>
       </c>
       <c r="M47" s="4">
         <f t="shared" si="16"/>
-        <v>1036.3878709746666</v>
+        <v>1020.9611191293332</v>
       </c>
       <c r="N47" s="4">
         <f t="shared" si="17"/>
-        <v>991.59806201066647</v>
+        <v>976.67141571599984</v>
       </c>
       <c r="O47" s="4">
         <f t="shared" si="18"/>
-        <v>1016.9087331148331</v>
+        <v>1003.4690247703332</v>
       </c>
     </row>
     <row r="49" spans="1:19" ht="12.75">
@@ -14352,39 +14352,39 @@
       </c>
       <c r="C50" s="3">
         <f t="shared" ref="C50:K50" si="22">MAX(C44:C47)</f>
-        <v>174.73035954213333</v>
+        <v>168.03199189613332</v>
       </c>
       <c r="D50" s="3">
         <f t="shared" si="22"/>
-        <v>1027.0085517279999</v>
+        <v>1010.1100896386664</v>
       </c>
       <c r="E50" s="3">
         <f t="shared" si="22"/>
-        <v>1035.5123462759998</v>
+        <v>1020.9611191293332</v>
       </c>
       <c r="F50" s="3">
         <f t="shared" si="22"/>
-        <v>1028.3225594039998</v>
+        <v>1012.8694013559999</v>
       </c>
       <c r="G50" s="3">
         <f t="shared" si="22"/>
-        <v>992.4917323279999</v>
+        <v>976.67141571599984</v>
       </c>
       <c r="H50" s="3">
         <f t="shared" si="22"/>
-        <v>1036.3878709746666</v>
+        <v>1020.9383244786666</v>
       </c>
       <c r="I50" s="3">
         <f t="shared" si="22"/>
-        <v>1031.2867762253331</v>
+        <v>1017.9016934226665</v>
       </c>
       <c r="J50" s="3">
         <f t="shared" si="22"/>
-        <v>992.66196597199996</v>
+        <v>984.83642817999998</v>
       </c>
       <c r="K50" s="3">
         <f t="shared" si="22"/>
-        <v>991.59806201066647</v>
+        <v>983.46372624133312</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="12.75">
@@ -14394,39 +14394,39 @@
       </c>
       <c r="C51" s="3">
         <f t="shared" ref="C51:K51" si="23">MIN(C44:C47)</f>
-        <v>107.74512708999998</v>
+        <v>107.9614920535</v>
       </c>
       <c r="D51" s="3">
         <f t="shared" si="23"/>
-        <v>735.51630859166653</v>
+        <v>735.56453886666668</v>
       </c>
       <c r="E51" s="3">
         <f t="shared" si="23"/>
-        <v>708.60236285333326</v>
+        <v>707.65106520666666</v>
       </c>
       <c r="F51" s="3">
         <f t="shared" si="23"/>
-        <v>775.70782548</v>
+        <v>772.26840771166667</v>
       </c>
       <c r="G51" s="3">
         <f t="shared" si="23"/>
-        <v>729.72669264666661</v>
+        <v>730.15599656333325</v>
       </c>
       <c r="H51" s="3">
         <f t="shared" si="23"/>
-        <v>726.00171408999984</v>
+        <v>725.87015534666659</v>
       </c>
       <c r="I51" s="3">
         <f t="shared" si="23"/>
-        <v>734.4425488866666</v>
+        <v>734.44378196166667</v>
       </c>
       <c r="J51" s="3">
         <f t="shared" si="23"/>
-        <v>685.00525052</v>
+        <v>684.63149780166657</v>
       </c>
       <c r="K51" s="3">
         <f t="shared" si="23"/>
-        <v>691.08480349999991</v>
+        <v>690.80790096999988</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="12.75">
@@ -14436,39 +14436,39 @@
       </c>
       <c r="C52" s="3">
         <f t="shared" ref="C52:K52" si="24">AVERAGE(C44:C47)</f>
-        <v>134.42727323193333</v>
+        <v>132.34612091228331</v>
       </c>
       <c r="D52" s="3">
         <f t="shared" si="24"/>
-        <v>874.26942932366671</v>
+        <v>868.20831134608329</v>
       </c>
       <c r="E52" s="3">
         <f t="shared" si="24"/>
-        <v>860.59430522458331</v>
+        <v>854.95558626499997</v>
       </c>
       <c r="F52" s="3">
         <f t="shared" si="24"/>
-        <v>907.37420638874983</v>
+        <v>897.35081063691666</v>
       </c>
       <c r="G52" s="3">
         <f t="shared" si="24"/>
-        <v>853.06552302441673</v>
+        <v>843.60536523708333</v>
       </c>
       <c r="H52" s="3">
         <f t="shared" si="24"/>
-        <v>861.91987529791663</v>
+        <v>856.15946493233332</v>
       </c>
       <c r="I52" s="3">
         <f t="shared" si="24"/>
-        <v>867.6939094359999</v>
+        <v>860.41438374458335</v>
       </c>
       <c r="J52" s="3">
         <f t="shared" si="24"/>
-        <v>834.23124821724991</v>
+        <v>828.08168459916658</v>
       </c>
       <c r="K52" s="3">
         <f t="shared" si="24"/>
-        <v>828.20783667166666</v>
+        <v>824.35525892383328</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="12.75">
@@ -14582,59 +14582,59 @@
       </c>
       <c r="D57" s="4">
         <f t="shared" ref="D57:K60" si="25">D28*$J6</f>
-        <v>842.57055237580005</v>
+        <v>837.81085573979999</v>
       </c>
       <c r="E57" s="4">
         <f t="shared" si="25"/>
-        <v>826.88346409379994</v>
+        <v>821.83289633179993</v>
       </c>
       <c r="F57" s="4">
         <f t="shared" si="25"/>
-        <v>865.94553744380005</v>
+        <v>858.86729370479998</v>
       </c>
       <c r="G57" s="4">
         <f t="shared" si="25"/>
-        <v>808.79511646280002</v>
+        <v>788.81376829179999</v>
       </c>
       <c r="H57" s="4">
         <f t="shared" si="25"/>
-        <v>813.91831024579994</v>
+        <v>808.22492340279996</v>
       </c>
       <c r="I57" s="4">
         <f t="shared" si="25"/>
-        <v>829.09257769879991</v>
+        <v>815.19096596880001</v>
       </c>
       <c r="J57" s="4">
         <f t="shared" si="25"/>
-        <v>797.36660326580011</v>
+        <v>786.11331398779998</v>
       </c>
       <c r="K57" s="4">
         <f t="shared" si="25"/>
-        <v>795.30579394680001</v>
+        <v>790.64767358379993</v>
       </c>
       <c r="M57" s="4">
         <f t="shared" ref="M57:M60" si="26">MAX(D57:K57)</f>
-        <v>865.94553744380005</v>
+        <v>858.86729370479998</v>
       </c>
       <c r="N57" s="4">
         <f t="shared" ref="N57:N60" si="27">MIN(D57:K57)</f>
-        <v>795.30579394680001</v>
+        <v>786.11331398779998</v>
       </c>
       <c r="O57" s="4">
         <f t="shared" ref="O57:O60" si="28">AVERAGE(D57:K57)</f>
-        <v>822.48474444167505</v>
+        <v>813.43771137642489</v>
       </c>
       <c r="Q57" s="4">
         <f>MAX(D57:K60)</f>
-        <v>865.94553744380005</v>
+        <v>858.86729370479998</v>
       </c>
       <c r="R57" s="4">
         <f>MIN(D57:K60)</f>
-        <v>577.26012343000002</v>
+        <v>576.67000574816666</v>
       </c>
       <c r="S57" s="4">
         <f>AVERAGE(D57:K60)</f>
-        <v>726.49226846609781</v>
+        <v>721.79523729834159</v>
       </c>
     </row>
     <row r="58" spans="1:19" ht="12.75">
@@ -14646,47 +14646,47 @@
       </c>
       <c r="D58" s="4">
         <f t="shared" si="25"/>
-        <v>627.77118150166666</v>
+        <v>627.60304681316666</v>
       </c>
       <c r="E58" s="4">
         <f t="shared" si="25"/>
-        <v>600.85723576333328</v>
+        <v>599.68957315316675</v>
       </c>
       <c r="F58" s="4">
         <f t="shared" si="25"/>
-        <v>667.96269839000001</v>
+        <v>664.30691565816664</v>
       </c>
       <c r="G58" s="4">
         <f t="shared" si="25"/>
-        <v>621.98156555666662</v>
+        <v>622.19450450983334</v>
       </c>
       <c r="H58" s="4">
         <f t="shared" si="25"/>
-        <v>618.25658699999997</v>
+        <v>617.90866329316668</v>
       </c>
       <c r="I58" s="4">
         <f t="shared" si="25"/>
-        <v>626.69742179666662</v>
+        <v>626.48228990816665</v>
       </c>
       <c r="J58" s="4">
         <f t="shared" si="25"/>
-        <v>577.26012343000002</v>
+        <v>576.67000574816666</v>
       </c>
       <c r="K58" s="4">
         <f t="shared" si="25"/>
-        <v>583.33967640999992</v>
+        <v>582.84640891649997</v>
       </c>
       <c r="M58" s="4">
         <f t="shared" si="26"/>
-        <v>667.96269839000001</v>
+        <v>664.30691565816664</v>
       </c>
       <c r="N58" s="4">
         <f t="shared" si="27"/>
-        <v>577.26012343000002</v>
+        <v>576.67000574816666</v>
       </c>
       <c r="O58" s="4">
         <f t="shared" si="28"/>
-        <v>615.51581123104165</v>
+        <v>614.71267600004171</v>
       </c>
     </row>
     <row r="59" spans="1:19" ht="12.75">
@@ -14698,47 +14698,47 @@
       </c>
       <c r="D59" s="4">
         <f t="shared" si="25"/>
-        <v>636.74869830360001</v>
+        <v>635.95676143970002</v>
       </c>
       <c r="E59" s="4">
         <f t="shared" si="25"/>
-        <v>616.14544137960002</v>
+        <v>615.98626469270005</v>
       </c>
       <c r="F59" s="4">
         <f t="shared" si="25"/>
-        <v>704.28729693159994</v>
+        <v>692.00714007570002</v>
       </c>
       <c r="G59" s="4">
         <f t="shared" si="25"/>
-        <v>626.01494436459996</v>
+        <v>625.38928067769996</v>
       </c>
       <c r="H59" s="4">
         <f t="shared" si="25"/>
-        <v>616.13799958560003</v>
+        <v>616.21345680169998</v>
       </c>
       <c r="I59" s="4">
         <f t="shared" si="25"/>
-        <v>620.72012863760006</v>
+        <v>620.73009392569998</v>
       </c>
       <c r="J59" s="4">
         <f t="shared" si="25"/>
-        <v>606.65756681560003</v>
+        <v>603.35449872769993</v>
       </c>
       <c r="K59" s="4">
         <f t="shared" si="25"/>
-        <v>579.60908093360001</v>
+        <v>579.11073520069988</v>
       </c>
       <c r="M59" s="4">
         <f t="shared" si="26"/>
-        <v>704.28729693159994</v>
+        <v>692.00714007570002</v>
       </c>
       <c r="N59" s="4">
         <f t="shared" si="27"/>
-        <v>579.60908093360001</v>
+        <v>579.11073520069988</v>
       </c>
       <c r="O59" s="4">
         <f t="shared" si="28"/>
-        <v>625.79014461897509</v>
+        <v>623.5935289427</v>
       </c>
     </row>
     <row r="60" spans="1:19" ht="12.75">
@@ -14750,47 +14750,47 @@
       </c>
       <c r="D60" s="4">
         <f t="shared" si="25"/>
-        <v>852.27819218586671</v>
+        <v>842.07809774253326</v>
       </c>
       <c r="E60" s="4">
         <f t="shared" si="25"/>
-        <v>860.78198673386657</v>
+        <v>852.92912723319978</v>
       </c>
       <c r="F60" s="4">
         <f t="shared" si="25"/>
-        <v>853.59219986186667</v>
+        <v>844.83740945986665</v>
       </c>
       <c r="G60" s="4">
         <f t="shared" si="25"/>
-        <v>817.76137278586668</v>
+        <v>808.63942381986635</v>
       </c>
       <c r="H60" s="4">
         <f t="shared" si="25"/>
-        <v>861.65751143253317</v>
+        <v>852.9063325825332</v>
       </c>
       <c r="I60" s="4">
         <f t="shared" si="25"/>
-        <v>856.55641668319993</v>
+        <v>849.86970152653328</v>
       </c>
       <c r="J60" s="4">
         <f t="shared" si="25"/>
-        <v>817.93160642986652</v>
+        <v>816.80443628386649</v>
       </c>
       <c r="K60" s="4">
         <f t="shared" si="25"/>
-        <v>816.86770246853325</v>
+        <v>815.43173434519986</v>
       </c>
       <c r="M60" s="4">
         <f t="shared" si="26"/>
-        <v>861.65751143253317</v>
+        <v>852.92912723319978</v>
       </c>
       <c r="N60" s="4">
         <f t="shared" si="27"/>
-        <v>816.86770246853325</v>
+        <v>808.63942381986635</v>
       </c>
       <c r="O60" s="4">
         <f t="shared" si="28"/>
-        <v>842.17837357269991</v>
+        <v>835.43703287419999</v>
       </c>
     </row>
     <row r="63" spans="1:19" ht="12.75">
@@ -14804,35 +14804,35 @@
       </c>
       <c r="D64" s="4">
         <f t="shared" ref="D64:K64" si="29">MAX(D57:D60)</f>
-        <v>852.27819218586671</v>
+        <v>842.07809774253326</v>
       </c>
       <c r="E64" s="4">
         <f t="shared" si="29"/>
-        <v>860.78198673386657</v>
+        <v>852.92912723319978</v>
       </c>
       <c r="F64" s="4">
         <f t="shared" si="29"/>
-        <v>865.94553744380005</v>
+        <v>858.86729370479998</v>
       </c>
       <c r="G64" s="4">
         <f t="shared" si="29"/>
-        <v>817.76137278586668</v>
+        <v>808.63942381986635</v>
       </c>
       <c r="H64" s="4">
         <f t="shared" si="29"/>
-        <v>861.65751143253317</v>
+        <v>852.9063325825332</v>
       </c>
       <c r="I64" s="4">
         <f t="shared" si="29"/>
-        <v>856.55641668319993</v>
+        <v>849.86970152653328</v>
       </c>
       <c r="J64" s="4">
         <f t="shared" si="29"/>
-        <v>817.93160642986652</v>
+        <v>816.80443628386649</v>
       </c>
       <c r="K64" s="4">
         <f t="shared" si="29"/>
-        <v>816.86770246853325</v>
+        <v>815.43173434519986</v>
       </c>
     </row>
     <row r="65" spans="1:22" ht="12.75">
@@ -14841,35 +14841,35 @@
       </c>
       <c r="D65" s="4">
         <f t="shared" ref="D65:K65" si="30">MIN(D57:D60)</f>
-        <v>627.77118150166666</v>
+        <v>627.60304681316666</v>
       </c>
       <c r="E65" s="4">
         <f t="shared" si="30"/>
-        <v>600.85723576333328</v>
+        <v>599.68957315316675</v>
       </c>
       <c r="F65" s="4">
         <f t="shared" si="30"/>
-        <v>667.96269839000001</v>
+        <v>664.30691565816664</v>
       </c>
       <c r="G65" s="4">
         <f t="shared" si="30"/>
-        <v>621.98156555666662</v>
+        <v>622.19450450983334</v>
       </c>
       <c r="H65" s="4">
         <f t="shared" si="30"/>
-        <v>616.13799958560003</v>
+        <v>616.21345680169998</v>
       </c>
       <c r="I65" s="4">
         <f t="shared" si="30"/>
-        <v>620.72012863760006</v>
+        <v>620.73009392569998</v>
       </c>
       <c r="J65" s="4">
         <f t="shared" si="30"/>
-        <v>577.26012343000002</v>
+        <v>576.67000574816666</v>
       </c>
       <c r="K65" s="4">
         <f t="shared" si="30"/>
-        <v>579.60908093360001</v>
+        <v>579.11073520069988</v>
       </c>
     </row>
     <row r="66" spans="1:22" ht="12.75">
@@ -14878,35 +14878,35 @@
       </c>
       <c r="D66" s="4">
         <f t="shared" ref="D66:K66" si="31">AVERAGE(D57:D60)</f>
-        <v>739.84215609173339</v>
+        <v>735.86219043380004</v>
       </c>
       <c r="E66" s="4">
         <f t="shared" si="31"/>
-        <v>726.16703199264998</v>
+        <v>722.6094653527166</v>
       </c>
       <c r="F66" s="4">
         <f t="shared" si="31"/>
-        <v>772.94693315681661</v>
+        <v>765.00468972463329</v>
       </c>
       <c r="G66" s="4">
         <f t="shared" si="31"/>
-        <v>718.63824979248329</v>
+        <v>711.25924432479985</v>
       </c>
       <c r="H66" s="4">
         <f t="shared" si="31"/>
-        <v>727.49260206598331</v>
+        <v>723.81334402004995</v>
       </c>
       <c r="I66" s="4">
         <f t="shared" si="31"/>
-        <v>733.26663620406657</v>
+        <v>728.06826283229998</v>
       </c>
       <c r="J66" s="4">
         <f t="shared" si="31"/>
-        <v>699.8039749853167</v>
+        <v>695.73556368688321</v>
       </c>
       <c r="K66" s="4">
         <f t="shared" si="31"/>
-        <v>693.78056343973321</v>
+        <v>692.00913801154991</v>
       </c>
     </row>
     <row r="68" spans="1:22" ht="15.75" customHeight="1">
@@ -14929,440 +14929,440 @@
       <c r="I70" s="77"/>
       <c r="N70" s="77"/>
     </row>
-    <row r="71" spans="1:22" s="83" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B71" s="83" t="s">
+    <row r="71" spans="1:22" s="80" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B71" s="80" t="s">
         <v>388</v>
       </c>
-      <c r="I71" s="84"/>
-      <c r="J71" s="84"/>
-      <c r="K71" s="84"/>
-      <c r="N71" s="84"/>
-      <c r="O71" s="84"/>
-      <c r="P71" s="84"/>
-    </row>
-    <row r="72" spans="1:22" s="83" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A72" s="84"/>
-      <c r="B72" s="84"/>
-      <c r="C72" s="84"/>
-      <c r="D72" s="84" t="s">
+      <c r="I71" s="81"/>
+      <c r="J71" s="81"/>
+      <c r="K71" s="81"/>
+      <c r="N71" s="81"/>
+      <c r="O71" s="81"/>
+      <c r="P71" s="81"/>
+    </row>
+    <row r="72" spans="1:22" s="80" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A72" s="81"/>
+      <c r="B72" s="81"/>
+      <c r="C72" s="81"/>
+      <c r="D72" s="81" t="s">
         <v>192</v>
       </c>
-      <c r="E72" s="84" t="s">
+      <c r="E72" s="81" t="s">
         <v>193</v>
       </c>
-      <c r="F72" s="84"/>
-      <c r="G72" s="84"/>
-      <c r="H72" s="84"/>
-      <c r="I72" s="84" t="s">
+      <c r="F72" s="81"/>
+      <c r="G72" s="81"/>
+      <c r="H72" s="81"/>
+      <c r="I72" s="81" t="s">
         <v>192</v>
       </c>
-      <c r="J72" s="84" t="s">
+      <c r="J72" s="81" t="s">
         <v>193</v>
       </c>
-      <c r="K72" s="84"/>
-      <c r="L72" s="84"/>
-      <c r="M72" s="84"/>
-      <c r="N72" s="84" t="s">
+      <c r="K72" s="81"/>
+      <c r="L72" s="81"/>
+      <c r="M72" s="81"/>
+      <c r="N72" s="81" t="s">
         <v>192</v>
       </c>
-      <c r="O72" s="84" t="s">
+      <c r="O72" s="81" t="s">
         <v>193</v>
       </c>
-      <c r="P72" s="84"/>
-      <c r="Q72" s="84"/>
-      <c r="R72" s="84"/>
-      <c r="S72" s="84" t="s">
+      <c r="P72" s="81"/>
+      <c r="Q72" s="81"/>
+      <c r="R72" s="81"/>
+      <c r="S72" s="81" t="s">
         <v>192</v>
       </c>
-      <c r="T72" s="84" t="s">
+      <c r="T72" s="81" t="s">
         <v>193</v>
       </c>
-      <c r="U72" s="84"/>
-      <c r="V72" s="84"/>
-    </row>
-    <row r="73" spans="1:22" s="83" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A73" s="84"/>
-      <c r="B73" s="84" t="s">
+      <c r="U72" s="81"/>
+      <c r="V72" s="81"/>
+    </row>
+    <row r="73" spans="1:22" s="80" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A73" s="81"/>
+      <c r="B73" s="81" t="s">
         <v>196</v>
       </c>
-      <c r="C73" s="84" t="s">
+      <c r="C73" s="81" t="s">
         <v>197</v>
       </c>
-      <c r="D73" s="84" t="s">
+      <c r="D73" s="81" t="s">
         <v>198</v>
       </c>
-      <c r="E73" s="84" t="s">
+      <c r="E73" s="81" t="s">
         <v>199</v>
       </c>
-      <c r="F73" s="84" t="s">
+      <c r="F73" s="81" t="s">
         <v>200</v>
       </c>
-      <c r="G73" s="84" t="s">
+      <c r="G73" s="81" t="s">
         <v>196</v>
       </c>
-      <c r="H73" s="84" t="s">
+      <c r="H73" s="81" t="s">
         <v>197</v>
       </c>
-      <c r="I73" s="84" t="s">
+      <c r="I73" s="81" t="s">
         <v>198</v>
       </c>
-      <c r="J73" s="84" t="s">
+      <c r="J73" s="81" t="s">
         <v>199</v>
       </c>
-      <c r="K73" s="84" t="s">
+      <c r="K73" s="81" t="s">
         <v>200</v>
       </c>
-      <c r="L73" s="84" t="s">
+      <c r="L73" s="81" t="s">
         <v>196</v>
       </c>
-      <c r="M73" s="84" t="s">
+      <c r="M73" s="81" t="s">
         <v>197</v>
       </c>
-      <c r="N73" s="84" t="s">
+      <c r="N73" s="81" t="s">
         <v>198</v>
       </c>
-      <c r="O73" s="84" t="s">
+      <c r="O73" s="81" t="s">
         <v>199</v>
       </c>
-      <c r="P73" s="84" t="s">
+      <c r="P73" s="81" t="s">
         <v>200</v>
       </c>
-      <c r="Q73" s="84" t="s">
+      <c r="Q73" s="81" t="s">
         <v>196</v>
       </c>
-      <c r="R73" s="84" t="s">
+      <c r="R73" s="81" t="s">
         <v>197</v>
       </c>
-      <c r="S73" s="84" t="s">
+      <c r="S73" s="81" t="s">
         <v>198</v>
       </c>
-      <c r="T73" s="84" t="s">
+      <c r="T73" s="81" t="s">
         <v>199</v>
       </c>
-      <c r="U73" s="84" t="s">
+      <c r="U73" s="81" t="s">
         <v>200</v>
       </c>
-      <c r="V73" s="84"/>
-    </row>
-    <row r="74" spans="1:22" s="83" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A74" s="84"/>
-      <c r="B74" s="84">
+      <c r="V73" s="81"/>
+    </row>
+    <row r="74" spans="1:22" s="80" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A74" s="81"/>
+      <c r="B74" s="81">
         <v>1</v>
       </c>
-      <c r="C74" s="84">
+      <c r="C74" s="81">
         <v>3</v>
       </c>
-      <c r="D74" s="83">
+      <c r="D74" s="80">
         <v>1.751345334</v>
       </c>
-      <c r="E74" s="83">
+      <c r="E74" s="80">
         <v>13.027399920000001</v>
       </c>
-      <c r="F74" s="83">
+      <c r="F74" s="80">
         <v>12.812353359999999</v>
       </c>
-      <c r="G74" s="84">
+      <c r="G74" s="81">
         <v>2</v>
       </c>
-      <c r="H74" s="84">
+      <c r="H74" s="81">
         <v>3</v>
       </c>
-      <c r="I74" s="83">
+      <c r="I74" s="80">
         <v>1.6153839210000001</v>
       </c>
-      <c r="J74" s="83">
+      <c r="J74" s="80">
         <v>11.0059532</v>
       </c>
-      <c r="K74" s="83">
+      <c r="K74" s="80">
         <v>10.588295240000001</v>
       </c>
-      <c r="L74" s="84">
+      <c r="L74" s="81">
         <v>3</v>
       </c>
-      <c r="M74" s="84">
+      <c r="M74" s="81">
         <v>3</v>
       </c>
-      <c r="N74" s="83">
+      <c r="N74" s="80">
         <v>1.9051938390000001</v>
       </c>
-      <c r="O74" s="83">
+      <c r="O74" s="80">
         <v>11.734510090000001</v>
       </c>
-      <c r="P74" s="83">
+      <c r="P74" s="80">
         <v>11.42584708</v>
       </c>
-      <c r="Q74" s="84">
+      <c r="Q74" s="81">
         <v>4</v>
       </c>
-      <c r="R74" s="84">
+      <c r="R74" s="81">
         <v>3</v>
       </c>
-      <c r="S74" s="83">
+      <c r="S74" s="80">
         <v>1.797774521</v>
       </c>
-      <c r="T74" s="83">
+      <c r="T74" s="80">
         <v>10.807169289999999</v>
       </c>
-      <c r="U74" s="83">
+      <c r="U74" s="80">
         <v>10.923264469999999</v>
       </c>
-      <c r="V74" s="84"/>
-    </row>
-    <row r="75" spans="1:22" s="83" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A75" s="84"/>
-      <c r="B75" s="84">
+      <c r="V74" s="81"/>
+    </row>
+    <row r="75" spans="1:22" s="80" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A75" s="81"/>
+      <c r="B75" s="81">
         <v>1</v>
       </c>
-      <c r="C75" s="84">
+      <c r="C75" s="81">
         <v>2</v>
       </c>
-      <c r="D75" s="83">
+      <c r="D75" s="80">
         <v>1.8857474729999999</v>
       </c>
-      <c r="E75" s="83">
+      <c r="E75" s="80">
         <v>11.88952067</v>
       </c>
-      <c r="F75" s="83">
+      <c r="F75" s="80">
         <v>11.374466200000001</v>
       </c>
-      <c r="G75" s="84">
+      <c r="G75" s="81">
         <v>2</v>
       </c>
-      <c r="H75" s="84">
+      <c r="H75" s="81">
         <v>2</v>
       </c>
-      <c r="I75" s="83">
+      <c r="I75" s="80">
         <v>1.582638532</v>
       </c>
-      <c r="J75" s="83">
+      <c r="J75" s="80">
         <v>10.466353270000001</v>
       </c>
-      <c r="K75" s="83">
+      <c r="K75" s="80">
         <v>10.248913780000001</v>
       </c>
-      <c r="L75" s="84">
+      <c r="L75" s="81">
         <v>3</v>
       </c>
-      <c r="M75" s="84">
+      <c r="M75" s="81">
         <v>2</v>
       </c>
-      <c r="N75" s="83">
+      <c r="N75" s="80">
         <v>1.791405567</v>
       </c>
-      <c r="O75" s="83">
+      <c r="O75" s="80">
         <v>11.1419382</v>
       </c>
-      <c r="P75" s="83">
+      <c r="P75" s="80">
         <v>10.583862140000001</v>
       </c>
-      <c r="Q75" s="84">
+      <c r="Q75" s="81">
         <v>4</v>
       </c>
-      <c r="R75" s="84">
+      <c r="R75" s="81">
         <v>2</v>
       </c>
-      <c r="S75" s="83">
+      <c r="S75" s="80">
         <v>1.6692033900000001</v>
       </c>
-      <c r="T75" s="83">
+      <c r="T75" s="80">
         <v>11.08524332</v>
       </c>
-      <c r="U75" s="83">
+      <c r="U75" s="80">
         <v>10.360162170000001</v>
       </c>
-      <c r="V75" s="84"/>
-    </row>
-    <row r="76" spans="1:22" s="83" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A76" s="84"/>
-      <c r="B76" s="84">
+      <c r="V75" s="81"/>
+    </row>
+    <row r="76" spans="1:22" s="80" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A76" s="81"/>
+      <c r="B76" s="81">
         <v>1</v>
       </c>
-      <c r="C76" s="84">
+      <c r="C76" s="81">
         <v>2</v>
       </c>
-      <c r="D76" s="83">
+      <c r="D76" s="80">
         <v>1.8857474729999999</v>
       </c>
-      <c r="E76" s="83">
+      <c r="E76" s="80">
         <v>11.49310616</v>
       </c>
-      <c r="F76" s="83">
+      <c r="F76" s="80">
         <v>11.812987659999999</v>
       </c>
-      <c r="G76" s="84">
+      <c r="G76" s="81">
         <v>2</v>
       </c>
-      <c r="H76" s="84">
+      <c r="H76" s="81">
         <v>2</v>
       </c>
-      <c r="I76" s="83">
+      <c r="I76" s="80">
         <v>1.582638532</v>
       </c>
-      <c r="J76" s="83">
+      <c r="J76" s="80">
         <v>10.4607989</v>
       </c>
-      <c r="K76" s="83">
+      <c r="K76" s="80">
         <v>10.339188050000001</v>
       </c>
-      <c r="L76" s="84">
+      <c r="L76" s="81">
         <v>3</v>
       </c>
-      <c r="M76" s="84">
+      <c r="M76" s="81">
         <v>2</v>
       </c>
-      <c r="N76" s="83">
+      <c r="N76" s="80">
         <v>1.791405567</v>
       </c>
-      <c r="O76" s="83">
+      <c r="O76" s="80">
         <v>11.291321050000001</v>
       </c>
-      <c r="P76" s="83">
+      <c r="P76" s="80">
         <v>10.89643323</v>
       </c>
-      <c r="Q76" s="84">
+      <c r="Q76" s="81">
         <v>4</v>
       </c>
-      <c r="R76" s="84">
+      <c r="R76" s="81">
         <v>2</v>
       </c>
-      <c r="S76" s="83">
+      <c r="S76" s="80">
         <v>1.6692033900000001</v>
       </c>
-      <c r="T76" s="83">
+      <c r="T76" s="80">
         <v>10.78809822</v>
       </c>
-      <c r="U76" s="83">
+      <c r="U76" s="80">
         <v>10.44195406</v>
       </c>
-      <c r="V76" s="84"/>
-    </row>
-    <row r="77" spans="1:22" s="83" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A77" s="84"/>
-      <c r="B77" s="84">
+      <c r="V76" s="81"/>
+    </row>
+    <row r="77" spans="1:22" s="80" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A77" s="81"/>
+      <c r="B77" s="81">
         <v>1</v>
       </c>
-      <c r="C77" s="84">
+      <c r="C77" s="81">
         <v>1</v>
       </c>
-      <c r="D77" s="83">
+      <c r="D77" s="80">
         <v>1.711534415</v>
       </c>
-      <c r="E77" s="83">
+      <c r="E77" s="80">
         <v>11.77550426</v>
       </c>
-      <c r="F77" s="83">
+      <c r="F77" s="80">
         <v>11.760609199999999</v>
       </c>
-      <c r="G77" s="84">
+      <c r="G77" s="81">
         <v>2</v>
       </c>
-      <c r="H77" s="84">
+      <c r="H77" s="81">
         <v>1</v>
       </c>
-      <c r="I77" s="83">
+      <c r="I77" s="80">
         <v>1.5142305439999999</v>
       </c>
-      <c r="J77" s="85">
+      <c r="J77" s="82">
         <v>10.104439449999999</v>
       </c>
-      <c r="K77" s="85">
+      <c r="K77" s="82">
         <v>10.07576607</v>
       </c>
-      <c r="L77" s="84">
+      <c r="L77" s="81">
         <v>3</v>
       </c>
-      <c r="M77" s="84">
+      <c r="M77" s="81">
         <v>1</v>
       </c>
-      <c r="N77" s="83">
+      <c r="N77" s="80">
         <v>1.578711121</v>
       </c>
-      <c r="O77" s="83">
+      <c r="O77" s="80">
         <v>11.25170795</v>
       </c>
-      <c r="P77" s="83">
+      <c r="P77" s="80">
         <v>11.321315609999999</v>
       </c>
-      <c r="Q77" s="84">
+      <c r="Q77" s="81">
         <v>4</v>
       </c>
-      <c r="R77" s="84">
+      <c r="R77" s="81">
         <v>1</v>
       </c>
-      <c r="S77" s="83">
+      <c r="S77" s="80">
         <v>1.7902534109999999</v>
       </c>
-      <c r="T77" s="83">
+      <c r="T77" s="80">
         <v>10.4876483</v>
       </c>
-      <c r="U77" s="83">
+      <c r="U77" s="80">
         <v>10.774973490000001</v>
       </c>
-      <c r="V77" s="84"/>
-    </row>
-    <row r="78" spans="1:22" s="83" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A78" s="84"/>
-      <c r="B78" s="84">
+      <c r="V77" s="81"/>
+    </row>
+    <row r="78" spans="1:22" s="80" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A78" s="81"/>
+      <c r="B78" s="81">
         <v>1</v>
       </c>
-      <c r="C78" s="84">
+      <c r="C78" s="81">
         <v>1</v>
       </c>
-      <c r="D78" s="83">
+      <c r="D78" s="80">
         <v>1.711534415</v>
       </c>
-      <c r="E78" s="83">
+      <c r="E78" s="80">
         <v>11.733416739999999</v>
       </c>
-      <c r="F78" s="83">
+      <c r="F78" s="80">
         <v>11.5305891</v>
       </c>
-      <c r="G78" s="84">
+      <c r="G78" s="81">
         <v>2</v>
       </c>
-      <c r="H78" s="84">
+      <c r="H78" s="81">
         <v>1</v>
       </c>
-      <c r="I78" s="83">
+      <c r="I78" s="80">
         <v>1.5142305439999999</v>
       </c>
-      <c r="J78" s="85">
+      <c r="J78" s="82">
         <v>10.67099247</v>
       </c>
-      <c r="K78" s="85">
+      <c r="K78" s="82">
         <v>10.806250289999999</v>
       </c>
-      <c r="L78" s="84">
+      <c r="L78" s="81">
         <v>3</v>
       </c>
-      <c r="M78" s="84">
+      <c r="M78" s="81">
         <v>1</v>
       </c>
-      <c r="N78" s="83">
+      <c r="N78" s="80">
         <v>1.578711121</v>
       </c>
-      <c r="O78" s="83">
+      <c r="O78" s="80">
         <v>11.726914519999999</v>
       </c>
-      <c r="P78" s="83">
+      <c r="P78" s="80">
         <v>11.221981599999999</v>
       </c>
-      <c r="Q78" s="84">
+      <c r="Q78" s="81">
         <v>4</v>
       </c>
-      <c r="R78" s="84">
+      <c r="R78" s="81">
         <v>1</v>
       </c>
-      <c r="S78" s="83">
+      <c r="S78" s="80">
         <v>1.7902534109999999</v>
       </c>
-      <c r="T78" s="83">
+      <c r="T78" s="80">
         <v>10.66818662</v>
       </c>
-      <c r="U78" s="83">
+      <c r="U78" s="80">
         <v>11.20134861</v>
       </c>
-      <c r="V78" s="84"/>
+      <c r="V78" s="81"/>
     </row>
     <row r="79" spans="1:22" ht="15.75" customHeight="1">
       <c r="A79" s="73"/>
@@ -16246,36 +16246,36 @@
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="C9" s="79" t="s">
+      <c r="C9" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="80"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="80"/>
-      <c r="K9" s="80"/>
-      <c r="L9" s="80"/>
-      <c r="M9" s="80"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="84"/>
+      <c r="L9" s="84"/>
+      <c r="M9" s="84"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="C10" s="79" t="s">
+      <c r="C10" s="83" t="s">
         <v>225</v>
       </c>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="82" t="s">
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="84"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="86" t="s">
         <v>226</v>
       </c>
-      <c r="J10" s="80"/>
-      <c r="K10" s="80"/>
-      <c r="L10" s="80"/>
-      <c r="M10" s="80"/>
+      <c r="J10" s="84"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="84"/>
+      <c r="M10" s="84"/>
       <c r="O10" s="1" t="s">
         <v>227</v>
       </c>
@@ -16951,36 +16951,36 @@
       </c>
     </row>
     <row r="31" spans="1:17">
-      <c r="C31" s="79" t="s">
+      <c r="C31" s="83" t="s">
         <v>230</v>
       </c>
-      <c r="D31" s="80"/>
-      <c r="E31" s="80"/>
-      <c r="F31" s="80"/>
-      <c r="G31" s="80"/>
-      <c r="H31" s="80"/>
-      <c r="I31" s="80"/>
-      <c r="J31" s="80"/>
-      <c r="K31" s="80"/>
-      <c r="L31" s="80"/>
-      <c r="M31" s="80"/>
+      <c r="D31" s="84"/>
+      <c r="E31" s="84"/>
+      <c r="F31" s="84"/>
+      <c r="G31" s="84"/>
+      <c r="H31" s="84"/>
+      <c r="I31" s="84"/>
+      <c r="J31" s="84"/>
+      <c r="K31" s="84"/>
+      <c r="L31" s="84"/>
+      <c r="M31" s="84"/>
     </row>
     <row r="32" spans="1:17">
-      <c r="C32" s="79" t="s">
+      <c r="C32" s="83" t="s">
         <v>225</v>
       </c>
-      <c r="D32" s="80"/>
-      <c r="E32" s="80"/>
-      <c r="F32" s="80"/>
-      <c r="G32" s="80"/>
-      <c r="H32" s="80"/>
-      <c r="I32" s="82" t="s">
+      <c r="D32" s="84"/>
+      <c r="E32" s="84"/>
+      <c r="F32" s="84"/>
+      <c r="G32" s="84"/>
+      <c r="H32" s="84"/>
+      <c r="I32" s="86" t="s">
         <v>226</v>
       </c>
-      <c r="J32" s="80"/>
-      <c r="K32" s="80"/>
-      <c r="L32" s="80"/>
-      <c r="M32" s="80"/>
+      <c r="J32" s="84"/>
+      <c r="K32" s="84"/>
+      <c r="L32" s="84"/>
+      <c r="M32" s="84"/>
       <c r="O32" s="1" t="s">
         <v>227</v>
       </c>

</xml_diff>